<commit_message>
chore: updating dummy data
</commit_message>
<xml_diff>
--- a/sql/02_dummy_data_generator.xlsx
+++ b/sql/02_dummy_data_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\budlib\budlib-api\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF471C20-FAD3-45F3-9968-030CDD718768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEC2C0C-9DE3-47D8-8F5F-1E1035A38B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="603">
   <si>
     <t>book_id</t>
   </si>
@@ -1104,33 +1104,9 @@
     <t>role</t>
   </si>
   <si>
-    <t>izabella</t>
-  </si>
-  <si>
-    <t>Izabella</t>
-  </si>
-  <si>
-    <t>Patterson</t>
-  </si>
-  <si>
-    <t>izabella.patterson@ucalgary.ca</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>Yuvraj</t>
-  </si>
-  <si>
-    <t>yuvraj</t>
-  </si>
-  <si>
-    <t>yuvraj.patterson@ucalgary.ca</t>
-  </si>
-  <si>
-    <t>Yash</t>
-  </si>
-  <si>
     <t>school_id</t>
   </si>
   <si>
@@ -1822,6 +1798,57 @@
   </si>
   <si>
     <t>due_date</t>
+  </si>
+  <si>
+    <t>irene</t>
+  </si>
+  <si>
+    <t>Irene</t>
+  </si>
+  <si>
+    <t>Pauchard</t>
+  </si>
+  <si>
+    <t>yves</t>
+  </si>
+  <si>
+    <t>Yves</t>
+  </si>
+  <si>
+    <t>i.pauchard@calgarywaldorf.org</t>
+  </si>
+  <si>
+    <t>yves.pauchard@ucalgary.ca</t>
+  </si>
+  <si>
+    <t>zbhavyai</t>
+  </si>
+  <si>
+    <t>Bhavyai</t>
+  </si>
+  <si>
+    <t>Gupta</t>
+  </si>
+  <si>
+    <t>zbhavyai@gmail.com</t>
+  </si>
+  <si>
+    <t>faculty</t>
+  </si>
+  <si>
+    <t>mmylee</t>
+  </si>
+  <si>
+    <t>mmylee@ucalgary.ca</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Man Yin</t>
+  </si>
+  <si>
+    <t>Lee</t>
   </si>
 </sst>
 </file>
@@ -1829,7 +1856,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2328,7 +2355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2734,13 +2761,13 @@
         <v>7</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="R1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO book (",
@@ -2826,7 +2853,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="K3">
         <v>4</v>
@@ -2870,7 +2897,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="K4">
         <v>9</v>
@@ -2898,7 +2925,7 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -2926,7 +2953,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="K6">
         <v>2</v>
@@ -2954,7 +2981,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="K7">
         <v>4</v>
@@ -2982,7 +3009,7 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="K8">
         <v>9</v>
@@ -3010,7 +3037,7 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="K9">
         <v>10</v>
@@ -3041,7 +3068,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="K10">
         <v>9</v>
@@ -3069,7 +3096,7 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -3097,7 +3124,7 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -3125,7 +3152,7 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="K13">
         <v>6</v>
@@ -3154,7 +3181,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -3182,7 +3209,7 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="K15">
         <v>7</v>
@@ -3235,7 +3262,7 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="K17">
         <v>6</v>
@@ -3266,7 +3293,7 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -3294,7 +3321,7 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="K19">
         <v>7</v>
@@ -3321,7 +3348,7 @@
         <v>1995</v>
       </c>
       <c r="H20" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -3348,7 +3375,7 @@
         <v>1993</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="K21">
         <v>4</v>
@@ -3375,7 +3402,7 @@
         <v>1994</v>
       </c>
       <c r="H22" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="K22">
         <v>10</v>
@@ -3402,7 +3429,7 @@
         <v>2001</v>
       </c>
       <c r="H23" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -3429,7 +3456,7 @@
         <v>1990</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="K24">
         <v>8</v>
@@ -3456,7 +3483,7 @@
         <v>1996</v>
       </c>
       <c r="H25" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="K25">
         <v>4</v>
@@ -3483,7 +3510,7 @@
         <v>1992</v>
       </c>
       <c r="H26" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="K26">
         <v>6</v>
@@ -3513,7 +3540,7 @@
         <v>1989</v>
       </c>
       <c r="H27" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -3540,7 +3567,7 @@
         <v>2001</v>
       </c>
       <c r="H28" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="K28">
         <v>9</v>
@@ -3570,7 +3597,7 @@
         <v>1994</v>
       </c>
       <c r="H29" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -3597,7 +3624,7 @@
         <v>1997</v>
       </c>
       <c r="H30" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -3624,7 +3651,7 @@
         <v>1988</v>
       </c>
       <c r="H31" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="K31">
         <v>8</v>
@@ -3651,7 +3678,7 @@
         <v>1994</v>
       </c>
       <c r="H32" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="K32">
         <v>8</v>
@@ -3678,7 +3705,7 @@
         <v>2008</v>
       </c>
       <c r="I33" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="K33">
         <v>2</v>
@@ -3705,7 +3732,7 @@
         <v>1990</v>
       </c>
       <c r="H34" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="K34">
         <v>10</v>
@@ -3732,7 +3759,7 @@
         <v>2001</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -3759,7 +3786,7 @@
         <v>1996</v>
       </c>
       <c r="H36" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="K36">
         <v>10</v>
@@ -3786,7 +3813,7 @@
         <v>1995</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="K37">
         <v>7</v>
@@ -3813,7 +3840,7 @@
         <v>1980</v>
       </c>
       <c r="H38" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="K38">
         <v>8</v>
@@ -3840,7 +3867,7 @@
         <v>1993</v>
       </c>
       <c r="H39" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="K39">
         <v>8</v>
@@ -3867,7 +3894,7 @@
         <v>1998</v>
       </c>
       <c r="H40" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="K40">
         <v>2</v>
@@ -3894,7 +3921,7 @@
         <v>1995</v>
       </c>
       <c r="H41" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="K41">
         <v>10</v>
@@ -3921,7 +3948,7 @@
         <v>2003</v>
       </c>
       <c r="H42" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="K42">
         <v>10</v>
@@ -3948,7 +3975,7 @@
         <v>1979</v>
       </c>
       <c r="H43" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="K43">
         <v>5</v>
@@ -3975,7 +4002,7 @@
         <v>1991</v>
       </c>
       <c r="H44" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -4002,7 +4029,7 @@
         <v>1986</v>
       </c>
       <c r="H45" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="K45">
         <v>2</v>
@@ -4029,7 +4056,7 @@
         <v>1981</v>
       </c>
       <c r="H46" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="K46">
         <v>5</v>
@@ -4059,7 +4086,7 @@
         <v>1983</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="K47">
         <v>4</v>
@@ -4086,7 +4113,7 @@
         <v>1983</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="K48">
         <v>4</v>
@@ -4113,7 +4140,7 @@
         <v>1996</v>
       </c>
       <c r="H49" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="K49">
         <v>5</v>
@@ -4140,7 +4167,7 @@
         <v>1990</v>
       </c>
       <c r="H50" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="K50">
         <v>4</v>
@@ -4167,7 +4194,7 @@
         <v>1987</v>
       </c>
       <c r="H51" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="K51">
         <v>7</v>
@@ -4194,7 +4221,7 @@
         <v>1979</v>
       </c>
       <c r="H52" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="K52">
         <v>9</v>
@@ -4221,7 +4248,7 @@
         <v>1989</v>
       </c>
       <c r="H53" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="K53">
         <v>6</v>
@@ -4248,7 +4275,7 @@
         <v>1990</v>
       </c>
       <c r="H54" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="K54">
         <v>2</v>
@@ -4275,7 +4302,7 @@
         <v>2001</v>
       </c>
       <c r="H55" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="K55">
         <v>3</v>
@@ -4302,7 +4329,7 @@
         <v>1993</v>
       </c>
       <c r="H56" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="K56">
         <v>9</v>
@@ -4329,7 +4356,7 @@
         <v>1994</v>
       </c>
       <c r="H57" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -4356,7 +4383,7 @@
         <v>2001</v>
       </c>
       <c r="H58" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="K58">
         <v>6</v>
@@ -4386,7 +4413,7 @@
         <v>1991</v>
       </c>
       <c r="H59" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="K59">
         <v>1</v>
@@ -4416,7 +4443,7 @@
         <v>1983</v>
       </c>
       <c r="H60" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="K60">
         <v>5</v>
@@ -4446,7 +4473,7 @@
         <v>1983</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="K61">
         <v>8</v>
@@ -4473,7 +4500,7 @@
         <v>1987</v>
       </c>
       <c r="H62" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K62">
         <v>9</v>
@@ -4500,7 +4527,7 @@
         <v>1994</v>
       </c>
       <c r="H63" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="K63">
         <v>5</v>
@@ -4527,7 +4554,7 @@
         <v>1983</v>
       </c>
       <c r="H64" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -4551,7 +4578,7 @@
         <v>267</v>
       </c>
       <c r="H65" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="K65">
         <v>1</v>
@@ -4578,7 +4605,7 @@
         <v>1984</v>
       </c>
       <c r="H66" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="K66">
         <v>3</v>
@@ -4605,7 +4632,7 @@
         <v>1986</v>
       </c>
       <c r="H67" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="K67">
         <v>7</v>
@@ -4648,7 +4675,7 @@
         <v>2002</v>
       </c>
       <c r="H68" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="K68">
         <v>6</v>
@@ -4675,7 +4702,7 @@
         <v>1988</v>
       </c>
       <c r="H69" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="K69">
         <v>8</v>
@@ -4702,7 +4729,7 @@
         <v>1992</v>
       </c>
       <c r="H70" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="K70">
         <v>10</v>
@@ -4729,7 +4756,7 @@
         <v>1985</v>
       </c>
       <c r="H71" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K71">
         <v>2</v>
@@ -4756,7 +4783,7 @@
         <v>1987</v>
       </c>
       <c r="H72" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="K72">
         <v>8</v>
@@ -4783,7 +4810,7 @@
         <v>1995</v>
       </c>
       <c r="H73" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -4810,7 +4837,7 @@
         <v>1989</v>
       </c>
       <c r="H74" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K74">
         <v>4</v>
@@ -4837,7 +4864,7 @@
         <v>991</v>
       </c>
       <c r="H75" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="K75">
         <v>10</v>
@@ -4864,7 +4891,7 @@
         <v>1992</v>
       </c>
       <c r="I76" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="K76">
         <v>5</v>
@@ -4891,7 +4918,7 @@
         <v>1991</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="K77">
         <v>2</v>
@@ -4918,7 +4945,7 @@
         <v>1992</v>
       </c>
       <c r="H78" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K78">
         <v>3</v>
@@ -4945,7 +4972,7 @@
         <v>1997</v>
       </c>
       <c r="H79" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="K79">
         <v>9</v>
@@ -4972,7 +4999,7 @@
         <v>1995</v>
       </c>
       <c r="H80" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="K80">
         <v>7</v>
@@ -4999,7 +5026,7 @@
         <v>1998</v>
       </c>
       <c r="H81" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="K81">
         <v>4</v>
@@ -5026,7 +5053,7 @@
         <v>2000</v>
       </c>
       <c r="H82" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="K82">
         <v>7</v>
@@ -5053,7 +5080,7 @@
         <v>1997</v>
       </c>
       <c r="H83" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="K83">
         <v>7</v>
@@ -5080,7 +5107,7 @@
         <v>1989</v>
       </c>
       <c r="H84" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="K84">
         <v>10</v>
@@ -5107,7 +5134,7 @@
         <v>1989</v>
       </c>
       <c r="H85" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="K85">
         <v>3</v>
@@ -5134,7 +5161,7 @@
         <v>1989</v>
       </c>
       <c r="H86" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="K86">
         <v>8</v>
@@ -5161,7 +5188,7 @@
         <v>2000</v>
       </c>
       <c r="H87" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="K87">
         <v>2</v>
@@ -5188,7 +5215,7 @@
         <v>1981</v>
       </c>
       <c r="H88" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="K88">
         <v>7</v>
@@ -5215,7 +5242,7 @@
         <v>1999</v>
       </c>
       <c r="H89" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="K89">
         <v>2</v>
@@ -5242,7 +5269,7 @@
         <v>1997</v>
       </c>
       <c r="H90" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -5269,7 +5296,7 @@
         <v>1980</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="K91">
         <v>4</v>
@@ -5296,7 +5323,7 @@
         <v>2000</v>
       </c>
       <c r="H92" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="K92">
         <v>10</v>
@@ -5323,7 +5350,7 @@
         <v>1986</v>
       </c>
       <c r="H93" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="K93">
         <v>5</v>
@@ -5350,7 +5377,7 @@
         <v>1995</v>
       </c>
       <c r="H94" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="K94">
         <v>4</v>
@@ -5377,7 +5404,7 @@
         <v>1997</v>
       </c>
       <c r="H95" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="K95">
         <v>3</v>
@@ -5404,7 +5431,7 @@
         <v>1993</v>
       </c>
       <c r="H96" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="K96">
         <v>4</v>
@@ -5431,7 +5458,7 @@
         <v>1983</v>
       </c>
       <c r="H97" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="K97">
         <v>3</v>
@@ -5458,7 +5485,7 @@
         <v>1994</v>
       </c>
       <c r="H98" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="K98">
         <v>2</v>
@@ -5485,7 +5512,7 @@
         <v>1985</v>
       </c>
       <c r="H99" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="K99">
         <v>6</v>
@@ -5512,7 +5539,7 @@
         <v>1989</v>
       </c>
       <c r="H100" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="K100">
         <v>2</v>
@@ -5539,7 +5566,7 @@
         <v>1979</v>
       </c>
       <c r="H101" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="K101">
         <v>3</v>
@@ -5566,7 +5593,7 @@
         <v>1998</v>
       </c>
       <c r="H102" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="K102">
         <v>3</v>
@@ -5593,7 +5620,7 @@
         <v>1996</v>
       </c>
       <c r="H103" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="K103">
         <v>3</v>
@@ -5620,7 +5647,7 @@
         <v>2010</v>
       </c>
       <c r="I104" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="K104">
         <v>9</v>
@@ -5647,7 +5674,7 @@
         <v>1991</v>
       </c>
       <c r="H105" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="K105">
         <v>6</v>
@@ -5674,7 +5701,7 @@
         <v>1980</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="K106">
         <v>5</v>
@@ -5701,7 +5728,7 @@
         <v>1991</v>
       </c>
       <c r="H107" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="K107">
         <v>4</v>
@@ -5728,7 +5755,7 @@
         <v>1984</v>
       </c>
       <c r="H108" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="K108">
         <v>7</v>
@@ -5755,7 +5782,7 @@
         <v>1989</v>
       </c>
       <c r="H109" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="K109">
         <v>10</v>
@@ -5782,7 +5809,7 @@
         <v>1977</v>
       </c>
       <c r="H110" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="K110">
         <v>1</v>
@@ -5812,7 +5839,7 @@
         <v>1973</v>
       </c>
       <c r="H111" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="K111">
         <v>3</v>
@@ -5839,7 +5866,7 @@
         <v>1967</v>
       </c>
       <c r="H112" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K112">
         <v>7</v>
@@ -5866,7 +5893,7 @@
         <v>1982</v>
       </c>
       <c r="H113" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="K113">
         <v>1</v>
@@ -5893,7 +5920,7 @@
         <v>1989</v>
       </c>
       <c r="H114" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="K114">
         <v>3</v>
@@ -5920,7 +5947,7 @@
         <v>1982</v>
       </c>
       <c r="H115" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="K115">
         <v>3</v>
@@ -5947,7 +5974,7 @@
         <v>1987</v>
       </c>
       <c r="H116" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="K116">
         <v>10</v>
@@ -5974,7 +6001,7 @@
         <v>1984</v>
       </c>
       <c r="H117" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="K117">
         <v>5</v>
@@ -6001,7 +6028,7 @@
         <v>1990</v>
       </c>
       <c r="H118" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="K118">
         <v>2</v>
@@ -6028,7 +6055,7 @@
         <v>1987</v>
       </c>
       <c r="H119" s="5" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="K119">
         <v>6</v>
@@ -6055,7 +6082,7 @@
         <v>1992</v>
       </c>
       <c r="H120" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K120">
         <v>9</v>
@@ -6082,7 +6109,7 @@
         <v>1964</v>
       </c>
       <c r="H121" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K121">
         <v>7</v>
@@ -6109,7 +6136,7 @@
         <v>1988</v>
       </c>
       <c r="H122" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="K122">
         <v>7</v>
@@ -6136,7 +6163,7 @@
         <v>1982</v>
       </c>
       <c r="H123" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="K123">
         <v>6</v>
@@ -6163,7 +6190,7 @@
         <v>1970</v>
       </c>
       <c r="H124" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K124">
         <v>2</v>
@@ -6193,7 +6220,7 @@
         <v>1992</v>
       </c>
       <c r="H125" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="K125">
         <v>5</v>
@@ -6220,7 +6247,7 @@
         <v>1979</v>
       </c>
       <c r="H126" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="K126">
         <v>2</v>
@@ -6247,7 +6274,7 @@
         <v>1985</v>
       </c>
       <c r="H127" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="K127">
         <v>1</v>
@@ -6277,7 +6304,7 @@
         <v>1990</v>
       </c>
       <c r="H128" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="K128">
         <v>1</v>
@@ -6304,7 +6331,7 @@
         <v>1986</v>
       </c>
       <c r="H129" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="K129">
         <v>5</v>
@@ -6334,7 +6361,7 @@
         <v>1986</v>
       </c>
       <c r="H130" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="K130">
         <v>1</v>
@@ -6361,7 +6388,7 @@
         <v>1990</v>
       </c>
       <c r="H131" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="K131">
         <v>3</v>
@@ -6407,7 +6434,7 @@
         <v>1995</v>
       </c>
       <c r="H132" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="K132">
         <v>8</v>
@@ -6434,7 +6461,7 @@
         <v>1992</v>
       </c>
       <c r="H133" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="K133">
         <v>10</v>
@@ -6461,7 +6488,7 @@
         <v>2004</v>
       </c>
       <c r="H134" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="K134">
         <v>8</v>
@@ -6488,7 +6515,7 @@
         <v>1986</v>
       </c>
       <c r="H135" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="K135">
         <v>2</v>
@@ -6515,7 +6542,7 @@
         <v>1993</v>
       </c>
       <c r="H136" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="K136">
         <v>10</v>
@@ -6542,7 +6569,7 @@
         <v>1996</v>
       </c>
       <c r="H137" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="K137">
         <v>3</v>
@@ -10045,22 +10072,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>586</v>
+      </c>
+      <c r="C2" t="s">
+        <v>587</v>
+      </c>
+      <c r="E2" t="s">
+        <v>588</v>
+      </c>
+      <c r="F2" t="s">
+        <v>591</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="C2" t="s">
-        <v>355</v>
-      </c>
-      <c r="E2" t="s">
-        <v>356</v>
-      </c>
-      <c r="F2" t="s">
-        <v>357</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>358</v>
-      </c>
       <c r="H2" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="J2" t="str">
         <f>_xlfn.CONCAT("(",
@@ -10070,9 +10097,9 @@
 IF(D2="","NULL",_xlfn.CONCAT("""",D2,"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",E2,"""")),",",
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
-IF(G2="","NULL",_xlfn.CONCAT("""",TEXT(G2,"YYYY-MM-DD"),"""")),",",
+IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),",",
 IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),"),")</f>
-        <v>("1","izabella","Izabella",NULL,"Patterson","izabella.patterson@ucalgary.ca","admin","admin"),</v>
+        <v>("1","irene","Irene",NULL,"Pauchard","i.pauchard@calgarywaldorf.org","admin","admin"),</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -10080,25 +10107,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>360</v>
+        <v>589</v>
       </c>
       <c r="C3" t="s">
-        <v>359</v>
-      </c>
-      <c r="D3" t="s">
-        <v>362</v>
+        <v>590</v>
       </c>
       <c r="E3" t="s">
-        <v>356</v>
+        <v>588</v>
       </c>
       <c r="F3" t="s">
-        <v>361</v>
+        <v>592</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="H3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="J3" t="str">
         <f>_xlfn.CONCAT("(",
@@ -10108,16 +10132,83 @@
 IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",E3,"""")),",",
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
-IF(G3="","NULL",_xlfn.CONCAT("""",TEXT(G3,"YYYY-MM-DD"),"""")),",",
-IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),");")</f>
-        <v>("2","yuvraj","Yuvraj","Yash","Patterson","yuvraj.patterson@ucalgary.ca","admin","admin");</v>
+IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),",",
+IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),"),")</f>
+        <v>("2","yves","Yves",NULL,"Pauchard","yves.pauchard@ucalgary.ca","admin","admin"),</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G4" s="1"/>
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>593</v>
+      </c>
+      <c r="C4" t="s">
+        <v>594</v>
+      </c>
+      <c r="E4" t="s">
+        <v>595</v>
+      </c>
+      <c r="F4" t="s">
+        <v>596</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H4" t="s">
+        <v>597</v>
+      </c>
+      <c r="J4" t="str">
+        <f>_xlfn.CONCAT("(",
+IF(A4="","NULL",_xlfn.CONCAT("""",A4,"""")),",",
+IF(B4="","NULL",_xlfn.CONCAT("""",B4,"""")),",",
+IF(C4="","NULL",_xlfn.CONCAT("""",C4,"""")),",",
+IF(D4="","NULL",_xlfn.CONCAT("""",D4,"""")),",",
+IF(E4="","NULL",_xlfn.CONCAT("""",E4,"""")),",",
+IF(F4="","NULL",_xlfn.CONCAT("""",F4,"""")),",",
+IF(G4="","NULL",_xlfn.CONCAT("""",G4,"""")),",",
+IF(H4="","NULL",_xlfn.CONCAT("""",H4,"""")),"),")</f>
+        <v>("3","zbhavyai","Bhavyai",NULL,"Gupta","zbhavyai@gmail.com","admin","faculty"),</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G5" s="1"/>
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>598</v>
+      </c>
+      <c r="C5" t="s">
+        <v>600</v>
+      </c>
+      <c r="D5" t="s">
+        <v>601</v>
+      </c>
+      <c r="E5" t="s">
+        <v>602</v>
+      </c>
+      <c r="F5" t="s">
+        <v>599</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H5" t="s">
+        <v>354</v>
+      </c>
+      <c r="J5" t="str">
+        <f>_xlfn.CONCAT("(",
+IF(A5="","NULL",_xlfn.CONCAT("""",A5,"""")),",",
+IF(B5="","NULL",_xlfn.CONCAT("""",B5,"""")),",",
+IF(C5="","NULL",_xlfn.CONCAT("""",C5,"""")),",",
+IF(D5="","NULL",_xlfn.CONCAT("""",D5,"""")),",",
+IF(E5="","NULL",_xlfn.CONCAT("""",E5,"""")),",",
+IF(F5="","NULL",_xlfn.CONCAT("""",F5,"""")),",",
+IF(G5="","NULL",_xlfn.CONCAT("""",G5,"""")),",",
+IF(H5="","NULL",_xlfn.CONCAT("""",H5,"""")),");")</f>
+        <v>("4","mmylee","Michael","Man Yin","Lee","mmylee@ucalgary.ca","admin","admin");</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G6" s="1"/>
@@ -10185,13 +10276,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>348</v>
@@ -10203,10 +10294,10 @@
         <v>350</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="J1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO loaner (",
@@ -10223,7 +10314,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -10233,10 +10324,10 @@
         <v>Mr</v>
       </c>
       <c r="D2" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="F2" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="G2" s="1"/>
       <c r="J2" t="str">
@@ -10254,7 +10345,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -10264,10 +10355,10 @@
         <v>Mr</v>
       </c>
       <c r="D3" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="F3" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" t="str">
@@ -10285,7 +10376,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -10295,16 +10386,16 @@
         <v/>
       </c>
       <c r="D4" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="F4" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="1"/>
@@ -10313,7 +10404,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -10323,16 +10414,16 @@
         <v/>
       </c>
       <c r="D5" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="F5" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="1"/>
@@ -10341,7 +10432,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -10351,16 +10442,16 @@
         <v/>
       </c>
       <c r="D6" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F6" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="1"/>
@@ -10369,7 +10460,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -10379,16 +10470,16 @@
         <v/>
       </c>
       <c r="D7" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="F7" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="1"/>
@@ -10397,7 +10488,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -10407,16 +10498,16 @@
         <v/>
       </c>
       <c r="D8" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F8" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="1"/>
@@ -10425,7 +10516,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -10435,16 +10526,16 @@
         <v/>
       </c>
       <c r="D9" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="F9" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="1"/>
@@ -10453,7 +10544,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -10463,16 +10554,16 @@
         <v/>
       </c>
       <c r="D10" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="F10" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="1"/>
@@ -10481,7 +10572,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -10491,16 +10582,16 @@
         <v/>
       </c>
       <c r="D11" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="F11" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="1"/>
@@ -10509,7 +10600,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -10519,16 +10610,16 @@
         <v/>
       </c>
       <c r="D12" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="F12" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="1"/>
@@ -10537,7 +10628,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -10547,16 +10638,16 @@
         <v/>
       </c>
       <c r="D13" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="F13" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="1"/>
@@ -10565,7 +10656,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -10575,10 +10666,10 @@
         <v>Mr</v>
       </c>
       <c r="D14" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="F14" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="G14" s="1"/>
       <c r="J14" t="str">
@@ -10588,7 +10679,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -10598,10 +10689,10 @@
         <v>Mr</v>
       </c>
       <c r="D15" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="F15" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="G15" s="1"/>
       <c r="J15" t="str">
@@ -10611,7 +10702,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -10621,10 +10712,10 @@
         <v>Mr</v>
       </c>
       <c r="D16" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="F16" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="G16" s="1"/>
       <c r="J16" t="str">
@@ -10634,7 +10725,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -10644,16 +10735,16 @@
         <v/>
       </c>
       <c r="D17" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="F17" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="H17" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="1"/>
@@ -10662,7 +10753,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -10672,16 +10763,16 @@
         <v/>
       </c>
       <c r="D18" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="F18" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="H18" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="1"/>
@@ -10690,7 +10781,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -10700,16 +10791,16 @@
         <v/>
       </c>
       <c r="D19" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="F19" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="H19" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="1"/>
@@ -10718,7 +10809,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -10728,16 +10819,16 @@
         <v/>
       </c>
       <c r="D20" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="F20" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="H20" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="1"/>
@@ -10746,7 +10837,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -10756,16 +10847,16 @@
         <v/>
       </c>
       <c r="D21" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="F21" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="H21" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="J21" t="str">
         <f>_xlfn.CONCAT("(",
@@ -10802,16 +10893,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="G1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO loan (",
@@ -11296,16 +11387,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="F1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO transaction (",
@@ -11330,7 +11421,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <f>_xlfn.CONCAT("(",
+        <f t="shared" ref="F2:F30" si="0">_xlfn.CONCAT("(",
 IF(A2="","NULL",_xlfn.CONCAT("""",TEXT(A2,"YYYY-MM-DD hh:mm:ss"),"""")),",",
 IF(B2="","NULL",_xlfn.CONCAT("""",B2,"""")),",",
 IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
@@ -11352,11 +11443,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A3="","NULL",_xlfn.CONCAT("""",TEXT(A3,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B3="","NULL",_xlfn.CONCAT("""",B3,"""")),",",
-IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
-IF(D3="","NULL",_xlfn.CONCAT("""",D3,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-01-16 16:09:51","0","2","2"),</v>
       </c>
     </row>
@@ -11374,11 +11461,7 @@
         <v>3</v>
       </c>
       <c r="F4" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A4="","NULL",_xlfn.CONCAT("""",TEXT(A4,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B4="","NULL",_xlfn.CONCAT("""",B4,"""")),",",
-IF(C4="","NULL",_xlfn.CONCAT("""",C4,"""")),",",
-IF(D4="","NULL",_xlfn.CONCAT("""",D4,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-02-07 10:31:55","0","2","3"),</v>
       </c>
     </row>
@@ -11396,11 +11479,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A5="","NULL",_xlfn.CONCAT("""",TEXT(A5,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B5="","NULL",_xlfn.CONCAT("""",B5,"""")),",",
-IF(C5="","NULL",_xlfn.CONCAT("""",C5,"""")),",",
-IF(D5="","NULL",_xlfn.CONCAT("""",D5,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-02-20 12:16:16","0","1","4"),</v>
       </c>
     </row>
@@ -11418,11 +11497,7 @@
         <v>5</v>
       </c>
       <c r="F6" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A6="","NULL",_xlfn.CONCAT("""",TEXT(A6,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B6="","NULL",_xlfn.CONCAT("""",B6,"""")),",",
-IF(C6="","NULL",_xlfn.CONCAT("""",C6,"""")),",",
-IF(D6="","NULL",_xlfn.CONCAT("""",D6,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-03-30 16:07:06","0","1","5"),</v>
       </c>
     </row>
@@ -11440,11 +11515,7 @@
         <v>6</v>
       </c>
       <c r="F7" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A7="","NULL",_xlfn.CONCAT("""",TEXT(A7,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B7="","NULL",_xlfn.CONCAT("""",B7,"""")),",",
-IF(C7="","NULL",_xlfn.CONCAT("""",C7,"""")),",",
-IF(D7="","NULL",_xlfn.CONCAT("""",D7,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-03-13 12:35:03","0","2","6"),</v>
       </c>
     </row>
@@ -11462,11 +11533,7 @@
         <v>7</v>
       </c>
       <c r="F8" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A8="","NULL",_xlfn.CONCAT("""",TEXT(A8,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B8="","NULL",_xlfn.CONCAT("""",B8,"""")),",",
-IF(C8="","NULL",_xlfn.CONCAT("""",C8,"""")),",",
-IF(D8="","NULL",_xlfn.CONCAT("""",D8,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-04-04 14:04:56","0","1","7"),</v>
       </c>
     </row>
@@ -11484,11 +11551,7 @@
         <v>8</v>
       </c>
       <c r="F9" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A9="","NULL",_xlfn.CONCAT("""",TEXT(A9,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B9="","NULL",_xlfn.CONCAT("""",B9,"""")),",",
-IF(C9="","NULL",_xlfn.CONCAT("""",C9,"""")),",",
-IF(D9="","NULL",_xlfn.CONCAT("""",D9,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-04-01 14:02:00","0","1","8"),</v>
       </c>
     </row>
@@ -11506,11 +11569,7 @@
         <v>9</v>
       </c>
       <c r="F10" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A10="","NULL",_xlfn.CONCAT("""",TEXT(A10,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B10="","NULL",_xlfn.CONCAT("""",B10,"""")),",",
-IF(C10="","NULL",_xlfn.CONCAT("""",C10,"""")),",",
-IF(D10="","NULL",_xlfn.CONCAT("""",D10,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-05-19 11:17:57","0","2","9"),</v>
       </c>
     </row>
@@ -11528,11 +11587,7 @@
         <v>10</v>
       </c>
       <c r="F11" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A11="","NULL",_xlfn.CONCAT("""",TEXT(A11,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B11="","NULL",_xlfn.CONCAT("""",B11,"""")),",",
-IF(C11="","NULL",_xlfn.CONCAT("""",C11,"""")),",",
-IF(D11="","NULL",_xlfn.CONCAT("""",D11,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-05-18 16:15:25","0","2","10"),</v>
       </c>
     </row>
@@ -11551,11 +11606,7 @@
         <v>11</v>
       </c>
       <c r="F12" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A12="","NULL",_xlfn.CONCAT("""",TEXT(A12,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B12="","NULL",_xlfn.CONCAT("""",B12,"""")),",",
-IF(C12="","NULL",_xlfn.CONCAT("""",C12,"""")),",",
-IF(D12="","NULL",_xlfn.CONCAT("""",D12,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-02-08 11:10:17","0","1","11"),</v>
       </c>
     </row>
@@ -11570,15 +11621,11 @@
         <v>1</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" ref="D13:D21" si="0">D12+1</f>
+        <f t="shared" ref="D13:D21" si="1">D12+1</f>
         <v>12</v>
       </c>
       <c r="F13" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A13="","NULL",_xlfn.CONCAT("""",TEXT(A13,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B13="","NULL",_xlfn.CONCAT("""",B13,"""")),",",
-IF(C13="","NULL",_xlfn.CONCAT("""",C13,"""")),",",
-IF(D13="","NULL",_xlfn.CONCAT("""",D13,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-01-28 10:20:40","0","1","12"),</v>
       </c>
     </row>
@@ -11593,15 +11640,11 @@
         <v>1</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="F14" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A14="","NULL",_xlfn.CONCAT("""",TEXT(A14,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B14="","NULL",_xlfn.CONCAT("""",B14,"""")),",",
-IF(C14="","NULL",_xlfn.CONCAT("""",C14,"""")),",",
-IF(D14="","NULL",_xlfn.CONCAT("""",D14,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-02-19 13:11:52","0","1","13"),</v>
       </c>
     </row>
@@ -11616,15 +11659,11 @@
         <v>1</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="F15" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A15="","NULL",_xlfn.CONCAT("""",TEXT(A15,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B15="","NULL",_xlfn.CONCAT("""",B15,"""")),",",
-IF(C15="","NULL",_xlfn.CONCAT("""",C15,"""")),",",
-IF(D15="","NULL",_xlfn.CONCAT("""",D15,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-03-04 14:02:42","0","1","14"),</v>
       </c>
     </row>
@@ -11639,15 +11678,11 @@
         <v>2</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="F16" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A16="","NULL",_xlfn.CONCAT("""",TEXT(A16,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B16="","NULL",_xlfn.CONCAT("""",B16,"""")),",",
-IF(C16="","NULL",_xlfn.CONCAT("""",C16,"""")),",",
-IF(D16="","NULL",_xlfn.CONCAT("""",D16,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-04-11 13:47:58","0","2","15"),</v>
       </c>
     </row>
@@ -11662,15 +11697,11 @@
         <v>1</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="F17" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A17="","NULL",_xlfn.CONCAT("""",TEXT(A17,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B17="","NULL",_xlfn.CONCAT("""",B17,"""")),",",
-IF(C17="","NULL",_xlfn.CONCAT("""",C17,"""")),",",
-IF(D17="","NULL",_xlfn.CONCAT("""",D17,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-03-25 12:08:56","0","1","16"),</v>
       </c>
     </row>
@@ -11685,15 +11716,11 @@
         <v>1</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="F18" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A18="","NULL",_xlfn.CONCAT("""",TEXT(A18,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B18="","NULL",_xlfn.CONCAT("""",B18,"""")),",",
-IF(C18="","NULL",_xlfn.CONCAT("""",C18,"""")),",",
-IF(D18="","NULL",_xlfn.CONCAT("""",D18,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-04-16 10:26:39","0","1","17"),</v>
       </c>
     </row>
@@ -11708,15 +11735,11 @@
         <v>1</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="F19" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A19="","NULL",_xlfn.CONCAT("""",TEXT(A19,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B19="","NULL",_xlfn.CONCAT("""",B19,"""")),",",
-IF(C19="","NULL",_xlfn.CONCAT("""",C19,"""")),",",
-IF(D19="","NULL",_xlfn.CONCAT("""",D19,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-04-13 16:25:58","0","1","18"),</v>
       </c>
     </row>
@@ -11731,15 +11754,11 @@
         <v>1</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="F20" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A20="","NULL",_xlfn.CONCAT("""",TEXT(A20,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B20="","NULL",_xlfn.CONCAT("""",B20,"""")),",",
-IF(C20="","NULL",_xlfn.CONCAT("""",C20,"""")),",",
-IF(D20="","NULL",_xlfn.CONCAT("""",D20,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-05-31 13:21:20","0","1","19"),</v>
       </c>
     </row>
@@ -11754,15 +11773,11 @@
         <v>2</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F21" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A21="","NULL",_xlfn.CONCAT("""",TEXT(A21,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B21="","NULL",_xlfn.CONCAT("""",B21,"""")),",",
-IF(C21="","NULL",_xlfn.CONCAT("""",C21,"""")),",",
-IF(D21="","NULL",_xlfn.CONCAT("""",D21,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-05-30 16:08:04","0","2","20"),</v>
       </c>
     </row>
@@ -11780,11 +11795,7 @@
         <v>11</v>
       </c>
       <c r="F22" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A22="","NULL",_xlfn.CONCAT("""",TEXT(A22,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B22="","NULL",_xlfn.CONCAT("""",B22,"""")),",",
-IF(C22="","NULL",_xlfn.CONCAT("""",C22,"""")),",",
-IF(D22="","NULL",_xlfn.CONCAT("""",D22,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-02-20 16:00:53","1","1","11"),</v>
       </c>
     </row>
@@ -11802,11 +11813,7 @@
         <v>12</v>
       </c>
       <c r="F23" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A23="","NULL",_xlfn.CONCAT("""",TEXT(A23,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B23="","NULL",_xlfn.CONCAT("""",B23,"""")),",",
-IF(C23="","NULL",_xlfn.CONCAT("""",C23,"""")),",",
-IF(D23="","NULL",_xlfn.CONCAT("""",D23,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-02-09 12:03:54","1","1","12"),</v>
       </c>
     </row>
@@ -11824,11 +11831,7 @@
         <v>13</v>
       </c>
       <c r="F24" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A24="","NULL",_xlfn.CONCAT("""",TEXT(A24,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B24="","NULL",_xlfn.CONCAT("""",B24,"""")),",",
-IF(C24="","NULL",_xlfn.CONCAT("""",C24,"""")),",",
-IF(D24="","NULL",_xlfn.CONCAT("""",D24,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-03-03 10:36:39","1","1","13"),</v>
       </c>
     </row>
@@ -11846,11 +11849,7 @@
         <v>14</v>
       </c>
       <c r="F25" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A25="","NULL",_xlfn.CONCAT("""",TEXT(A25,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B25="","NULL",_xlfn.CONCAT("""",B25,"""")),",",
-IF(C25="","NULL",_xlfn.CONCAT("""",C25,"""")),",",
-IF(D25="","NULL",_xlfn.CONCAT("""",D25,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-03-16 11:41:07","1","1","14"),</v>
       </c>
     </row>
@@ -11868,11 +11867,7 @@
         <v>15</v>
       </c>
       <c r="F26" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A26="","NULL",_xlfn.CONCAT("""",TEXT(A26,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B26="","NULL",_xlfn.CONCAT("""",B26,"""")),",",
-IF(C26="","NULL",_xlfn.CONCAT("""",C26,"""")),",",
-IF(D26="","NULL",_xlfn.CONCAT("""",D26,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-04-23 16:50:25","1","2","15"),</v>
       </c>
     </row>
@@ -11890,11 +11885,7 @@
         <v>16</v>
       </c>
       <c r="F27" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A27="","NULL",_xlfn.CONCAT("""",TEXT(A27,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B27="","NULL",_xlfn.CONCAT("""",B27,"""")),",",
-IF(C27="","NULL",_xlfn.CONCAT("""",C27,"""")),",",
-IF(D27="","NULL",_xlfn.CONCAT("""",D27,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-04-06 15:15:35","1","1","16"),</v>
       </c>
     </row>
@@ -11912,11 +11903,7 @@
         <v>17</v>
       </c>
       <c r="F28" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A28="","NULL",_xlfn.CONCAT("""",TEXT(A28,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B28="","NULL",_xlfn.CONCAT("""",B28,"""")),",",
-IF(C28="","NULL",_xlfn.CONCAT("""",C28,"""")),",",
-IF(D28="","NULL",_xlfn.CONCAT("""",D28,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-04-28 14:36:28","1","1","17"),</v>
       </c>
     </row>
@@ -11934,11 +11921,7 @@
         <v>18</v>
       </c>
       <c r="F29" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A29="","NULL",_xlfn.CONCAT("""",TEXT(A29,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B29="","NULL",_xlfn.CONCAT("""",B29,"""")),",",
-IF(C29="","NULL",_xlfn.CONCAT("""",C29,"""")),",",
-IF(D29="","NULL",_xlfn.CONCAT("""",D29,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-04-25 12:06:36","1","1","18"),</v>
       </c>
     </row>
@@ -11956,11 +11939,7 @@
         <v>19</v>
       </c>
       <c r="F30" t="str">
-        <f>_xlfn.CONCAT("(",
-IF(A30="","NULL",_xlfn.CONCAT("""",TEXT(A30,"YYYY-MM-DD hh:mm:ss"),"""")),",",
-IF(B30="","NULL",_xlfn.CONCAT("""",B30,"""")),",",
-IF(C30="","NULL",_xlfn.CONCAT("""",C30,"""")),",",
-IF(D30="","NULL",_xlfn.CONCAT("""",D30,"""")),"),")</f>
+        <f t="shared" si="0"/>
         <v>("2021-06-12 14:25:59","1","1","19"),</v>
       </c>
     </row>
@@ -12005,13 +11984,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="E1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO trn_quantities (",

</xml_diff>

<commit_message>
fix: #11 #12 fixing basic authentication of librarians
</commit_message>
<xml_diff>
--- a/sql/02_dummy_data_generator.xlsx
+++ b/sql/02_dummy_data_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\budlib\budlib-api\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEC2C0C-9DE3-47D8-8F5F-1E1035A38B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2F6F69-9739-479A-8C11-20474CF07386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="608">
   <si>
     <t>book_id</t>
   </si>
@@ -1849,6 +1849,21 @@
   </si>
   <si>
     <t>Lee</t>
+  </si>
+  <si>
+    <t>PARENT</t>
+  </si>
+  <si>
+    <t>$2a$10$..4RvEGzO5/TiayeVSm1lOTHqo456ZPPCrf7G7.eyPvndgkICr/tq</t>
+  </si>
+  <si>
+    <t>$2a$10$Gitv.jdJOSpID30NmPEqn.IwH5CztayH4HbRUjxGDJKNM3DWCwMmy</t>
+  </si>
+  <si>
+    <t>$2a$10$GWg.rygxrh6caI2PaZTFvOreHBGaglUmkx1tyhutkxPN0QC1G1oT2</t>
+  </si>
+  <si>
+    <t>$2a$10$vrf9vKF0tT3xBQlEFbVjje.4LZgyCtRfBaIjCf4KO0QDQuvOKEijC</t>
   </si>
 </sst>
 </file>
@@ -2807,9 +2822,8 @@
         <v>1986</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="J2" t="str">
-        <f>SUBSTITUTE(H2,"-","")</f>
-        <v/>
+      <c r="J2" t="s">
+        <v>603</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -2835,7 +2849,7 @@
 IF(N2="","NULL",_xlfn.CONCAT("""",N2,"""")),",",
 IF(O2="","NULL",_xlfn.CONCAT("""",O2,"""")),",",
 IF(P2="","NULL",_xlfn.CONCAT("""",P2,"""")),"),")</f>
-        <v>("Education Towards Freedom",NULL,"Rudel, Joan and Siegfried","Lanthorn Press, Peredur, East Grinstead, England","4","1986",NULL,NULL,NULL,NULL,"1","0",NULL,NULL,NULL,NULL),</v>
+        <v>("Education Towards Freedom",NULL,"Rudel, Joan and Siegfried","Lanthorn Press, Peredur, East Grinstead, England","4","1986",NULL,NULL,NULL,"PARENT","1","0",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -2854,6 +2868,9 @@
       <c r="G3" s="1"/>
       <c r="H3" t="s">
         <v>413</v>
+      </c>
+      <c r="J3" t="s">
+        <v>603</v>
       </c>
       <c r="K3">
         <v>4</v>
@@ -2879,7 +2896,7 @@
 IF(N3="","NULL",_xlfn.CONCAT("""",N3,"""")),",",
 IF(O3="","NULL",_xlfn.CONCAT("""",O3,"""")),",",
 IF(P3="","NULL",_xlfn.CONCAT("""",P3,"""")),"),")</f>
-        <v>("Bullying - Changing the Course of Your Child's Life",NULL,"Voors, William","Hazelden",NULL,"2000",NULL,"156838517X",NULL,NULL,"4","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Bullying - Changing the Course of Your Child's Life",NULL,"Voors, William","Hazelden",NULL,"2000",NULL,"156838517X",NULL,"PARENT","4","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -2899,6 +2916,9 @@
       <c r="H4" t="s">
         <v>414</v>
       </c>
+      <c r="J4" t="s">
+        <v>603</v>
+      </c>
       <c r="K4">
         <v>9</v>
       </c>
@@ -2907,7 +2927,7 @@
       </c>
       <c r="R4" t="str">
         <f t="shared" si="0"/>
-        <v>("Awakening Your Child's Natural Genius",NULL,"Armstrong, Thomas","Jeremy P. Tarcher, Inc., Los Angeles",NULL,"1991",NULL,"0874776082",NULL,NULL,"9","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Awakening Your Child's Natural Genius",NULL,"Armstrong, Thomas","Jeremy P. Tarcher, Inc., Los Angeles",NULL,"1991",NULL,"0874776082",NULL,"PARENT","9","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -2927,6 +2947,9 @@
       <c r="H5" t="s">
         <v>415</v>
       </c>
+      <c r="J5" t="s">
+        <v>603</v>
+      </c>
       <c r="K5">
         <v>3</v>
       </c>
@@ -2935,7 +2958,7 @@
       </c>
       <c r="R5" t="str">
         <f t="shared" si="0"/>
-        <v>("From Your Child's Teacher",NULL,"Bright, Robin","FP Hendricks Publishing Ltd.",NULL,"1998",NULL,"096829703X",NULL,NULL,"3","0",NULL,NULL,NULL,NULL),</v>
+        <v>("From Your Child's Teacher",NULL,"Bright, Robin","FP Hendricks Publishing Ltd.",NULL,"1998",NULL,"096829703X",NULL,"PARENT","3","0",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -2955,6 +2978,9 @@
       <c r="H6" t="s">
         <v>416</v>
       </c>
+      <c r="J6" t="s">
+        <v>603</v>
+      </c>
       <c r="K6">
         <v>2</v>
       </c>
@@ -2963,7 +2989,7 @@
       </c>
       <c r="R6" t="str">
         <f t="shared" si="0"/>
-        <v>("Parents Do Make a Difference",NULL,"Borba, Michele","Jossey-Bass",NULL,"1999",NULL,"0787946052",NULL,NULL,"2","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Parents Do Make a Difference",NULL,"Borba, Michele","Jossey-Bass",NULL,"1999",NULL,"0787946052",NULL,"PARENT","2","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -2983,6 +3009,9 @@
       <c r="H7" t="s">
         <v>417</v>
       </c>
+      <c r="J7" t="s">
+        <v>603</v>
+      </c>
       <c r="K7">
         <v>4</v>
       </c>
@@ -2991,7 +3020,7 @@
       </c>
       <c r="R7" t="str">
         <f t="shared" si="0"/>
-        <v>("Rythms of Learning",NULL,"Trostli, Roberto","Anthroposophic Press",NULL,"1998",NULL,"0880104511",NULL,NULL,"4","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Rythms of Learning",NULL,"Trostli, Roberto","Anthroposophic Press",NULL,"1998",NULL,"0880104511",NULL,"PARENT","4","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -3011,6 +3040,9 @@
       <c r="H8" t="s">
         <v>418</v>
       </c>
+      <c r="J8" t="s">
+        <v>603</v>
+      </c>
       <c r="K8">
         <v>9</v>
       </c>
@@ -3019,7 +3051,7 @@
       </c>
       <c r="R8" t="str">
         <f t="shared" si="0"/>
-        <v>("Parents as People",NULL,"Kane, Franklin G.","Aurora Publishers",NULL,"1987",NULL,"0889258201",NULL,NULL,"9","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Parents as People",NULL,"Kane, Franklin G.","Aurora Publishers",NULL,"1987",NULL,"0889258201",NULL,"PARENT","9","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -3039,6 +3071,9 @@
       <c r="H9" t="s">
         <v>419</v>
       </c>
+      <c r="J9" t="s">
+        <v>603</v>
+      </c>
       <c r="K9">
         <v>10</v>
       </c>
@@ -3047,7 +3082,7 @@
       </c>
       <c r="R9" t="str">
         <f t="shared" si="0"/>
-        <v>("Spelling for Parents",NULL,"Phenix, Jo / Scott-Dunne, Doreen","Pembrook Publishers Limited",NULL,"1994",NULL,"1551380196",NULL,NULL,"10","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Spelling for Parents",NULL,"Phenix, Jo / Scott-Dunne, Doreen","Pembrook Publishers Limited",NULL,"1994",NULL,"1551380196",NULL,"PARENT","10","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -3070,6 +3105,9 @@
       <c r="H10" t="s">
         <v>420</v>
       </c>
+      <c r="J10" t="s">
+        <v>603</v>
+      </c>
       <c r="K10">
         <v>9</v>
       </c>
@@ -3078,7 +3116,7 @@
       </c>
       <c r="R10" t="str">
         <f t="shared" si="0"/>
-        <v>("Lifeways - Working with Family Questions",NULL,"Davy, Gudrun / Voors, Bons","Hawthorn Press","3","1985",NULL,"0950706248",NULL,NULL,"9","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Lifeways - Working with Family Questions",NULL,"Davy, Gudrun / Voors, Bons","Hawthorn Press","3","1985",NULL,"0950706248",NULL,"PARENT","9","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -3098,6 +3136,9 @@
       <c r="H11" t="s">
         <v>421</v>
       </c>
+      <c r="J11" t="s">
+        <v>603</v>
+      </c>
       <c r="K11">
         <v>1</v>
       </c>
@@ -3106,7 +3147,7 @@
       </c>
       <c r="R11" t="str">
         <f t="shared" si="0"/>
-        <v>("Why Motor Skills Matter",NULL,"Losquadro Liddle, Tara","The McGraw-Hill Companies",NULL,"2004",NULL,"0071408185",NULL,NULL,"1","0",NULL,NULL,NULL,NULL),</v>
+        <v>("Why Motor Skills Matter",NULL,"Losquadro Liddle, Tara","The McGraw-Hill Companies",NULL,"2004",NULL,"0071408185",NULL,"PARENT","1","0",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -3126,6 +3167,9 @@
       <c r="H12" t="s">
         <v>422</v>
       </c>
+      <c r="J12" t="s">
+        <v>603</v>
+      </c>
       <c r="K12">
         <v>1</v>
       </c>
@@ -3134,7 +3178,7 @@
       </c>
       <c r="R12" t="str">
         <f t="shared" si="0"/>
-        <v>("A Guide to Child Health",NULL,"Gloeckler, Michaela / Goebel, Wolfgang","Floris Books",NULL,"1984",NULL,"0863151043",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("A Guide to Child Health",NULL,"Gloeckler, Michaela / Goebel, Wolfgang","Floris Books",NULL,"1984",NULL,"0863151043",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -3154,6 +3198,9 @@
       <c r="H13" t="s">
         <v>423</v>
       </c>
+      <c r="J13" t="s">
+        <v>603</v>
+      </c>
       <c r="K13">
         <v>6</v>
       </c>
@@ -3162,7 +3209,7 @@
       </c>
       <c r="R13" t="str">
         <f t="shared" si="0"/>
-        <v>("Navigating the Terrain of Childhood",NULL,"Petrash, Jack","Nova Institute Press",NULL,"2004",NULL,"0975855204",NULL,NULL,"6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Navigating the Terrain of Childhood",NULL,"Petrash, Jack","Nova Institute Press",NULL,"2004",NULL,"0975855204",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -3183,6 +3230,9 @@
       <c r="I14" s="4" t="s">
         <v>537</v>
       </c>
+      <c r="J14" t="s">
+        <v>603</v>
+      </c>
       <c r="K14">
         <v>1</v>
       </c>
@@ -3191,7 +3241,7 @@
       </c>
       <c r="R14" t="str">
         <f t="shared" si="0"/>
-        <v>("Healign Stories for Challenging Behaviour",NULL,"Perrow, Susan","Hawthorn Press",NULL,"2012",NULL,NULL,"9781903458785",NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Healign Stories for Challenging Behaviour",NULL,"Perrow, Susan","Hawthorn Press",NULL,"2012",NULL,NULL,"9781903458785","PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -3211,6 +3261,9 @@
       <c r="H15" t="s">
         <v>424</v>
       </c>
+      <c r="J15" t="s">
+        <v>603</v>
+      </c>
       <c r="K15">
         <v>7</v>
       </c>
@@ -3219,7 +3272,7 @@
       </c>
       <c r="R15" t="str">
         <f t="shared" si="0"/>
-        <v>("Hold on to Your Kids",NULL,"Neufeld, Gordon / Mate, Gabor","Vintage Canada",NULL,"2005",NULL,"0676974724",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Hold on to Your Kids",NULL,"Neufeld, Gordon / Mate, Gabor","Vintage Canada",NULL,"2005",NULL,"0676974724",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -3236,6 +3289,9 @@
         <v>1982</v>
       </c>
       <c r="G16" s="1"/>
+      <c r="J16" t="s">
+        <v>603</v>
+      </c>
       <c r="K16">
         <v>1</v>
       </c>
@@ -3244,7 +3300,7 @@
       </c>
       <c r="R16" t="str">
         <f t="shared" si="0"/>
-        <v>("Echoes of a Dream",NULL,"Smith, Susan","Beacon Herald Fine Printing Division, Stratford, Ontario, Canada",NULL,"1982",NULL,NULL,NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Echoes of a Dream",NULL,"Smith, Susan","Beacon Herald Fine Printing Division, Stratford, Ontario, Canada",NULL,"1982",NULL,NULL,NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
@@ -3264,6 +3320,9 @@
       <c r="H17" t="s">
         <v>426</v>
       </c>
+      <c r="J17" t="s">
+        <v>603</v>
+      </c>
       <c r="K17">
         <v>6</v>
       </c>
@@ -3272,7 +3331,7 @@
       </c>
       <c r="R17" t="str">
         <f t="shared" si="0"/>
-        <v>("If Learning is so Natural, Why am I going to School?",NULL,"Nikiforuk, Andrew","Penguin Books",NULL,"1994",NULL,"0140242643",NULL,NULL,"6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("If Learning is so Natural, Why am I going to School?",NULL,"Nikiforuk, Andrew","Penguin Books",NULL,"1994",NULL,"0140242643",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
@@ -3295,6 +3354,9 @@
       <c r="H18" t="s">
         <v>427</v>
       </c>
+      <c r="J18" t="s">
+        <v>603</v>
+      </c>
       <c r="K18">
         <v>1</v>
       </c>
@@ -3303,7 +3365,7 @@
       </c>
       <c r="R18" t="str">
         <f t="shared" si="0"/>
-        <v>("The Gift of Dyslexia",NULL,"Davis, Ronald D.","The Berkely Publishing Group","2","1997",NULL,"039952293X",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("The Gift of Dyslexia",NULL,"Davis, Ronald D.","The Berkely Publishing Group","2","1997",NULL,"039952293X",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
@@ -3323,6 +3385,9 @@
       <c r="H19" t="s">
         <v>428</v>
       </c>
+      <c r="J19" t="s">
+        <v>603</v>
+      </c>
       <c r="K19">
         <v>7</v>
       </c>
@@ -3331,7 +3396,7 @@
       </c>
       <c r="R19" t="str">
         <f t="shared" si="0"/>
-        <v>("the Out-of-Sync Child",NULL,"Stock Kranowitz, Carol","The Berkely Publishing Group",NULL,"2005",NULL,"0399531653",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("the Out-of-Sync Child",NULL,"Stock Kranowitz, Carol","The Berkely Publishing Group",NULL,"2005",NULL,"0399531653",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
@@ -3350,6 +3415,9 @@
       <c r="H20" t="s">
         <v>429</v>
       </c>
+      <c r="J20" t="s">
+        <v>603</v>
+      </c>
       <c r="K20">
         <v>1</v>
       </c>
@@ -3358,7 +3426,7 @@
       </c>
       <c r="R20" t="str">
         <f t="shared" si="0"/>
-        <v>("The Optimistic Child",NULL,"Seligman, Martin E.","Harper Perennial",NULL,"1995",NULL,"0060977094",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("The Optimistic Child",NULL,"Seligman, Martin E.","Harper Perennial",NULL,"1995",NULL,"0060977094",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -3377,6 +3445,9 @@
       <c r="H21" s="4" t="s">
         <v>538</v>
       </c>
+      <c r="J21" t="s">
+        <v>603</v>
+      </c>
       <c r="K21">
         <v>4</v>
       </c>
@@ -3385,7 +3456,7 @@
       </c>
       <c r="R21" t="str">
         <f t="shared" si="0"/>
-        <v>("365 Outdoor Activities",NULL,"Bennett, Steve and Ruth","Bob Adams, Inc., Publishers",NULL,"1993",NULL,"1558502602",NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("365 Outdoor Activities",NULL,"Bennett, Steve and Ruth","Bob Adams, Inc., Publishers",NULL,"1993",NULL,"1558502602",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
@@ -3404,6 +3475,9 @@
       <c r="H22" t="s">
         <v>430</v>
       </c>
+      <c r="J22" t="s">
+        <v>603</v>
+      </c>
       <c r="K22">
         <v>10</v>
       </c>
@@ -3412,7 +3486,7 @@
       </c>
       <c r="R22" t="str">
         <f t="shared" si="0"/>
-        <v>("Kids are Worth it!",NULL,"Coloroso, Barbara","Somerville House Publishing",NULL,"1994",NULL,"0921051743",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Kids are Worth it!",NULL,"Coloroso, Barbara","Somerville House Publishing",NULL,"1994",NULL,"0921051743",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -3431,6 +3505,9 @@
       <c r="H23" t="s">
         <v>431</v>
       </c>
+      <c r="J23" t="s">
+        <v>603</v>
+      </c>
       <c r="K23">
         <v>1</v>
       </c>
@@ -3439,7 +3516,7 @@
       </c>
       <c r="R23" t="str">
         <f t="shared" si="0"/>
-        <v>("How to Keep Your Teenager Out of Troubl and What to Do if You Can't",NULL,"Bernstein, Neil I.","Workman Publishing",NULL,"2001",NULL,"0761115706",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("How to Keep Your Teenager Out of Troubl and What to Do if You Can't",NULL,"Bernstein, Neil I.","Workman Publishing",NULL,"2001",NULL,"0761115706",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -3458,6 +3535,9 @@
       <c r="H24" s="5" t="s">
         <v>432</v>
       </c>
+      <c r="J24" t="s">
+        <v>603</v>
+      </c>
       <c r="K24">
         <v>8</v>
       </c>
@@ -3466,7 +3546,7 @@
       </c>
       <c r="R24" t="str">
         <f t="shared" si="0"/>
-        <v>("Commonsense Schooling",NULL,"Wilkinson, Roy","The Robinswook Press",NULL,"1990",NULL,"186981081",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Commonsense Schooling",NULL,"Wilkinson, Roy","The Robinswook Press",NULL,"1990",NULL,"186981081",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
@@ -3485,6 +3565,9 @@
       <c r="H25" t="s">
         <v>433</v>
       </c>
+      <c r="J25" t="s">
+        <v>603</v>
+      </c>
       <c r="K25">
         <v>4</v>
       </c>
@@ -3493,7 +3576,7 @@
       </c>
       <c r="R25" t="str">
         <f t="shared" si="0"/>
-        <v>("Grading the Teacher",NULL,"Jacobs, Nellie","Penguin Books",NULL,"1996",NULL,"0140256121",NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Grading the Teacher",NULL,"Jacobs, Nellie","Penguin Books",NULL,"1996",NULL,"0140256121",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
@@ -3512,6 +3595,9 @@
       <c r="H26" t="s">
         <v>434</v>
       </c>
+      <c r="J26" t="s">
+        <v>603</v>
+      </c>
       <c r="K26">
         <v>6</v>
       </c>
@@ -3520,7 +3606,7 @@
       </c>
       <c r="R26" t="str">
         <f t="shared" si="0"/>
-        <v>("On the Threshold of Adolsescence",NULL,"Koepke, Hermann","Anthroposophic Press",NULL,"1992",NULL,"0880103574",NULL,NULL,"6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("On the Threshold of Adolsescence",NULL,"Koepke, Hermann","Anthroposophic Press",NULL,"1992",NULL,"0880103574",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
@@ -3542,6 +3628,9 @@
       <c r="H27" t="s">
         <v>435</v>
       </c>
+      <c r="J27" t="s">
+        <v>603</v>
+      </c>
       <c r="K27">
         <v>1</v>
       </c>
@@ -3550,7 +3639,7 @@
       </c>
       <c r="R27" t="str">
         <f t="shared" si="0"/>
-        <v>("Thirteen to Nineteen - Discovering the Light ",NULL,"Sleigh, Julian","Floris Books","2","1989",NULL,"0863150780",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Thirteen to Nineteen - Discovering the Light ",NULL,"Sleigh, Julian","Floris Books","2","1989",NULL,"0863150780",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
@@ -3569,6 +3658,9 @@
       <c r="H28" t="s">
         <v>436</v>
       </c>
+      <c r="J28" t="s">
+        <v>603</v>
+      </c>
       <c r="K28">
         <v>9</v>
       </c>
@@ -3577,7 +3669,7 @@
       </c>
       <c r="R28" t="str">
         <f t="shared" si="0"/>
-        <v>("Closing the Gap - A Strategy for Bringing Parents and Teens Together",NULL,"McGraw, Jay","Fireside",NULL,"2001",NULL,"0743224698",NULL,NULL,"9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("Closing the Gap - A Strategy for Bringing Parents and Teens Together",NULL,"McGraw, Jay","Fireside",NULL,"2001",NULL,"0743224698",NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -3599,6 +3691,9 @@
       <c r="H29" t="s">
         <v>437</v>
       </c>
+      <c r="J29" t="s">
+        <v>603</v>
+      </c>
       <c r="K29">
         <v>1</v>
       </c>
@@ -3607,7 +3702,7 @@
       </c>
       <c r="R29" t="str">
         <f t="shared" si="0"/>
-        <v>("Voyage Through Childhood Into the Adult World",NULL,"Frommer, Eva A.","Hawthorn Press","2","1994",NULL,"1869890590",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Voyage Through Childhood Into the Adult World",NULL,"Frommer, Eva A.","Hawthorn Press","2","1994",NULL,"1869890590",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -3626,6 +3721,9 @@
       <c r="H30" t="s">
         <v>438</v>
       </c>
+      <c r="J30" t="s">
+        <v>603</v>
+      </c>
       <c r="K30">
         <v>1</v>
       </c>
@@ -3634,7 +3732,7 @@
       </c>
       <c r="R30" t="str">
         <f t="shared" si="0"/>
-        <v>("More Lifeways - Finding Support and Inspiration I Family Life",NULL,"Smith, Patti / Eklund Schaefer, Signe","Hawthorn Press",NULL,"1997",NULL,"1869890868",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("More Lifeways - Finding Support and Inspiration I Family Life",NULL,"Smith, Patti / Eklund Schaefer, Signe","Hawthorn Press",NULL,"1997",NULL,"1869890868",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -3653,6 +3751,9 @@
       <c r="H31" t="s">
         <v>439</v>
       </c>
+      <c r="J31" t="s">
+        <v>603</v>
+      </c>
       <c r="K31">
         <v>8</v>
       </c>
@@ -3661,7 +3762,7 @@
       </c>
       <c r="R31" t="str">
         <f t="shared" si="0"/>
-        <v>("The Motherly and Fatherly Roles in Education ",NULL,"Gabert, Erich","Anthroposophic Press",NULL,"1988",NULL,"0880101997",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("The Motherly and Fatherly Roles in Education ",NULL,"Gabert, Erich","Anthroposophic Press",NULL,"1988",NULL,"0880101997",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
@@ -3680,6 +3781,9 @@
       <c r="H32" t="s">
         <v>440</v>
       </c>
+      <c r="J32" t="s">
+        <v>603</v>
+      </c>
       <c r="K32">
         <v>8</v>
       </c>
@@ -3688,7 +3792,7 @@
       </c>
       <c r="R32" t="str">
         <f t="shared" si="0"/>
-        <v>("Raising a Daughter",NULL,"Elium, Jeanne and Don","Celestial Arts",NULL,"1994",NULL,"0890877084",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Raising a Daughter",NULL,"Elium, Jeanne and Don","Celestial Arts",NULL,"1994",NULL,"0890877084",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
@@ -3707,6 +3811,9 @@
       <c r="I33" t="s">
         <v>441</v>
       </c>
+      <c r="J33" t="s">
+        <v>603</v>
+      </c>
       <c r="K33">
         <v>2</v>
       </c>
@@ -3715,7 +3822,7 @@
       </c>
       <c r="R33" t="str">
         <f t="shared" si="0"/>
-        <v>("Adventures in Parenting",NULL,"Ross, Rachel C.","The Association of Waldorf Schools of North America (AWSNA)",NULL,"2008",NULL,NULL,"9781888364764",NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Adventures in Parenting",NULL,"Ross, Rachel C.","The Association of Waldorf Schools of North America (AWSNA)",NULL,"2008",NULL,NULL,"9781888364764","PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
@@ -3734,6 +3841,9 @@
       <c r="H34" t="s">
         <v>442</v>
       </c>
+      <c r="J34" t="s">
+        <v>603</v>
+      </c>
       <c r="K34">
         <v>10</v>
       </c>
@@ -3742,7 +3852,7 @@
       </c>
       <c r="R34" t="str">
         <f t="shared" si="0"/>
-        <v>("Spiritual Parenting - A Loving Guide for the New Age Parent",NULL,"Carroll, David","Paragon House, New York",NULL,"1990",NULL,"1557781125",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Spiritual Parenting - A Loving Guide for the New Age Parent",NULL,"Carroll, David","Paragon House, New York",NULL,"1990",NULL,"1557781125",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
@@ -3761,6 +3871,9 @@
       <c r="H35" s="5" t="s">
         <v>443</v>
       </c>
+      <c r="J35" t="s">
+        <v>603</v>
+      </c>
       <c r="K35">
         <v>1</v>
       </c>
@@ -3769,7 +3882,7 @@
       </c>
       <c r="R35" t="str">
         <f t="shared" si="0"/>
-        <v>("Reading Magic",NULL,"Fox, Mem","Harcourt, Inc.",NULL,"2001",NULL,"015601763",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Reading Magic",NULL,"Fox, Mem","Harcourt, Inc.",NULL,"2001",NULL,"015601763",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
@@ -3788,6 +3901,9 @@
       <c r="H36" t="s">
         <v>444</v>
       </c>
+      <c r="J36" t="s">
+        <v>603</v>
+      </c>
       <c r="K36">
         <v>10</v>
       </c>
@@ -3796,7 +3912,7 @@
       </c>
       <c r="R36" t="str">
         <f t="shared" si="0"/>
-        <v>("Raising a Creative Child",NULL,"MacGregor, Cynthia","Carol Publishing Group",NULL,"1996",NULL,"0806517417",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Raising a Creative Child",NULL,"MacGregor, Cynthia","Carol Publishing Group",NULL,"1996",NULL,"0806517417",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
@@ -3815,6 +3931,9 @@
       <c r="H37" s="5" t="s">
         <v>445</v>
       </c>
+      <c r="J37" t="s">
+        <v>603</v>
+      </c>
       <c r="K37">
         <v>7</v>
       </c>
@@ -3823,7 +3942,7 @@
       </c>
       <c r="R37" t="str">
         <f t="shared" si="0"/>
-        <v>("Parenting for a Healthy Future",NULL,"Coplen, Dotty","Hawthorn Press",NULL,"1995",NULL,"186989531",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Parenting for a Healthy Future",NULL,"Coplen, Dotty","Hawthorn Press",NULL,"1995",NULL,"186989531",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
@@ -3842,6 +3961,9 @@
       <c r="H38" t="s">
         <v>446</v>
       </c>
+      <c r="J38" t="s">
+        <v>603</v>
+      </c>
       <c r="K38">
         <v>8</v>
       </c>
@@ -3850,7 +3972,7 @@
       </c>
       <c r="R38" t="str">
         <f t="shared" si="0"/>
-        <v>("How to Talk to Kids will Listen and Listen so Kids Will Talk",NULL,"Faber, Adele / Mazlish, Elaine","Avon Books",NULL,"1980",NULL,"0380570009",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("How to Talk to Kids will Listen and Listen so Kids Will Talk",NULL,"Faber, Adele / Mazlish, Elaine","Avon Books",NULL,"1980",NULL,"0380570009",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
@@ -3869,6 +3991,9 @@
       <c r="H39" t="s">
         <v>447</v>
       </c>
+      <c r="J39" t="s">
+        <v>603</v>
+      </c>
       <c r="K39">
         <v>8</v>
       </c>
@@ -3877,7 +4002,7 @@
       </c>
       <c r="R39" t="str">
         <f t="shared" si="0"/>
-        <v>("School's Out",NULL,"Nikiforuk, Andrew","Macfarlane Walter and Ross, Toronto",NULL,"1993",NULL,"0921912838",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("School's Out",NULL,"Nikiforuk, Andrew","Macfarlane Walter and Ross, Toronto",NULL,"1993",NULL,"0921912838",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
@@ -3896,6 +4021,9 @@
       <c r="H40" t="s">
         <v>448</v>
       </c>
+      <c r="J40" t="s">
+        <v>603</v>
+      </c>
       <c r="K40">
         <v>2</v>
       </c>
@@ -3904,7 +4032,7 @@
       </c>
       <c r="R40" t="str">
         <f t="shared" si="0"/>
-        <v>("Children's Symptoms",NULL,"Valman, Bernard / Youger-Lewis Catherine","Reader's Digest Association (Canada) Ltd. Montreal",NULL,"1998",NULL,"0888506120",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Children's Symptoms",NULL,"Valman, Bernard / Youger-Lewis Catherine","Reader's Digest Association (Canada) Ltd. Montreal",NULL,"1998",NULL,"0888506120",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
@@ -3923,6 +4051,9 @@
       <c r="H41" t="s">
         <v>449</v>
       </c>
+      <c r="J41" t="s">
+        <v>603</v>
+      </c>
       <c r="K41">
         <v>10</v>
       </c>
@@ -3931,7 +4062,7 @@
       </c>
       <c r="R41" t="str">
         <f t="shared" si="0"/>
-        <v>("Families Apart - Ten Keys to Successful Co-Parenting",NULL,"Blau, Melinda","The Berkely Publishing Group",NULL,"1995",NULL,"039952150X",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Families Apart - Ten Keys to Successful Co-Parenting",NULL,"Blau, Melinda","The Berkely Publishing Group",NULL,"1995",NULL,"039952150X",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
@@ -3950,6 +4081,9 @@
       <c r="H42" t="s">
         <v>450</v>
       </c>
+      <c r="J42" t="s">
+        <v>603</v>
+      </c>
       <c r="K42">
         <v>10</v>
       </c>
@@ -3958,7 +4092,7 @@
       </c>
       <c r="R42" t="str">
         <f t="shared" si="0"/>
-        <v>("The Complete Kid's Allergy and Asthma Guide",NULL,"Gold, Milton","Robert Rose Inc.",NULL,"2003",NULL,"0778800784",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("The Complete Kid's Allergy and Asthma Guide",NULL,"Gold, Milton","Robert Rose Inc.",NULL,"2003",NULL,"0778800784",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
@@ -3977,6 +4111,9 @@
       <c r="H43" t="s">
         <v>451</v>
       </c>
+      <c r="J43" t="s">
+        <v>603</v>
+      </c>
       <c r="K43">
         <v>5</v>
       </c>
@@ -3985,7 +4122,7 @@
       </c>
       <c r="R43" t="str">
         <f t="shared" si="0"/>
-        <v>("Sharing Nature with Children",NULL,"Cornell, Joseph","Dawn Publications",NULL,"1979",NULL,"0916124142",NULL,NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Sharing Nature with Children",NULL,"Cornell, Joseph","Dawn Publications",NULL,"1979",NULL,"0916124142",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
@@ -4004,6 +4141,9 @@
       <c r="H44" t="s">
         <v>452</v>
       </c>
+      <c r="J44" t="s">
+        <v>603</v>
+      </c>
       <c r="K44">
         <v>2</v>
       </c>
@@ -4012,7 +4152,7 @@
       </c>
       <c r="R44" t="str">
         <f t="shared" si="0"/>
-        <v>("How Childern Play",NULL,"Haller, Ingeborg","Floris Books",NULL,"1991",NULL,"0863151272",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("How Childern Play",NULL,"Haller, Ingeborg","Floris Books",NULL,"1991",NULL,"0863151272",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
@@ -4031,6 +4171,9 @@
       <c r="H45" t="s">
         <v>453</v>
       </c>
+      <c r="J45" t="s">
+        <v>603</v>
+      </c>
       <c r="K45">
         <v>2</v>
       </c>
@@ -4039,7 +4182,7 @@
       </c>
       <c r="R45" t="str">
         <f t="shared" si="0"/>
-        <v>("Remember the Light",NULL,"Fisher, Mary Pat","Fenton Valley Press",NULL,"1986",NULL,"0961514973",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Remember the Light",NULL,"Fisher, Mary Pat","Fenton Valley Press",NULL,"1986",NULL,"0961514973",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
@@ -4058,6 +4201,9 @@
       <c r="H46" t="s">
         <v>454</v>
       </c>
+      <c r="J46" t="s">
+        <v>603</v>
+      </c>
       <c r="K46">
         <v>5</v>
       </c>
@@ -4066,7 +4212,7 @@
       </c>
       <c r="R46" t="str">
         <f t="shared" si="0"/>
-        <v>("Making Soft Toys",NULL,"Jaffke, Freya","Celestial Arts",NULL,"1981",NULL,"0897420446",NULL,NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Making Soft Toys",NULL,"Jaffke, Freya","Celestial Arts",NULL,"1981",NULL,"0897420446",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
@@ -4088,6 +4234,9 @@
       <c r="H47" s="5" t="s">
         <v>455</v>
       </c>
+      <c r="J47" t="s">
+        <v>603</v>
+      </c>
       <c r="K47">
         <v>4</v>
       </c>
@@ -4096,7 +4245,7 @@
       </c>
       <c r="R47" t="str">
         <f t="shared" si="0"/>
-        <v>("Summer",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"094626023",NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Summer",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"094626023",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
@@ -4115,6 +4264,9 @@
       <c r="H48" s="5" t="s">
         <v>456</v>
       </c>
+      <c r="J48" t="s">
+        <v>603</v>
+      </c>
       <c r="K48">
         <v>4</v>
       </c>
@@ -4123,7 +4275,7 @@
       </c>
       <c r="R48" t="str">
         <f t="shared" si="0"/>
-        <v>("Conception Birth and Early Childhood",NULL,"Glas, Norbert","Anthroposophic Press",NULL,"1983",NULL,"091142548",NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Conception Birth and Early Childhood",NULL,"Glas, Norbert","Anthroposophic Press",NULL,"1983",NULL,"091142548",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
@@ -4142,6 +4294,9 @@
       <c r="H49" t="s">
         <v>457</v>
       </c>
+      <c r="J49" t="s">
+        <v>603</v>
+      </c>
       <c r="K49">
         <v>5</v>
       </c>
@@ -4150,7 +4305,7 @@
       </c>
       <c r="R49" t="str">
         <f t="shared" si="0"/>
-        <v>("Children at Play",NULL,"Britz-Crecelius, Heidi","Parkstreet Press, Rochester, Vermont",NULL,"1996",NULL,"0892816295",NULL,NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Children at Play",NULL,"Britz-Crecelius, Heidi","Parkstreet Press, Rochester, Vermont",NULL,"1996",NULL,"0892816295",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
@@ -4169,6 +4324,9 @@
       <c r="H50" t="s">
         <v>458</v>
       </c>
+      <c r="J50" t="s">
+        <v>603</v>
+      </c>
       <c r="K50">
         <v>4</v>
       </c>
@@ -4177,7 +4335,7 @@
       </c>
       <c r="R50" t="str">
         <f t="shared" si="0"/>
-        <v>("50 Simple Things Kids Can Do to Save The Earth",NULL,"Javna, John","Andrews and McMeel",NULL,"1990",NULL,"0836223012",NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("50 Simple Things Kids Can Do to Save The Earth",NULL,"Javna, John","Andrews and McMeel",NULL,"1990",NULL,"0836223012",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
@@ -4196,6 +4354,9 @@
       <c r="H51" t="s">
         <v>459</v>
       </c>
+      <c r="J51" t="s">
+        <v>603</v>
+      </c>
       <c r="K51">
         <v>7</v>
       </c>
@@ -4204,7 +4365,7 @@
       </c>
       <c r="R51" t="str">
         <f t="shared" si="0"/>
-        <v>("Sewing for Baby",NULL,"Martensson, Kerstin","?",NULL,"1987",NULL,"0913212105",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Sewing for Baby",NULL,"Martensson, Kerstin","?",NULL,"1987",NULL,"0913212105",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
@@ -4223,6 +4384,9 @@
       <c r="H52" t="s">
         <v>460</v>
       </c>
+      <c r="J52" t="s">
+        <v>603</v>
+      </c>
       <c r="K52">
         <v>9</v>
       </c>
@@ -4231,7 +4395,7 @@
       </c>
       <c r="R52" t="str">
         <f t="shared" si="0"/>
-        <v>("Advent for Children",NULL,"Jaffke, Freya","Floris Books",NULL,"1979",NULL,"0863150098",NULL,NULL,"9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("Advent for Children",NULL,"Jaffke, Freya","Floris Books",NULL,"1979",NULL,"0863150098",NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
@@ -4250,6 +4414,9 @@
       <c r="H53" t="s">
         <v>461</v>
       </c>
+      <c r="J53" t="s">
+        <v>603</v>
+      </c>
       <c r="K53">
         <v>6</v>
       </c>
@@ -4258,7 +4425,7 @@
       </c>
       <c r="R53" t="str">
         <f t="shared" si="0"/>
-        <v>("Making Dolls",NULL,"Reinckens, Sunnhild","Floris Books",NULL,"1989",NULL,"0863150934",NULL,NULL,"6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Making Dolls",NULL,"Reinckens, Sunnhild","Floris Books",NULL,"1989",NULL,"0863150934",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
@@ -4277,6 +4444,9 @@
       <c r="H54" t="s">
         <v>462</v>
       </c>
+      <c r="J54" t="s">
+        <v>603</v>
+      </c>
       <c r="K54">
         <v>2</v>
       </c>
@@ -4285,7 +4455,7 @@
       </c>
       <c r="R54" t="str">
         <f t="shared" si="0"/>
-        <v>("The Nature Corner",NULL,"v Leeuwen, M / Moeskops, J","Floris Books",NULL,"1990",NULL,"0863151116",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("The Nature Corner",NULL,"v Leeuwen, M / Moeskops, J","Floris Books",NULL,"1990",NULL,"0863151116",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
@@ -4304,6 +4474,9 @@
       <c r="H55" t="s">
         <v>463</v>
       </c>
+      <c r="J55" t="s">
+        <v>603</v>
+      </c>
       <c r="K55">
         <v>3</v>
       </c>
@@ -4312,7 +4485,7 @@
       </c>
       <c r="R55" t="str">
         <f t="shared" si="0"/>
-        <v>("The Christmas Craft Book",NULL,"Berger, Thomas","Floris Books",NULL,"2001",NULL,"0863151108",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("The Christmas Craft Book",NULL,"Berger, Thomas","Floris Books",NULL,"2001",NULL,"0863151108",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
@@ -4331,6 +4504,9 @@
       <c r="H56" t="s">
         <v>464</v>
       </c>
+      <c r="J56" t="s">
+        <v>603</v>
+      </c>
       <c r="K56">
         <v>9</v>
       </c>
@@ -4339,7 +4515,7 @@
       </c>
       <c r="R56" t="str">
         <f t="shared" si="0"/>
-        <v>("The Harvest Craft Book",NULL,"Berger, Thomas","Floris Books",NULL,"1993",NULL,"0863151477",NULL,NULL,"9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("The Harvest Craft Book",NULL,"Berger, Thomas","Floris Books",NULL,"1993",NULL,"0863151477",NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
@@ -4358,6 +4534,9 @@
       <c r="H57" t="s">
         <v>465</v>
       </c>
+      <c r="J57" t="s">
+        <v>603</v>
+      </c>
       <c r="K57">
         <v>1</v>
       </c>
@@ -4366,7 +4545,7 @@
       </c>
       <c r="R57" t="str">
         <f t="shared" si="0"/>
-        <v>("The Easter Craft Book",NULL,"Berger, Thomas and Petra","Floris Books",NULL,"1994",NULL,"0863151612",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("The Easter Craft Book",NULL,"Berger, Thomas and Petra","Floris Books",NULL,"1994",NULL,"0863151612",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
@@ -4385,6 +4564,9 @@
       <c r="H58" t="s">
         <v>466</v>
       </c>
+      <c r="J58" t="s">
+        <v>603</v>
+      </c>
       <c r="K58">
         <v>6</v>
       </c>
@@ -4393,7 +4575,7 @@
       </c>
       <c r="R58" t="str">
         <f t="shared" si="0"/>
-        <v>("The Gnome Graft Book",NULL,"Berger, Thomas and Petra","Floris Books",NULL,"2001",NULL,"0863153003",NULL,NULL,"6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("The Gnome Graft Book",NULL,"Berger, Thomas and Petra","Floris Books",NULL,"2001",NULL,"0863153003",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
@@ -4415,6 +4597,9 @@
       <c r="H59" t="s">
         <v>467</v>
       </c>
+      <c r="J59" t="s">
+        <v>603</v>
+      </c>
       <c r="K59">
         <v>1</v>
       </c>
@@ -4423,7 +4608,7 @@
       </c>
       <c r="R59" t="str">
         <f t="shared" si="0"/>
-        <v>("Festivals with Children",NULL,"Barz, Brigitte","Floris Books","2","1991",NULL,"0863150551",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Festivals with Children",NULL,"Barz, Brigitte","Floris Books","2","1991",NULL,"0863150551",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
@@ -4445,6 +4630,9 @@
       <c r="H60" t="s">
         <v>468</v>
       </c>
+      <c r="J60" t="s">
+        <v>603</v>
+      </c>
       <c r="K60">
         <v>5</v>
       </c>
@@ -4453,7 +4641,7 @@
       </c>
       <c r="R60" t="str">
         <f t="shared" si="0"/>
-        <v>("Autumn",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"0946206031",NULL,NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Autumn",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"0946206031",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
@@ -4475,6 +4663,9 @@
       <c r="H61" s="5" t="s">
         <v>469</v>
       </c>
+      <c r="J61" t="s">
+        <v>603</v>
+      </c>
       <c r="K61">
         <v>8</v>
       </c>
@@ -4483,7 +4674,7 @@
       </c>
       <c r="R61" t="str">
         <f t="shared" si="0"/>
-        <v>("Gateways",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"094626058",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Gateways",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"094626058",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
@@ -4502,6 +4693,9 @@
       <c r="H62" t="s">
         <v>425</v>
       </c>
+      <c r="J62" t="s">
+        <v>603</v>
+      </c>
       <c r="K62">
         <v>9</v>
       </c>
@@ -4510,7 +4704,7 @@
       </c>
       <c r="R62" t="str">
         <f t="shared" si="0"/>
-        <v>("Stories They'll Remember",NULL,"Lord, Frank M.","Treehouse Communication Inc.",NULL,"1987",NULL,NULL,NULL,NULL,"9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("Stories They'll Remember",NULL,"Lord, Frank M.","Treehouse Communication Inc.",NULL,"1987",NULL,NULL,NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
@@ -4529,6 +4723,9 @@
       <c r="H63" t="s">
         <v>470</v>
       </c>
+      <c r="J63" t="s">
+        <v>603</v>
+      </c>
       <c r="K63">
         <v>5</v>
       </c>
@@ -4537,7 +4734,7 @@
       </c>
       <c r="R63" t="str">
         <f t="shared" si="0"/>
-        <v>("Natural Childhood",NULL,"Thomson, John","Fireside, Simon &amp; Schuster Inc.",NULL,"1994",NULL,"0020207395",NULL,NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Natural Childhood",NULL,"Thomson, John","Fireside, Simon &amp; Schuster Inc.",NULL,"1994",NULL,"0020207395",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
@@ -4556,6 +4753,9 @@
       <c r="H64" t="s">
         <v>471</v>
       </c>
+      <c r="J64" t="s">
+        <v>603</v>
+      </c>
       <c r="K64">
         <v>1</v>
       </c>
@@ -4564,7 +4764,7 @@
       </c>
       <c r="R64" t="str">
         <f t="shared" si="0"/>
-        <v>("Festivals Family and Food",NULL,"Carey, Diana / Large, Judy","Hawthorn Press",NULL,"1983",NULL,"095070623X",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Festivals Family and Food",NULL,"Carey, Diana / Large, Judy","Hawthorn Press",NULL,"1983",NULL,"095070623X",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.3">
@@ -4580,6 +4780,9 @@
       <c r="H65" t="s">
         <v>472</v>
       </c>
+      <c r="J65" t="s">
+        <v>603</v>
+      </c>
       <c r="K65">
         <v>1</v>
       </c>
@@ -4588,7 +4791,7 @@
       </c>
       <c r="R65" t="str">
         <f t="shared" si="0"/>
-        <v>("All Year Round",NULL,"Druitt, Ann / Fynes-Clinton, Christine / Rowling, Maije","Hawthorn Press",NULL,NULL,NULL,"1869890477",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("All Year Round",NULL,"Druitt, Ann / Fynes-Clinton, Christine / Rowling, Maije","Hawthorn Press",NULL,NULL,NULL,"1869890477",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.3">
@@ -4607,6 +4810,9 @@
       <c r="H66" t="s">
         <v>473</v>
       </c>
+      <c r="J66" t="s">
+        <v>603</v>
+      </c>
       <c r="K66">
         <v>3</v>
       </c>
@@ -4615,7 +4821,7 @@
       </c>
       <c r="R66" t="str">
         <f t="shared" si="0"/>
-        <v>("Days, Weeks and Months",NULL,"Joy, Margaret","Faber and Faber, London Boston",NULL,"1984",NULL,"0571131719",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Days, Weeks and Months",NULL,"Joy, Margaret","Faber and Faber, London Boston",NULL,"1984",NULL,"0571131719",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.3">
@@ -4633,6 +4839,9 @@
       </c>
       <c r="H67" t="s">
         <v>474</v>
+      </c>
+      <c r="J67" t="s">
+        <v>603</v>
       </c>
       <c r="K67">
         <v>7</v>
@@ -4658,7 +4867,7 @@
 IF(N67="","NULL",_xlfn.CONCAT("""",N67,"""")),",",
 IF(O67="","NULL",_xlfn.CONCAT("""",O67,"""")),",",
 IF(P67="","NULL",_xlfn.CONCAT("""",P67,"""")),"),")</f>
-        <v>("The Children's Year",NULL,"Cooper, Stephanie / Fynes-Clinton, Christine / Rowling, Marye","Hawthorn Press",NULL,"1986",NULL,"1869890000",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("The Children's Year",NULL,"Cooper, Stephanie / Fynes-Clinton, Christine / Rowling, Marye","Hawthorn Press",NULL,"1986",NULL,"1869890000",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.3">
@@ -4677,6 +4886,9 @@
       <c r="H68" t="s">
         <v>475</v>
       </c>
+      <c r="J68" t="s">
+        <v>603</v>
+      </c>
       <c r="K68">
         <v>6</v>
       </c>
@@ -4685,7 +4897,7 @@
       </c>
       <c r="R68" t="str">
         <f t="shared" si="1"/>
-        <v>("Understanding Waldorf Education ",NULL,"Petrash, Jack","Gryphon House Inc.",NULL,"2002",NULL,"0876592469",NULL,NULL,"6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Understanding Waldorf Education ",NULL,"Petrash, Jack","Gryphon House Inc.",NULL,"2002",NULL,"0876592469",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.3">
@@ -4704,6 +4916,9 @@
       <c r="H69" t="s">
         <v>476</v>
       </c>
+      <c r="J69" t="s">
+        <v>603</v>
+      </c>
       <c r="K69">
         <v>8</v>
       </c>
@@ -4712,7 +4927,7 @@
       </c>
       <c r="R69" t="str">
         <f t="shared" si="1"/>
-        <v>("Parent's Guide to the Best Books for Children",NULL,"Lipson, Eden Ross","Times Books",NULL,"1988",NULL,"0812917758",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Parent's Guide to the Best Books for Children",NULL,"Lipson, Eden Ross","Times Books",NULL,"1988",NULL,"0812917758",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.3">
@@ -4731,6 +4946,9 @@
       <c r="H70" t="s">
         <v>477</v>
       </c>
+      <c r="J70" t="s">
+        <v>603</v>
+      </c>
       <c r="K70">
         <v>10</v>
       </c>
@@ -4739,7 +4957,7 @@
       </c>
       <c r="R70" t="str">
         <f t="shared" si="1"/>
-        <v>("Waldorf Education - A Family Guide",NULL,"Johnson Fenner, Pamela / Rivers, Karen L.","Michealmas Press",NULL,"1992",NULL,"0964783215",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Waldorf Education - A Family Guide",NULL,"Johnson Fenner, Pamela / Rivers, Karen L.","Michealmas Press",NULL,"1992",NULL,"0964783215",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.3">
@@ -4758,6 +4976,9 @@
       <c r="H71" t="s">
         <v>425</v>
       </c>
+      <c r="J71" t="s">
+        <v>603</v>
+      </c>
       <c r="K71">
         <v>2</v>
       </c>
@@ -4766,7 +4987,7 @@
       </c>
       <c r="R71" t="str">
         <f t="shared" si="1"/>
-        <v>("Pentatonic Songs",NULL,"Lebret, Elisabeth","Waldorf Schools of Ontario",NULL,"1985",NULL,NULL,NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Pentatonic Songs",NULL,"Lebret, Elisabeth","Waldorf Schools of Ontario",NULL,"1985",NULL,NULL,NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.3">
@@ -4785,6 +5006,9 @@
       <c r="H72" t="s">
         <v>478</v>
       </c>
+      <c r="J72" t="s">
+        <v>603</v>
+      </c>
       <c r="K72">
         <v>8</v>
       </c>
@@ -4793,7 +5017,7 @@
       </c>
       <c r="R72" t="str">
         <f t="shared" si="1"/>
-        <v>("Painting with Children",NULL,"Muller, Brunhild","Floris Books",NULL,"1987",NULL,"0863150489",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Painting with Children",NULL,"Muller, Brunhild","Floris Books",NULL,"1987",NULL,"0863150489",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.3">
@@ -4812,6 +5036,9 @@
       <c r="H73" t="s">
         <v>425</v>
       </c>
+      <c r="J73" t="s">
+        <v>603</v>
+      </c>
       <c r="K73">
         <v>1</v>
       </c>
@@ -4820,7 +5047,7 @@
       </c>
       <c r="R73" t="str">
         <f t="shared" si="1"/>
-        <v>("Child and Man (Journal)",NULL,"Masters, Brian (Editor)","Imprint",NULL,"1995",NULL,NULL,NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Child and Man (Journal)",NULL,"Masters, Brian (Editor)","Imprint",NULL,"1995",NULL,NULL,NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.3">
@@ -4839,6 +5066,9 @@
       <c r="H74" t="s">
         <v>425</v>
       </c>
+      <c r="J74" t="s">
+        <v>603</v>
+      </c>
       <c r="K74">
         <v>4</v>
       </c>
@@ -4847,7 +5077,7 @@
       </c>
       <c r="R74" t="str">
         <f t="shared" si="1"/>
-        <v>("Rudolf Steiner Waldorf Education",NULL,"Steiner Schools","The Robinswook Press",NULL,"1989",NULL,NULL,NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Rudolf Steiner Waldorf Education",NULL,"Steiner Schools","The Robinswook Press",NULL,"1989",NULL,NULL,NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.3">
@@ -4866,6 +5096,9 @@
       <c r="H75" t="s">
         <v>479</v>
       </c>
+      <c r="J75" t="s">
+        <v>603</v>
+      </c>
       <c r="K75">
         <v>10</v>
       </c>
@@ -4874,7 +5107,7 @@
       </c>
       <c r="R75" t="str">
         <f t="shared" si="1"/>
-        <v>("Earth Child (Paperback)",NULL,"Sheehan, Kathryn / Waidner, Mary","Council Oak Books",NULL,"991",NULL,"0933031394",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Earth Child (Paperback)",NULL,"Sheehan, Kathryn / Waidner, Mary","Council Oak Books",NULL,"991",NULL,"0933031394",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.3">
@@ -4893,6 +5126,9 @@
       <c r="I76" t="s">
         <v>480</v>
       </c>
+      <c r="J76" t="s">
+        <v>603</v>
+      </c>
       <c r="K76">
         <v>5</v>
       </c>
@@ -4901,7 +5137,7 @@
       </c>
       <c r="R76" t="str">
         <f t="shared" si="1"/>
-        <v>("Earthways ",NULL,"Petrash, Carol","The Gryphon House Book",NULL,"1992",NULL,NULL,"9780876591567",NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Earthways ",NULL,"Petrash, Carol","The Gryphon House Book",NULL,"1992",NULL,NULL,"9780876591567","PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.3">
@@ -4920,6 +5156,9 @@
       <c r="H77" s="5" t="s">
         <v>481</v>
       </c>
+      <c r="J77" t="s">
+        <v>603</v>
+      </c>
       <c r="K77">
         <v>2</v>
       </c>
@@ -4928,7 +5167,7 @@
       </c>
       <c r="R77" t="str">
         <f t="shared" si="1"/>
-        <v>("Work and Play in Early Childhood",NULL,"Jaffke, Freya","Anthroposophic Press",NULL,"1991",NULL,"088014422",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Work and Play in Early Childhood",NULL,"Jaffke, Freya","Anthroposophic Press",NULL,"1991",NULL,"088014422",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.3">
@@ -4947,6 +5186,9 @@
       <c r="H78" t="s">
         <v>425</v>
       </c>
+      <c r="J78" t="s">
+        <v>603</v>
+      </c>
       <c r="K78">
         <v>3</v>
       </c>
@@ -4955,7 +5197,7 @@
       </c>
       <c r="R78" t="str">
         <f t="shared" si="1"/>
-        <v>("Adventuring with Children",NULL,"Jeffrey, Nan","Avalon House Printing",NULL,"1992",NULL,NULL,NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Adventuring with Children",NULL,"Jeffrey, Nan","Avalon House Printing",NULL,"1992",NULL,NULL,NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.3">
@@ -4974,6 +5216,9 @@
       <c r="H79" t="s">
         <v>482</v>
       </c>
+      <c r="J79" t="s">
+        <v>603</v>
+      </c>
       <c r="K79">
         <v>9</v>
       </c>
@@ -4982,7 +5227,7 @@
       </c>
       <c r="R79" t="str">
         <f t="shared" si="1"/>
-        <v>("Becoming the Parent You Want to Be",NULL,"Davis, Laura / Keyser, Janis","Broadway Books, NY",NULL,"1997",NULL,"0553067508",NULL,NULL,"9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("Becoming the Parent You Want to Be",NULL,"Davis, Laura / Keyser, Janis","Broadway Books, NY",NULL,"1997",NULL,"0553067508",NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.3">
@@ -5001,6 +5246,9 @@
       <c r="H80" t="s">
         <v>483</v>
       </c>
+      <c r="J80" t="s">
+        <v>603</v>
+      </c>
       <c r="K80">
         <v>7</v>
       </c>
@@ -5009,7 +5257,7 @@
       </c>
       <c r="R80" t="str">
         <f t="shared" si="1"/>
-        <v>("Vegetarian Baby and Child",NULL,"Jackson, Petra","Crescent Books, NY",NULL,"1995",NULL,"0517121522",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Vegetarian Baby and Child",NULL,"Jackson, Petra","Crescent Books, NY",NULL,"1995",NULL,"0517121522",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.3">
@@ -5028,6 +5276,9 @@
       <c r="H81" t="s">
         <v>484</v>
       </c>
+      <c r="J81" t="s">
+        <v>603</v>
+      </c>
       <c r="K81">
         <v>4</v>
       </c>
@@ -5036,7 +5287,7 @@
       </c>
       <c r="R81" t="str">
         <f t="shared" si="1"/>
-        <v>("Your Self-Confident Baby",NULL,"Gerber, Magda","John Wiley &amp; Sons, Inc.",NULL,"1998",NULL,"0471178837",NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Your Self-Confident Baby",NULL,"Gerber, Magda","John Wiley &amp; Sons, Inc.",NULL,"1998",NULL,"0471178837",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.3">
@@ -5055,6 +5306,9 @@
       <c r="H82" t="s">
         <v>485</v>
       </c>
+      <c r="J82" t="s">
+        <v>603</v>
+      </c>
       <c r="K82">
         <v>7</v>
       </c>
@@ -5063,7 +5317,7 @@
       </c>
       <c r="R82" t="str">
         <f t="shared" si="1"/>
-        <v>("Mitten Strings of God",NULL,"Kenison, Katrina","Warner Books",NULL,"2000",NULL,"044+525316",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Mitten Strings of God",NULL,"Kenison, Katrina","Warner Books",NULL,"2000",NULL,"044+525316",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.3">
@@ -5082,6 +5336,9 @@
       <c r="H83" t="s">
         <v>486</v>
       </c>
+      <c r="J83" t="s">
+        <v>603</v>
+      </c>
       <c r="K83">
         <v>7</v>
       </c>
@@ -5090,7 +5347,7 @@
       </c>
       <c r="R83" t="str">
         <f t="shared" si="1"/>
-        <v>("Loving Hands - The Traditional Art of Baby Massage",NULL,"Leboyer, Frederick","Newmarket Press",NULL,"1997",NULL,"1557043140",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Loving Hands - The Traditional Art of Baby Massage",NULL,"Leboyer, Frederick","Newmarket Press",NULL,"1997",NULL,"1557043140",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.3">
@@ -5109,6 +5366,9 @@
       <c r="H84" t="s">
         <v>487</v>
       </c>
+      <c r="J84" t="s">
+        <v>603</v>
+      </c>
       <c r="K84">
         <v>10</v>
       </c>
@@ -5117,7 +5377,7 @@
       </c>
       <c r="R84" t="str">
         <f t="shared" si="1"/>
-        <v>("Keeping Childhood",NULL,"Aldrich, Nancy","Childhood Press",NULL,"1989",NULL,"0962358304",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Keeping Childhood",NULL,"Aldrich, Nancy","Childhood Press",NULL,"1989",NULL,"0962358304",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.3">
@@ -5136,6 +5396,9 @@
       <c r="H85" t="s">
         <v>488</v>
       </c>
+      <c r="J85" t="s">
+        <v>603</v>
+      </c>
       <c r="K85">
         <v>3</v>
       </c>
@@ -5144,7 +5407,7 @@
       </c>
       <c r="R85" t="str">
         <f t="shared" si="1"/>
-        <v>("You Are Your Child's First Teacher",NULL,"Baldwin Dancy, Rahima","Celestial Arts",NULL,"1989",NULL,"0890875197",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("You Are Your Child's First Teacher",NULL,"Baldwin Dancy, Rahima","Celestial Arts",NULL,"1989",NULL,"0890875197",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.3">
@@ -5163,6 +5426,9 @@
       <c r="H86" t="s">
         <v>489</v>
       </c>
+      <c r="J86" t="s">
+        <v>603</v>
+      </c>
       <c r="K86">
         <v>8</v>
       </c>
@@ -5171,7 +5437,7 @@
       </c>
       <c r="R86" t="str">
         <f t="shared" si="1"/>
-        <v>("Learning All the Time",NULL,"Holt, John","Addison-Wesley Publishing Company, Inc.",NULL,"1989",NULL,"020112095X",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Learning All the Time",NULL,"Holt, John","Addison-Wesley Publishing Company, Inc.",NULL,"1989",NULL,"020112095X",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.3">
@@ -5190,6 +5456,9 @@
       <c r="H87" t="s">
         <v>490</v>
       </c>
+      <c r="J87" t="s">
+        <v>603</v>
+      </c>
       <c r="K87">
         <v>2</v>
       </c>
@@ -5198,7 +5467,7 @@
       </c>
       <c r="R87" t="str">
         <f t="shared" si="1"/>
-        <v>("Our Last Best Shot",NULL,"Sessions Stepp, Laura","Riverhead Books, NY",NULL,"2000",NULL,"1573228753",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Our Last Best Shot",NULL,"Sessions Stepp, Laura","Riverhead Books, NY",NULL,"2000",NULL,"1573228753",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.3">
@@ -5217,6 +5486,9 @@
       <c r="H88" t="s">
         <v>491</v>
       </c>
+      <c r="J88" t="s">
+        <v>603</v>
+      </c>
       <c r="K88">
         <v>7</v>
       </c>
@@ -5225,7 +5497,7 @@
       </c>
       <c r="R88" t="str">
         <f t="shared" si="1"/>
-        <v>("The Hurried Child ",NULL,"Elkind, David","Addison-Wesley Publishing Company, Inc.",NULL,"1981",NULL,"0201039672",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("The Hurried Child ",NULL,"Elkind, David","Addison-Wesley Publishing Company, Inc.",NULL,"1981",NULL,"0201039672",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.3">
@@ -5244,6 +5516,9 @@
       <c r="H89" t="s">
         <v>492</v>
       </c>
+      <c r="J89" t="s">
+        <v>603</v>
+      </c>
       <c r="K89">
         <v>2</v>
       </c>
@@ -5252,7 +5527,7 @@
       </c>
       <c r="R89" t="str">
         <f t="shared" si="1"/>
-        <v>("Reading Is More than Phonics",NULL,"Goodman, Vera","Reading Wings",NULL,"1999",NULL,"096999382X",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Reading Is More than Phonics",NULL,"Goodman, Vera","Reading Wings",NULL,"1999",NULL,"096999382X",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.3">
@@ -5271,6 +5546,9 @@
       <c r="H90" t="s">
         <v>493</v>
       </c>
+      <c r="J90" t="s">
+        <v>603</v>
+      </c>
       <c r="K90">
         <v>1</v>
       </c>
@@ -5279,7 +5557,7 @@
       </c>
       <c r="R90" t="str">
         <f t="shared" si="1"/>
-        <v>("Raising a Family - Living on Planet Parenthood",NULL,"Elium, Jeanne and Don","Celestial Arts",NULL,"1997",NULL,"0890878188",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Raising a Family - Living on Planet Parenthood",NULL,"Elium, Jeanne and Don","Celestial Arts",NULL,"1997",NULL,"0890878188",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.3">
@@ -5298,6 +5576,9 @@
       <c r="H91" s="5" t="s">
         <v>494</v>
       </c>
+      <c r="J91" t="s">
+        <v>603</v>
+      </c>
       <c r="K91">
         <v>4</v>
       </c>
@@ -5306,7 +5587,7 @@
       </c>
       <c r="R91" t="str">
         <f t="shared" si="1"/>
-        <v>("Wakdorf Education for Adolescence",NULL,"Steiner, Rudolf","Kolisko Archive Publications",NULL,"1980",NULL,"096492378",NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Wakdorf Education for Adolescence",NULL,"Steiner, Rudolf","Kolisko Archive Publications",NULL,"1980",NULL,"096492378",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.3">
@@ -5325,6 +5606,9 @@
       <c r="H92" t="s">
         <v>495</v>
       </c>
+      <c r="J92" t="s">
+        <v>603</v>
+      </c>
       <c r="K92">
         <v>10</v>
       </c>
@@ -5333,7 +5617,7 @@
       </c>
       <c r="R92" t="str">
         <f t="shared" si="1"/>
-        <v>("Life Strategies for Teens",NULL,"McGraw, Jay","Fireside",NULL,"2000",NULL,"074321546X",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Life Strategies for Teens",NULL,"McGraw, Jay","Fireside",NULL,"2000",NULL,"074321546X",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.3">
@@ -5352,6 +5636,9 @@
       <c r="H93" t="s">
         <v>496</v>
       </c>
+      <c r="J93" t="s">
+        <v>603</v>
+      </c>
       <c r="K93">
         <v>5</v>
       </c>
@@ -5360,7 +5647,7 @@
       </c>
       <c r="R93" t="str">
         <f t="shared" si="1"/>
-        <v>("Summer Children - Ready or Not For School",NULL,"Uphoff, James K","J&amp;J Publishing Co.",NULL,"1986",NULL,"0961856106",NULL,NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Summer Children - Ready or Not For School",NULL,"Uphoff, James K","J&amp;J Publishing Co.",NULL,"1986",NULL,"0961856106",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.3">
@@ -5379,6 +5666,9 @@
       <c r="H94" t="s">
         <v>497</v>
       </c>
+      <c r="J94" t="s">
+        <v>603</v>
+      </c>
       <c r="K94">
         <v>4</v>
       </c>
@@ -5387,7 +5677,7 @@
       </c>
       <c r="R94" t="str">
         <f t="shared" si="1"/>
-        <v>("An Education for the 21st Century - Essays on Waldorf Education ",NULL,"Maher, Stanford","Novalis Press",NULL,"1995",NULL,"0958388512",NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("An Education for the 21st Century - Essays on Waldorf Education ",NULL,"Maher, Stanford","Novalis Press",NULL,"1995",NULL,"0958388512",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.3">
@@ -5406,6 +5696,9 @@
       <c r="H95" t="s">
         <v>498</v>
       </c>
+      <c r="J95" t="s">
+        <v>603</v>
+      </c>
       <c r="K95">
         <v>3</v>
       </c>
@@ -5414,7 +5707,7 @@
       </c>
       <c r="R95" t="str">
         <f t="shared" si="1"/>
-        <v>("Exrtaordinary Minds",NULL,"Gardner, Howard","Basic Books",NULL,"1997",NULL,"0465021255",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Exrtaordinary Minds",NULL,"Gardner, Howard","Basic Books",NULL,"1997",NULL,"0465021255",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.3">
@@ -5433,6 +5726,9 @@
       <c r="H96" t="s">
         <v>499</v>
       </c>
+      <c r="J96" t="s">
+        <v>603</v>
+      </c>
       <c r="K96">
         <v>4</v>
       </c>
@@ -5441,7 +5737,7 @@
       </c>
       <c r="R96" t="str">
         <f t="shared" si="1"/>
-        <v>("Multiple Intelligences",NULL,"Gardner, Howard","Basic Books",NULL,"1993",NULL,"046501822X",NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Multiple Intelligences",NULL,"Gardner, Howard","Basic Books",NULL,"1993",NULL,"046501822X",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.3">
@@ -5460,6 +5756,9 @@
       <c r="H97" t="s">
         <v>500</v>
       </c>
+      <c r="J97" t="s">
+        <v>603</v>
+      </c>
       <c r="K97">
         <v>3</v>
       </c>
@@ -5468,7 +5767,7 @@
       </c>
       <c r="R97" t="str">
         <f t="shared" si="1"/>
-        <v>("Frames of Mind",NULL,"Gardner, Howard","Basic Books",NULL,"1983",NULL,"0465025099",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Frames of Mind",NULL,"Gardner, Howard","Basic Books",NULL,"1983",NULL,"0465025099",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.3">
@@ -5487,6 +5786,9 @@
       <c r="H98" t="s">
         <v>501</v>
       </c>
+      <c r="J98" t="s">
+        <v>603</v>
+      </c>
       <c r="K98">
         <v>2</v>
       </c>
@@ -5495,7 +5797,7 @@
       </c>
       <c r="R98" t="str">
         <f t="shared" si="1"/>
-        <v>("Turning",NULL,"Anthroposiphic Press","Anthroposophic Press",NULL,"1994",NULL,"0880103841",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Turning",NULL,"Anthroposiphic Press","Anthroposophic Press",NULL,"1994",NULL,"0880103841",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.3">
@@ -5514,6 +5816,9 @@
       <c r="H99" t="s">
         <v>502</v>
       </c>
+      <c r="J99" t="s">
+        <v>603</v>
+      </c>
       <c r="K99">
         <v>6</v>
       </c>
@@ -5522,7 +5827,7 @@
       </c>
       <c r="R99" t="str">
         <f t="shared" si="1"/>
-        <v>("Teaching as a Lively Art",NULL,"Spock, Marjorie","Anthroposophic Press",NULL,"1985",NULL,"088010127X",NULL,NULL,"6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Teaching as a Lively Art",NULL,"Spock, Marjorie","Anthroposophic Press",NULL,"1985",NULL,"088010127X",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.3">
@@ -5541,6 +5846,9 @@
       <c r="H100" t="s">
         <v>503</v>
       </c>
+      <c r="J100" t="s">
+        <v>603</v>
+      </c>
       <c r="K100">
         <v>2</v>
       </c>
@@ -5549,7 +5857,7 @@
       </c>
       <c r="R100" t="str">
         <f t="shared" si="1"/>
-        <v>("Celebrating the Festivals with Children",NULL,"Lenz, Friedel","Anthroposophic Press",NULL,"1989",NULL,"0880101512",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Celebrating the Festivals with Children",NULL,"Lenz, Friedel","Anthroposophic Press",NULL,"1989",NULL,"0880101512",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.3">
@@ -5568,6 +5876,9 @@
       <c r="H101" t="s">
         <v>504</v>
       </c>
+      <c r="J101" t="s">
+        <v>603</v>
+      </c>
       <c r="K101">
         <v>3</v>
       </c>
@@ -5576,7 +5887,7 @@
       </c>
       <c r="R101" t="str">
         <f t="shared" si="1"/>
-        <v>("The Education of the Child",NULL,"Steiner, Rudolf","Rudolf Steiner Press",NULL,"1979",NULL,"0854400303",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("The Education of the Child",NULL,"Steiner, Rudolf","Rudolf Steiner Press",NULL,"1979",NULL,"0854400303",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.3">
@@ -5595,6 +5906,9 @@
       <c r="H102" t="s">
         <v>505</v>
       </c>
+      <c r="J102" t="s">
+        <v>603</v>
+      </c>
       <c r="K102">
         <v>3</v>
       </c>
@@ -5603,7 +5917,7 @@
       </c>
       <c r="R102" t="str">
         <f t="shared" si="1"/>
-        <v>("The Child and the Machine",NULL,"Armstrong, Alison / Casement, Charles","Key Porter Books",NULL,"1998",NULL,"1552630048",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("The Child and the Machine",NULL,"Armstrong, Alison / Casement, Charles","Key Porter Books",NULL,"1998",NULL,"1552630048",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
@@ -5622,6 +5936,9 @@
       <c r="H103" t="s">
         <v>506</v>
       </c>
+      <c r="J103" t="s">
+        <v>603</v>
+      </c>
       <c r="K103">
         <v>3</v>
       </c>
@@ -5630,7 +5947,7 @@
       </c>
       <c r="R103" t="str">
         <f t="shared" si="1"/>
-        <v>("Between From and Freedom",NULL,"Staley, Betty","Hawthorn Press",NULL,"1996",NULL,"1869890086",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Between From and Freedom",NULL,"Staley, Betty","Hawthorn Press",NULL,"1996",NULL,"1869890086",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.3">
@@ -5649,6 +5966,9 @@
       <c r="I104" t="s">
         <v>507</v>
       </c>
+      <c r="J104" t="s">
+        <v>603</v>
+      </c>
       <c r="K104">
         <v>9</v>
       </c>
@@ -5657,7 +5977,7 @@
       </c>
       <c r="R104" t="str">
         <f t="shared" si="1"/>
-        <v>("The Curse of the Good Girl",NULL,"Simmons, Rachel","Penguin Books",NULL,"2010",NULL,NULL,"9780143117988",NULL,"9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("The Curse of the Good Girl",NULL,"Simmons, Rachel","Penguin Books",NULL,"2010",NULL,NULL,"9780143117988","PARENT","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.3">
@@ -5676,6 +5996,9 @@
       <c r="H105" t="s">
         <v>508</v>
       </c>
+      <c r="J105" t="s">
+        <v>603</v>
+      </c>
       <c r="K105">
         <v>6</v>
       </c>
@@ -5684,7 +6007,7 @@
       </c>
       <c r="R105" t="str">
         <f t="shared" si="1"/>
-        <v>("Too Old Too Soon",NULL,"Fields, Doug","Harvest House Publishers",NULL,"1991",NULL,"0890818487",NULL,NULL,"6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Too Old Too Soon",NULL,"Fields, Doug","Harvest House Publishers",NULL,"1991",NULL,"0890818487",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.3">
@@ -5703,6 +6026,9 @@
       <c r="H106" s="5" t="s">
         <v>509</v>
       </c>
+      <c r="J106" t="s">
+        <v>603</v>
+      </c>
       <c r="K106">
         <v>5</v>
       </c>
@@ -5711,7 +6037,7 @@
       </c>
       <c r="R106" t="str">
         <f t="shared" si="1"/>
-        <v>("A Child Is Born",NULL,"zur Linden, Wilhelm","Rudolf Steiner Press",NULL,"1980",NULL,"085443574",NULL,NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("A Child Is Born",NULL,"zur Linden, Wilhelm","Rudolf Steiner Press",NULL,"1980",NULL,"085443574",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.3">
@@ -5730,6 +6056,9 @@
       <c r="H107" t="s">
         <v>510</v>
       </c>
+      <c r="J107" t="s">
+        <v>603</v>
+      </c>
       <c r="K107">
         <v>4</v>
       </c>
@@ -5738,7 +6067,7 @@
       </c>
       <c r="R107" t="str">
         <f t="shared" si="1"/>
-        <v>("Steiner Education in Theory and Practice",NULL,"Childs, Gilbert","Floris Books",NULL,"1991",NULL,"0863151310",NULL,NULL,"4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Steiner Education in Theory and Practice",NULL,"Childs, Gilbert","Floris Books",NULL,"1991",NULL,"0863151310",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.3">
@@ -5757,6 +6086,9 @@
       <c r="H108" t="s">
         <v>511</v>
       </c>
+      <c r="J108" t="s">
+        <v>603</v>
+      </c>
       <c r="K108">
         <v>7</v>
       </c>
@@ -5765,7 +6097,7 @@
       </c>
       <c r="R108" t="str">
         <f t="shared" si="1"/>
-        <v>("When a Child Is Born",NULL,"zur Linden, Wilhelm","Thorsons Publishers Inc., NY",NULL,"1984",NULL,"0722509561",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("When a Child Is Born",NULL,"zur Linden, Wilhelm","Thorsons Publishers Inc., NY",NULL,"1984",NULL,"0722509561",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.3">
@@ -5784,6 +6116,9 @@
       <c r="H109" t="s">
         <v>512</v>
       </c>
+      <c r="J109" t="s">
+        <v>603</v>
+      </c>
       <c r="K109">
         <v>10</v>
       </c>
@@ -5792,7 +6127,7 @@
       </c>
       <c r="R109" t="str">
         <f t="shared" si="1"/>
-        <v>("The Curriculum of the First Waldorf School",NULL,"von Heydebrand, Caroline","Steiner Schools Fellowhsip Publications",NULL,"1989",NULL,"0951033131",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("The Curriculum of the First Waldorf School",NULL,"von Heydebrand, Caroline","Steiner Schools Fellowhsip Publications",NULL,"1989",NULL,"0951033131",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.3">
@@ -5811,6 +6146,9 @@
       <c r="H110" t="s">
         <v>513</v>
       </c>
+      <c r="J110" t="s">
+        <v>603</v>
+      </c>
       <c r="K110">
         <v>1</v>
       </c>
@@ -5819,7 +6157,7 @@
       </c>
       <c r="R110" t="str">
         <f t="shared" si="1"/>
-        <v>("Reincarnation and Karma - Their Significance in Modern Culture",NULL,"Steiner, Rudolf","Steiner Book Centre, Inc., Vancouver",NULL,"1977",NULL,"0919924069",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Reincarnation and Karma - Their Significance in Modern Culture",NULL,"Steiner, Rudolf","Steiner Book Centre, Inc., Vancouver",NULL,"1977",NULL,"0919924069",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.3">
@@ -5841,6 +6179,9 @@
       <c r="H111" t="s">
         <v>514</v>
       </c>
+      <c r="J111" t="s">
+        <v>603</v>
+      </c>
       <c r="K111">
         <v>3</v>
       </c>
@@ -5849,7 +6190,7 @@
       </c>
       <c r="R111" t="str">
         <f t="shared" si="1"/>
-        <v>("Theosophy",NULL,"Steiner, Rudolf","Rudolf Steiner Press","4","1973",NULL,"0854402705",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Theosophy",NULL,"Steiner, Rudolf","Rudolf Steiner Press","4","1973",NULL,"0854402705",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.3">
@@ -5868,6 +6209,9 @@
       <c r="H112" t="s">
         <v>425</v>
       </c>
+      <c r="J112" t="s">
+        <v>603</v>
+      </c>
       <c r="K112">
         <v>7</v>
       </c>
@@ -5876,7 +6220,7 @@
       </c>
       <c r="R112" t="str">
         <f t="shared" si="1"/>
-        <v>("The Younger Generation",NULL,"Steiner, Rudolf","Anthroposophic Press",NULL,"1967",NULL,NULL,NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("The Younger Generation",NULL,"Steiner, Rudolf","Anthroposophic Press",NULL,"1967",NULL,NULL,NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.3">
@@ -5895,6 +6239,9 @@
       <c r="H113" t="s">
         <v>515</v>
       </c>
+      <c r="J113" t="s">
+        <v>603</v>
+      </c>
       <c r="K113">
         <v>1</v>
       </c>
@@ -5903,7 +6250,7 @@
       </c>
       <c r="R113" t="str">
         <f t="shared" si="1"/>
-        <v>("The Kingdom of Childhood",NULL,"Steiner, Rudolf","Rudolf Steiner Press",NULL,"1982",NULL,"0854402845",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("The Kingdom of Childhood",NULL,"Steiner, Rudolf","Rudolf Steiner Press",NULL,"1982",NULL,"0854402845",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.3">
@@ -5922,6 +6269,9 @@
       <c r="H114" t="s">
         <v>516</v>
       </c>
+      <c r="J114" t="s">
+        <v>603</v>
+      </c>
       <c r="K114">
         <v>3</v>
       </c>
@@ -5930,7 +6280,7 @@
       </c>
       <c r="R114" t="str">
         <f t="shared" si="1"/>
-        <v>("Encountering the Self",NULL,"Koepke, Hermann","Anthroposophic Press",NULL,"1989",NULL,"0880102799",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Encountering the Self",NULL,"Koepke, Hermann","Anthroposophic Press",NULL,"1989",NULL,"0880102799",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.3">
@@ -5949,6 +6299,9 @@
       <c r="H115" t="s">
         <v>517</v>
       </c>
+      <c r="J115" t="s">
+        <v>603</v>
+      </c>
       <c r="K115">
         <v>3</v>
       </c>
@@ -5957,7 +6310,7 @@
       </c>
       <c r="R115" t="str">
         <f t="shared" si="1"/>
-        <v>("The Recovery of Man in Childhood",NULL,"Harwood, A.C.","Anthroposophic Press",NULL,"1982",NULL,"088010001X",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("The Recovery of Man in Childhood",NULL,"Harwood, A.C.","Anthroposophic Press",NULL,"1982",NULL,"088010001X",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.3">
@@ -5976,6 +6329,9 @@
       <c r="H116" t="s">
         <v>518</v>
       </c>
+      <c r="J116" t="s">
+        <v>603</v>
+      </c>
       <c r="K116">
         <v>10</v>
       </c>
@@ -5984,7 +6340,7 @@
       </c>
       <c r="R116" t="str">
         <f t="shared" si="1"/>
-        <v>("Rudold Steiner - Life, Work, Inner Path and Social Initiatives",NULL,"Lissau, Rudi","Hawthorn Press",NULL,"1987",NULL,"1869890068",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Rudold Steiner - Life, Work, Inner Path and Social Initiatives",NULL,"Lissau, Rudi","Hawthorn Press",NULL,"1987",NULL,"1869890068",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.3">
@@ -6003,6 +6359,9 @@
       <c r="H117" t="s">
         <v>519</v>
       </c>
+      <c r="J117" t="s">
+        <v>603</v>
+      </c>
       <c r="K117">
         <v>5</v>
       </c>
@@ -6011,7 +6370,7 @@
       </c>
       <c r="R117" t="str">
         <f t="shared" si="1"/>
-        <v>("The First Three Years of The Child",NULL,"Konig, Karl","Anthroposophic Press",NULL,"1984",NULL,"0880100435",NULL,NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("The First Three Years of The Child",NULL,"Konig, Karl","Anthroposophic Press",NULL,"1984",NULL,"0880100435",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.3">
@@ -6030,6 +6389,9 @@
       <c r="H118" t="s">
         <v>520</v>
       </c>
+      <c r="J118" t="s">
+        <v>603</v>
+      </c>
       <c r="K118">
         <v>2</v>
       </c>
@@ -6038,7 +6400,7 @@
       </c>
       <c r="R118" t="str">
         <f t="shared" si="1"/>
-        <v>("Confessions of a Waldorf Parent",NULL,"Gorman, Margaret","Rudolf Steiner College Publications",NULL,"1990",NULL,"0945803060",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Confessions of a Waldorf Parent",NULL,"Gorman, Margaret","Rudolf Steiner College Publications",NULL,"1990",NULL,"0945803060",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.3">
@@ -6057,6 +6419,9 @@
       <c r="H119" s="5" t="s">
         <v>521</v>
       </c>
+      <c r="J119" t="s">
+        <v>603</v>
+      </c>
       <c r="K119">
         <v>6</v>
       </c>
@@ -6065,7 +6430,7 @@
       </c>
       <c r="R119" t="str">
         <f t="shared" si="1"/>
-        <v>("Creativity in Education - The Waldorf Approach",NULL,"Querido, Rene M.","H. S. Dakin Company",NULL,"1987",NULL,"09304205",NULL,NULL,"6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Creativity in Education - The Waldorf Approach",NULL,"Querido, Rene M.","H. S. Dakin Company",NULL,"1987",NULL,"09304205",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.3">
@@ -6084,6 +6449,9 @@
       <c r="H120" t="s">
         <v>425</v>
       </c>
+      <c r="J120" t="s">
+        <v>603</v>
+      </c>
       <c r="K120">
         <v>9</v>
       </c>
@@ -6092,7 +6460,7 @@
       </c>
       <c r="R120" t="str">
         <f t="shared" si="1"/>
-        <v>("The Child, The Teachers and The Community",NULL,"Smit, Jorgen","Mercury Press",NULL,"1992",NULL,NULL,NULL,NULL,"9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("The Child, The Teachers and The Community",NULL,"Smit, Jorgen","Mercury Press",NULL,"1992",NULL,NULL,NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.3">
@@ -6111,6 +6479,9 @@
       <c r="H121" t="s">
         <v>425</v>
       </c>
+      <c r="J121" t="s">
+        <v>603</v>
+      </c>
       <c r="K121">
         <v>7</v>
       </c>
@@ -6119,7 +6490,7 @@
       </c>
       <c r="R121" t="str">
         <f t="shared" si="1"/>
-        <v>("The Philosophy of Freedom",NULL,"Steiner, Rudolf","Anthroposophic Press",NULL,"1964",NULL,NULL,NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("The Philosophy of Freedom",NULL,"Steiner, Rudolf","Anthroposophic Press",NULL,"1964",NULL,NULL,NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.3">
@@ -6138,6 +6509,9 @@
       <c r="H122" t="s">
         <v>522</v>
       </c>
+      <c r="J122" t="s">
+        <v>603</v>
+      </c>
       <c r="K122">
         <v>7</v>
       </c>
@@ -6146,7 +6520,7 @@
       </c>
       <c r="R122" t="str">
         <f t="shared" si="1"/>
-        <v>("Questions of Destiny",NULL,"Pietzner, Carlo","Anthroposophic Press",NULL,"1988",NULL,"0880102640",NULL,NULL,"7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Questions of Destiny",NULL,"Pietzner, Carlo","Anthroposophic Press",NULL,"1988",NULL,"0880102640",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.3">
@@ -6165,6 +6539,9 @@
       <c r="H123" t="s">
         <v>523</v>
       </c>
+      <c r="J123" t="s">
+        <v>603</v>
+      </c>
       <c r="K123">
         <v>6</v>
       </c>
@@ -6173,7 +6550,7 @@
       </c>
       <c r="R123" t="str">
         <f t="shared" si="1"/>
-        <v>("Anthroposophy - A Way of Life",NULL,"Edmunds, Francis","Carnant Books",NULL,"1982",NULL,"0903580659",NULL,NULL,"6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Anthroposophy - A Way of Life",NULL,"Edmunds, Francis","Carnant Books",NULL,"1982",NULL,"0903580659",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.3">
@@ -6192,6 +6569,9 @@
       <c r="H124" t="s">
         <v>425</v>
       </c>
+      <c r="J124" t="s">
+        <v>603</v>
+      </c>
       <c r="K124">
         <v>2</v>
       </c>
@@ -6200,7 +6580,7 @@
       </c>
       <c r="R124" t="str">
         <f t="shared" si="1"/>
-        <v>("Waldorf: Education for Tomorrow",NULL,"Toronto Waldorf Schools","Torornto Waldorf Schools",NULL,"1970",NULL,NULL,NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Waldorf: Education for Tomorrow",NULL,"Toronto Waldorf Schools","Torornto Waldorf Schools",NULL,"1970",NULL,NULL,NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.3">
@@ -6222,6 +6602,9 @@
       <c r="H125" t="s">
         <v>524</v>
       </c>
+      <c r="J125" t="s">
+        <v>603</v>
+      </c>
       <c r="K125">
         <v>5</v>
       </c>
@@ -6230,7 +6613,7 @@
       </c>
       <c r="R125" t="str">
         <f t="shared" si="1"/>
-        <v>("Waldorf Parenting Book",NULL,"Cusick, Lois","Rudolf Steiner College Publications","3","1992",NULL,"0916786757",NULL,NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Waldorf Parenting Book",NULL,"Cusick, Lois","Rudolf Steiner College Publications","3","1992",NULL,"0916786757",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.3">
@@ -6249,6 +6632,9 @@
       <c r="H126" t="s">
         <v>525</v>
       </c>
+      <c r="J126" t="s">
+        <v>603</v>
+      </c>
       <c r="K126">
         <v>2</v>
       </c>
@@ -6257,7 +6643,7 @@
       </c>
       <c r="R126" t="str">
         <f t="shared" si="1"/>
-        <v>("The Goetheanum - Rudolf Steiner's Architectual Impulse",NULL,"Biesantz, Hagen / Klingborg, Arne","Rudolf Steiner Press",NULL,"1979",NULL,"0854403558",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("The Goetheanum - Rudolf Steiner's Architectual Impulse",NULL,"Biesantz, Hagen / Klingborg, Arne","Rudolf Steiner Press",NULL,"1979",NULL,"0854403558",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.3">
@@ -6276,6 +6662,9 @@
       <c r="H127" t="s">
         <v>526</v>
       </c>
+      <c r="J127" t="s">
+        <v>603</v>
+      </c>
       <c r="K127">
         <v>1</v>
       </c>
@@ -6284,7 +6673,7 @@
       </c>
       <c r="R127" t="str">
         <f t="shared" si="1"/>
-        <v>("The Plug-In Drug - Television, Children and the Family",NULL,"Winn, Marie","Penguin Books",NULL,"1985",NULL,"0140076980",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("The Plug-In Drug - Television, Children and the Family",NULL,"Winn, Marie","Penguin Books",NULL,"1985",NULL,"0140076980",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.3">
@@ -6306,6 +6695,9 @@
       <c r="H128" t="s">
         <v>527</v>
       </c>
+      <c r="J128" t="s">
+        <v>603</v>
+      </c>
       <c r="K128">
         <v>1</v>
       </c>
@@ -6314,7 +6706,7 @@
       </c>
       <c r="R128" t="str">
         <f t="shared" si="1"/>
-        <v>("Who's Bringing Them Up?",NULL,"Large, Martin","Hawthorn Press","2","1990",NULL,"1869890248",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Who's Bringing Them Up?",NULL,"Large, Martin","Hawthorn Press","2","1990",NULL,"1869890248",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.3">
@@ -6333,6 +6725,9 @@
       <c r="H129" t="s">
         <v>528</v>
       </c>
+      <c r="J129" t="s">
+        <v>603</v>
+      </c>
       <c r="K129">
         <v>5</v>
       </c>
@@ -6341,7 +6736,7 @@
       </c>
       <c r="R129" t="str">
         <f t="shared" si="1"/>
-        <v>("The Young Child",NULL,"De Haes, Daniel Udo","Floris Books",NULL,"1986",NULL,"0863150373",NULL,NULL,"5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("The Young Child",NULL,"De Haes, Daniel Udo","Floris Books",NULL,"1986",NULL,"0863150373",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.3">
@@ -6363,6 +6758,9 @@
       <c r="H130" t="s">
         <v>529</v>
       </c>
+      <c r="J130" t="s">
+        <v>603</v>
+      </c>
       <c r="K130">
         <v>1</v>
       </c>
@@ -6371,7 +6769,7 @@
       </c>
       <c r="R130" t="str">
         <f t="shared" si="1"/>
-        <v>("Vision in Action ",NULL,"Schaefer, Christopher / Voors, Tyno","Lindisfarne Press","2","1986",NULL,"0940262746",NULL,NULL,"1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Vision in Action ",NULL,"Schaefer, Christopher / Voors, Tyno","Lindisfarne Press","2","1986",NULL,"0940262746",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.3">
@@ -6389,6 +6787,9 @@
       </c>
       <c r="H131" t="s">
         <v>530</v>
+      </c>
+      <c r="J131" t="s">
+        <v>603</v>
       </c>
       <c r="K131">
         <v>3</v>
@@ -6414,7 +6815,7 @@
 IF(N131="","NULL",_xlfn.CONCAT("""",N131,"""")),",",
 IF(O131="","NULL",_xlfn.CONCAT("""",O131,"""")),",",
 IF(P131="","NULL",_xlfn.CONCAT("""",P131,"""")),"),")</f>
-        <v>("Endangered Minds ",NULL,"Healy, Jane M.","Touchstone Book",NULL,"1990",NULL,"067174920X",NULL,NULL,"3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Endangered Minds ",NULL,"Healy, Jane M.","Touchstone Book",NULL,"1990",NULL,"067174920X",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.3">
@@ -6436,6 +6837,9 @@
       <c r="H132" t="s">
         <v>531</v>
       </c>
+      <c r="J132" t="s">
+        <v>603</v>
+      </c>
       <c r="K132">
         <v>8</v>
       </c>
@@ -6444,7 +6848,7 @@
       </c>
       <c r="R132" t="str">
         <f t="shared" si="2"/>
-        <v>("Waldorf Student Reading List",NULL,"Johnson Fenner, Pamela / Rivers, Karen L.","Michealmas Press","3","1995",NULL,"0964783207",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Waldorf Student Reading List",NULL,"Johnson Fenner, Pamela / Rivers, Karen L.","Michealmas Press","3","1995",NULL,"0964783207",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.3">
@@ -6463,6 +6867,9 @@
       <c r="H133" t="s">
         <v>532</v>
       </c>
+      <c r="J133" t="s">
+        <v>603</v>
+      </c>
       <c r="K133">
         <v>10</v>
       </c>
@@ -6471,7 +6878,7 @@
       </c>
       <c r="R133" t="str">
         <f t="shared" si="2"/>
-        <v>("The Recovery of Man in Childhood",NULL,"Harwood, A.C.","The Myrin Book, NY",NULL,"1992",NULL,"0913098434",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("The Recovery of Man in Childhood",NULL,"Harwood, A.C.","The Myrin Book, NY",NULL,"1992",NULL,"0913098434",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.3">
@@ -6490,6 +6897,9 @@
       <c r="H134" t="s">
         <v>533</v>
       </c>
+      <c r="J134" t="s">
+        <v>603</v>
+      </c>
       <c r="K134">
         <v>8</v>
       </c>
@@ -6498,7 +6908,7 @@
       </c>
       <c r="R134" t="str">
         <f t="shared" si="2"/>
-        <v>("The First Seven Years -  Physiology of Childhood",NULL,"Schoorel, Edmond","Rudolf Steiner College Press",NULL,"2004",NULL,"0945803680",NULL,NULL,"8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("The First Seven Years -  Physiology of Childhood",NULL,"Schoorel, Edmond","Rudolf Steiner College Press",NULL,"2004",NULL,"0945803680",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.3">
@@ -6517,6 +6927,9 @@
       <c r="H135" t="s">
         <v>534</v>
       </c>
+      <c r="J135" t="s">
+        <v>603</v>
+      </c>
       <c r="K135">
         <v>2</v>
       </c>
@@ -6525,7 +6938,7 @@
       </c>
       <c r="R135" t="str">
         <f t="shared" si="2"/>
-        <v>("Rudolf Steiner Education and The Developing Child",NULL,"Aeppli, Willi","Anthroposophic Press",NULL,"1986",NULL,"0880101644",NULL,NULL,"2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Rudolf Steiner Education and The Developing Child",NULL,"Aeppli, Willi","Anthroposophic Press",NULL,"1986",NULL,"0880101644",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.3">
@@ -6544,6 +6957,9 @@
       <c r="H136" t="s">
         <v>535</v>
       </c>
+      <c r="J136" t="s">
+        <v>603</v>
+      </c>
       <c r="K136">
         <v>10</v>
       </c>
@@ -6552,7 +6968,7 @@
       </c>
       <c r="R136" t="str">
         <f t="shared" si="2"/>
-        <v>("Waldorf Schools  -Upper Grades and High School",NULL,"Pusch, Ruth","Mercury Press",NULL,"1993",NULL,"0929979303",NULL,NULL,"10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Waldorf Schools  -Upper Grades and High School",NULL,"Pusch, Ruth","Mercury Press",NULL,"1993",NULL,"0929979303",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.3">
@@ -6570,6 +6986,9 @@
       </c>
       <c r="H137" t="s">
         <v>536</v>
+      </c>
+      <c r="J137" t="s">
+        <v>603</v>
       </c>
       <c r="K137">
         <v>3</v>
@@ -6595,7 +7014,7 @@
 IF(N137="","NULL",_xlfn.CONCAT("""",N137,"""")),",",
 IF(O137="","NULL",_xlfn.CONCAT("""",O137,"""")),",",
 IF(P137="","NULL",_xlfn.CONCAT("""",P137,"""")),");")</f>
-        <v>("Waldorf Schools  -Kindergarten and Early Grades",NULL,"Pusch, Ruth","Mercury Press",NULL,"1996",NULL,"092997929X",NULL,NULL,"3","3",NULL,NULL,NULL,NULL);</v>
+        <v>("Waldorf Schools  -Kindergarten and Early Grades",NULL,"Pusch, Ruth","Mercury Press",NULL,"1996",NULL,"092997929X",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -10084,7 +10503,7 @@
         <v>591</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>354</v>
+        <v>605</v>
       </c>
       <c r="H2" t="s">
         <v>354</v>
@@ -10099,7 +10518,7 @@
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),",",
 IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),"),")</f>
-        <v>("1","irene","Irene",NULL,"Pauchard","i.pauchard@calgarywaldorf.org","admin","admin"),</v>
+        <v>("1","irene","Irene",NULL,"Pauchard","i.pauchard@calgarywaldorf.org","$2a$10$Gitv.jdJOSpID30NmPEqn.IwH5CztayH4HbRUjxGDJKNM3DWCwMmy","admin"),</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -10119,7 +10538,7 @@
         <v>592</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>354</v>
+        <v>606</v>
       </c>
       <c r="H3" t="s">
         <v>354</v>
@@ -10134,7 +10553,7 @@
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),",",
 IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),"),")</f>
-        <v>("2","yves","Yves",NULL,"Pauchard","yves.pauchard@ucalgary.ca","admin","admin"),</v>
+        <v>("2","yves","Yves",NULL,"Pauchard","yves.pauchard@ucalgary.ca","$2a$10$GWg.rygxrh6caI2PaZTFvOreHBGaglUmkx1tyhutkxPN0QC1G1oT2","admin"),</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -10154,7 +10573,7 @@
         <v>596</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>354</v>
+        <v>604</v>
       </c>
       <c r="H4" t="s">
         <v>597</v>
@@ -10169,7 +10588,7 @@
 IF(F4="","NULL",_xlfn.CONCAT("""",F4,"""")),",",
 IF(G4="","NULL",_xlfn.CONCAT("""",G4,"""")),",",
 IF(H4="","NULL",_xlfn.CONCAT("""",H4,"""")),"),")</f>
-        <v>("3","zbhavyai","Bhavyai",NULL,"Gupta","zbhavyai@gmail.com","admin","faculty"),</v>
+        <v>("3","zbhavyai","Bhavyai",NULL,"Gupta","zbhavyai@gmail.com","$2a$10$..4RvEGzO5/TiayeVSm1lOTHqo456ZPPCrf7G7.eyPvndgkICr/tq","faculty"),</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -10192,7 +10611,7 @@
         <v>599</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>354</v>
+        <v>607</v>
       </c>
       <c r="H5" t="s">
         <v>354</v>
@@ -10207,7 +10626,7 @@
 IF(F5="","NULL",_xlfn.CONCAT("""",F5,"""")),",",
 IF(G5="","NULL",_xlfn.CONCAT("""",G5,"""")),",",
 IF(H5="","NULL",_xlfn.CONCAT("""",H5,"""")),");")</f>
-        <v>("4","mmylee","Michael","Man Yin","Lee","mmylee@ucalgary.ca","admin","admin");</v>
+        <v>("4","mmylee","Michael","Man Yin","Lee","mmylee@ucalgary.ca","$2a$10$vrf9vKF0tT3xBQlEFbVjje.4LZgyCtRfBaIjCf4KO0QDQuvOKEijC","admin");</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
build: #11 #12 changing librarian roles from string to enum
</commit_message>
<xml_diff>
--- a/sql/02_dummy_data_generator.xlsx
+++ b/sql/02_dummy_data_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\budlib\budlib-api\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2F6F69-9739-479A-8C11-20474CF07386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BAF87A-9004-4880-A5F7-D2053ED00DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="606">
   <si>
     <t>book_id</t>
   </si>
@@ -1104,9 +1104,6 @@
     <t>role</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>school_id</t>
   </si>
   <si>
@@ -1831,9 +1828,6 @@
   </si>
   <si>
     <t>zbhavyai@gmail.com</t>
-  </si>
-  <si>
-    <t>faculty</t>
   </si>
   <si>
     <t>mmylee</t>
@@ -2776,13 +2770,13 @@
         <v>7</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>411</v>
       </c>
       <c r="R1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO book (",
@@ -2823,7 +2817,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="J2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -2867,10 +2861,10 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J3" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K3">
         <v>4</v>
@@ -2914,10 +2908,10 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J4" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K4">
         <v>9</v>
@@ -2945,10 +2939,10 @@
       </c>
       <c r="G5" s="1"/>
       <c r="H5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -2976,10 +2970,10 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="J6" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K6">
         <v>2</v>
@@ -3007,10 +3001,10 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J7" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K7">
         <v>4</v>
@@ -3038,10 +3032,10 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J8" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K8">
         <v>9</v>
@@ -3069,10 +3063,10 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J9" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K9">
         <v>10</v>
@@ -3103,10 +3097,10 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J10" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K10">
         <v>9</v>
@@ -3134,10 +3128,10 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J11" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -3165,10 +3159,10 @@
       </c>
       <c r="G12" s="1"/>
       <c r="H12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="J12" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -3196,10 +3190,10 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="J13" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K13">
         <v>6</v>
@@ -3228,10 +3222,10 @@
       <c r="G14" s="1"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="J14" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -3259,10 +3253,10 @@
       </c>
       <c r="G15" s="1"/>
       <c r="H15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J15" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K15">
         <v>7</v>
@@ -3290,7 +3284,7 @@
       </c>
       <c r="G16" s="1"/>
       <c r="J16" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -3318,10 +3312,10 @@
       </c>
       <c r="G17" s="1"/>
       <c r="H17" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="J17" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K17">
         <v>6</v>
@@ -3352,10 +3346,10 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="J18" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -3383,10 +3377,10 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="J19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K19">
         <v>7</v>
@@ -3413,10 +3407,10 @@
         <v>1995</v>
       </c>
       <c r="H20" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="J20" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -3443,10 +3437,10 @@
         <v>1993</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J21" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K21">
         <v>4</v>
@@ -3473,10 +3467,10 @@
         <v>1994</v>
       </c>
       <c r="H22" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="J22" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K22">
         <v>10</v>
@@ -3503,10 +3497,10 @@
         <v>2001</v>
       </c>
       <c r="H23" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J23" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -3533,10 +3527,10 @@
         <v>1990</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J24" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K24">
         <v>8</v>
@@ -3563,10 +3557,10 @@
         <v>1996</v>
       </c>
       <c r="H25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J25" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K25">
         <v>4</v>
@@ -3593,10 +3587,10 @@
         <v>1992</v>
       </c>
       <c r="H26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J26" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K26">
         <v>6</v>
@@ -3626,10 +3620,10 @@
         <v>1989</v>
       </c>
       <c r="H27" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J27" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -3656,10 +3650,10 @@
         <v>2001</v>
       </c>
       <c r="H28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J28" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K28">
         <v>9</v>
@@ -3689,10 +3683,10 @@
         <v>1994</v>
       </c>
       <c r="H29" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J29" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -3719,10 +3713,10 @@
         <v>1997</v>
       </c>
       <c r="H30" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J30" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -3749,10 +3743,10 @@
         <v>1988</v>
       </c>
       <c r="H31" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J31" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K31">
         <v>8</v>
@@ -3779,10 +3773,10 @@
         <v>1994</v>
       </c>
       <c r="H32" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J32" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K32">
         <v>8</v>
@@ -3809,10 +3803,10 @@
         <v>2008</v>
       </c>
       <c r="I33" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J33" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K33">
         <v>2</v>
@@ -3839,10 +3833,10 @@
         <v>1990</v>
       </c>
       <c r="H34" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J34" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K34">
         <v>10</v>
@@ -3869,10 +3863,10 @@
         <v>2001</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J35" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -3899,10 +3893,10 @@
         <v>1996</v>
       </c>
       <c r="H36" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="J36" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K36">
         <v>10</v>
@@ -3929,10 +3923,10 @@
         <v>1995</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J37" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K37">
         <v>7</v>
@@ -3959,10 +3953,10 @@
         <v>1980</v>
       </c>
       <c r="H38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J38" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K38">
         <v>8</v>
@@ -3989,10 +3983,10 @@
         <v>1993</v>
       </c>
       <c r="H39" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J39" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K39">
         <v>8</v>
@@ -4019,10 +4013,10 @@
         <v>1998</v>
       </c>
       <c r="H40" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J40" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K40">
         <v>2</v>
@@ -4049,10 +4043,10 @@
         <v>1995</v>
       </c>
       <c r="H41" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="J41" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K41">
         <v>10</v>
@@ -4079,10 +4073,10 @@
         <v>2003</v>
       </c>
       <c r="H42" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J42" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K42">
         <v>10</v>
@@ -4109,10 +4103,10 @@
         <v>1979</v>
       </c>
       <c r="H43" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J43" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K43">
         <v>5</v>
@@ -4139,10 +4133,10 @@
         <v>1991</v>
       </c>
       <c r="H44" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J44" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -4169,10 +4163,10 @@
         <v>1986</v>
       </c>
       <c r="H45" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J45" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K45">
         <v>2</v>
@@ -4199,10 +4193,10 @@
         <v>1981</v>
       </c>
       <c r="H46" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J46" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K46">
         <v>5</v>
@@ -4232,10 +4226,10 @@
         <v>1983</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J47" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K47">
         <v>4</v>
@@ -4262,10 +4256,10 @@
         <v>1983</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J48" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K48">
         <v>4</v>
@@ -4292,10 +4286,10 @@
         <v>1996</v>
       </c>
       <c r="H49" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J49" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K49">
         <v>5</v>
@@ -4322,10 +4316,10 @@
         <v>1990</v>
       </c>
       <c r="H50" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J50" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K50">
         <v>4</v>
@@ -4352,10 +4346,10 @@
         <v>1987</v>
       </c>
       <c r="H51" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J51" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K51">
         <v>7</v>
@@ -4382,10 +4376,10 @@
         <v>1979</v>
       </c>
       <c r="H52" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="J52" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K52">
         <v>9</v>
@@ -4412,10 +4406,10 @@
         <v>1989</v>
       </c>
       <c r="H53" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="J53" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K53">
         <v>6</v>
@@ -4442,10 +4436,10 @@
         <v>1990</v>
       </c>
       <c r="H54" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J54" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K54">
         <v>2</v>
@@ -4472,10 +4466,10 @@
         <v>2001</v>
       </c>
       <c r="H55" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J55" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K55">
         <v>3</v>
@@ -4502,10 +4496,10 @@
         <v>1993</v>
       </c>
       <c r="H56" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J56" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K56">
         <v>9</v>
@@ -4532,10 +4526,10 @@
         <v>1994</v>
       </c>
       <c r="H57" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J57" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -4562,10 +4556,10 @@
         <v>2001</v>
       </c>
       <c r="H58" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="J58" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K58">
         <v>6</v>
@@ -4595,10 +4589,10 @@
         <v>1991</v>
       </c>
       <c r="H59" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="J59" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K59">
         <v>1</v>
@@ -4628,10 +4622,10 @@
         <v>1983</v>
       </c>
       <c r="H60" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J60" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K60">
         <v>5</v>
@@ -4661,10 +4655,10 @@
         <v>1983</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="J61" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K61">
         <v>8</v>
@@ -4691,10 +4685,10 @@
         <v>1987</v>
       </c>
       <c r="H62" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J62" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K62">
         <v>9</v>
@@ -4721,10 +4715,10 @@
         <v>1994</v>
       </c>
       <c r="H63" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J63" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K63">
         <v>5</v>
@@ -4751,10 +4745,10 @@
         <v>1983</v>
       </c>
       <c r="H64" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="J64" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -4778,10 +4772,10 @@
         <v>267</v>
       </c>
       <c r="H65" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J65" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K65">
         <v>1</v>
@@ -4808,10 +4802,10 @@
         <v>1984</v>
       </c>
       <c r="H66" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J66" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K66">
         <v>3</v>
@@ -4838,10 +4832,10 @@
         <v>1986</v>
       </c>
       <c r="H67" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="J67" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K67">
         <v>7</v>
@@ -4884,10 +4878,10 @@
         <v>2002</v>
       </c>
       <c r="H68" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="J68" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K68">
         <v>6</v>
@@ -4914,10 +4908,10 @@
         <v>1988</v>
       </c>
       <c r="H69" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="J69" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K69">
         <v>8</v>
@@ -4944,10 +4938,10 @@
         <v>1992</v>
       </c>
       <c r="H70" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J70" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K70">
         <v>10</v>
@@ -4974,10 +4968,10 @@
         <v>1985</v>
       </c>
       <c r="H71" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J71" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K71">
         <v>2</v>
@@ -5004,10 +4998,10 @@
         <v>1987</v>
       </c>
       <c r="H72" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J72" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K72">
         <v>8</v>
@@ -5034,10 +5028,10 @@
         <v>1995</v>
       </c>
       <c r="H73" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J73" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -5064,10 +5058,10 @@
         <v>1989</v>
       </c>
       <c r="H74" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J74" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K74">
         <v>4</v>
@@ -5094,10 +5088,10 @@
         <v>991</v>
       </c>
       <c r="H75" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J75" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K75">
         <v>10</v>
@@ -5124,10 +5118,10 @@
         <v>1992</v>
       </c>
       <c r="I76" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="J76" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K76">
         <v>5</v>
@@ -5154,10 +5148,10 @@
         <v>1991</v>
       </c>
       <c r="H77" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J77" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K77">
         <v>2</v>
@@ -5184,10 +5178,10 @@
         <v>1992</v>
       </c>
       <c r="H78" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J78" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K78">
         <v>3</v>
@@ -5214,10 +5208,10 @@
         <v>1997</v>
       </c>
       <c r="H79" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J79" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K79">
         <v>9</v>
@@ -5244,10 +5238,10 @@
         <v>1995</v>
       </c>
       <c r="H80" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="J80" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K80">
         <v>7</v>
@@ -5274,10 +5268,10 @@
         <v>1998</v>
       </c>
       <c r="H81" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J81" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K81">
         <v>4</v>
@@ -5304,10 +5298,10 @@
         <v>2000</v>
       </c>
       <c r="H82" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J82" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K82">
         <v>7</v>
@@ -5334,10 +5328,10 @@
         <v>1997</v>
       </c>
       <c r="H83" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J83" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K83">
         <v>7</v>
@@ -5364,10 +5358,10 @@
         <v>1989</v>
       </c>
       <c r="H84" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J84" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K84">
         <v>10</v>
@@ -5394,10 +5388,10 @@
         <v>1989</v>
       </c>
       <c r="H85" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J85" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K85">
         <v>3</v>
@@ -5424,10 +5418,10 @@
         <v>1989</v>
       </c>
       <c r="H86" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J86" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K86">
         <v>8</v>
@@ -5454,10 +5448,10 @@
         <v>2000</v>
       </c>
       <c r="H87" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J87" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K87">
         <v>2</v>
@@ -5484,10 +5478,10 @@
         <v>1981</v>
       </c>
       <c r="H88" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J88" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K88">
         <v>7</v>
@@ -5514,10 +5508,10 @@
         <v>1999</v>
       </c>
       <c r="H89" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="J89" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K89">
         <v>2</v>
@@ -5544,10 +5538,10 @@
         <v>1997</v>
       </c>
       <c r="H90" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J90" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -5574,10 +5568,10 @@
         <v>1980</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J91" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K91">
         <v>4</v>
@@ -5604,10 +5598,10 @@
         <v>2000</v>
       </c>
       <c r="H92" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="J92" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K92">
         <v>10</v>
@@ -5634,10 +5628,10 @@
         <v>1986</v>
       </c>
       <c r="H93" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="J93" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K93">
         <v>5</v>
@@ -5664,10 +5658,10 @@
         <v>1995</v>
       </c>
       <c r="H94" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="J94" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K94">
         <v>4</v>
@@ -5694,10 +5688,10 @@
         <v>1997</v>
       </c>
       <c r="H95" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="J95" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K95">
         <v>3</v>
@@ -5724,10 +5718,10 @@
         <v>1993</v>
       </c>
       <c r="H96" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="J96" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K96">
         <v>4</v>
@@ -5754,10 +5748,10 @@
         <v>1983</v>
       </c>
       <c r="H97" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J97" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K97">
         <v>3</v>
@@ -5784,10 +5778,10 @@
         <v>1994</v>
       </c>
       <c r="H98" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J98" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K98">
         <v>2</v>
@@ -5814,10 +5808,10 @@
         <v>1985</v>
       </c>
       <c r="H99" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="J99" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K99">
         <v>6</v>
@@ -5844,10 +5838,10 @@
         <v>1989</v>
       </c>
       <c r="H100" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="J100" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K100">
         <v>2</v>
@@ -5874,10 +5868,10 @@
         <v>1979</v>
       </c>
       <c r="H101" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J101" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K101">
         <v>3</v>
@@ -5904,10 +5898,10 @@
         <v>1998</v>
       </c>
       <c r="H102" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J102" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K102">
         <v>3</v>
@@ -5934,10 +5928,10 @@
         <v>1996</v>
       </c>
       <c r="H103" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J103" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K103">
         <v>3</v>
@@ -5964,10 +5958,10 @@
         <v>2010</v>
       </c>
       <c r="I104" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J104" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K104">
         <v>9</v>
@@ -5994,10 +5988,10 @@
         <v>1991</v>
       </c>
       <c r="H105" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J105" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K105">
         <v>6</v>
@@ -6024,10 +6018,10 @@
         <v>1980</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J106" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K106">
         <v>5</v>
@@ -6054,10 +6048,10 @@
         <v>1991</v>
       </c>
       <c r="H107" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J107" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K107">
         <v>4</v>
@@ -6084,10 +6078,10 @@
         <v>1984</v>
       </c>
       <c r="H108" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="J108" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K108">
         <v>7</v>
@@ -6114,10 +6108,10 @@
         <v>1989</v>
       </c>
       <c r="H109" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J109" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K109">
         <v>10</v>
@@ -6144,10 +6138,10 @@
         <v>1977</v>
       </c>
       <c r="H110" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J110" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K110">
         <v>1</v>
@@ -6177,10 +6171,10 @@
         <v>1973</v>
       </c>
       <c r="H111" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="J111" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K111">
         <v>3</v>
@@ -6207,10 +6201,10 @@
         <v>1967</v>
       </c>
       <c r="H112" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J112" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K112">
         <v>7</v>
@@ -6237,10 +6231,10 @@
         <v>1982</v>
       </c>
       <c r="H113" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J113" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K113">
         <v>1</v>
@@ -6267,10 +6261,10 @@
         <v>1989</v>
       </c>
       <c r="H114" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J114" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K114">
         <v>3</v>
@@ -6297,10 +6291,10 @@
         <v>1982</v>
       </c>
       <c r="H115" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J115" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K115">
         <v>3</v>
@@ -6327,10 +6321,10 @@
         <v>1987</v>
       </c>
       <c r="H116" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J116" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K116">
         <v>10</v>
@@ -6357,10 +6351,10 @@
         <v>1984</v>
       </c>
       <c r="H117" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="J117" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K117">
         <v>5</v>
@@ -6387,10 +6381,10 @@
         <v>1990</v>
       </c>
       <c r="H118" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J118" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K118">
         <v>2</v>
@@ -6417,10 +6411,10 @@
         <v>1987</v>
       </c>
       <c r="H119" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="J119" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K119">
         <v>6</v>
@@ -6447,10 +6441,10 @@
         <v>1992</v>
       </c>
       <c r="H120" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J120" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K120">
         <v>9</v>
@@ -6477,10 +6471,10 @@
         <v>1964</v>
       </c>
       <c r="H121" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J121" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K121">
         <v>7</v>
@@ -6507,10 +6501,10 @@
         <v>1988</v>
       </c>
       <c r="H122" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="J122" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K122">
         <v>7</v>
@@ -6537,10 +6531,10 @@
         <v>1982</v>
       </c>
       <c r="H123" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="J123" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K123">
         <v>6</v>
@@ -6567,10 +6561,10 @@
         <v>1970</v>
       </c>
       <c r="H124" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J124" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K124">
         <v>2</v>
@@ -6600,10 +6594,10 @@
         <v>1992</v>
       </c>
       <c r="H125" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="J125" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K125">
         <v>5</v>
@@ -6630,10 +6624,10 @@
         <v>1979</v>
       </c>
       <c r="H126" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J126" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K126">
         <v>2</v>
@@ -6660,10 +6654,10 @@
         <v>1985</v>
       </c>
       <c r="H127" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J127" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K127">
         <v>1</v>
@@ -6693,10 +6687,10 @@
         <v>1990</v>
       </c>
       <c r="H128" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J128" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K128">
         <v>1</v>
@@ -6723,10 +6717,10 @@
         <v>1986</v>
       </c>
       <c r="H129" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="J129" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K129">
         <v>5</v>
@@ -6756,10 +6750,10 @@
         <v>1986</v>
       </c>
       <c r="H130" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J130" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K130">
         <v>1</v>
@@ -6786,10 +6780,10 @@
         <v>1990</v>
       </c>
       <c r="H131" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J131" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K131">
         <v>3</v>
@@ -6835,10 +6829,10 @@
         <v>1995</v>
       </c>
       <c r="H132" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="J132" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K132">
         <v>8</v>
@@ -6865,10 +6859,10 @@
         <v>1992</v>
       </c>
       <c r="H133" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="J133" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K133">
         <v>10</v>
@@ -6895,10 +6889,10 @@
         <v>2004</v>
       </c>
       <c r="H134" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="J134" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K134">
         <v>8</v>
@@ -6925,10 +6919,10 @@
         <v>1986</v>
       </c>
       <c r="H135" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J135" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K135">
         <v>2</v>
@@ -6955,10 +6949,10 @@
         <v>1993</v>
       </c>
       <c r="H136" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J136" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K136">
         <v>10</v>
@@ -6985,10 +6979,10 @@
         <v>1996</v>
       </c>
       <c r="H137" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J137" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K137">
         <v>3</v>
@@ -10491,22 +10485,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>585</v>
+      </c>
+      <c r="C2" t="s">
         <v>586</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>587</v>
       </c>
-      <c r="E2" t="s">
-        <v>588</v>
-      </c>
       <c r="F2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="H2" t="s">
-        <v>354</v>
+        <v>603</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
       <c r="J2" t="str">
         <f>_xlfn.CONCAT("(",
@@ -10518,7 +10512,7 @@
 IF(F2="","NULL",_xlfn.CONCAT("""",F2,"""")),",",
 IF(G2="","NULL",_xlfn.CONCAT("""",G2,"""")),",",
 IF(H2="","NULL",_xlfn.CONCAT("""",H2,"""")),"),")</f>
-        <v>("1","irene","Irene",NULL,"Pauchard","i.pauchard@calgarywaldorf.org","$2a$10$Gitv.jdJOSpID30NmPEqn.IwH5CztayH4HbRUjxGDJKNM3DWCwMmy","admin"),</v>
+        <v>("1","irene","Irene",NULL,"Pauchard","i.pauchard@calgarywaldorf.org","$2a$10$Gitv.jdJOSpID30NmPEqn.IwH5CztayH4HbRUjxGDJKNM3DWCwMmy","0"),</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -10526,22 +10520,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>588</v>
+      </c>
+      <c r="C3" t="s">
         <v>589</v>
       </c>
-      <c r="C3" t="s">
-        <v>590</v>
-      </c>
       <c r="E3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="H3" t="s">
-        <v>354</v>
+        <v>604</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
       </c>
       <c r="J3" t="str">
         <f>_xlfn.CONCAT("(",
@@ -10553,7 +10547,7 @@
 IF(F3="","NULL",_xlfn.CONCAT("""",F3,"""")),",",
 IF(G3="","NULL",_xlfn.CONCAT("""",G3,"""")),",",
 IF(H3="","NULL",_xlfn.CONCAT("""",H3,"""")),"),")</f>
-        <v>("2","yves","Yves",NULL,"Pauchard","yves.pauchard@ucalgary.ca","$2a$10$GWg.rygxrh6caI2PaZTFvOreHBGaglUmkx1tyhutkxPN0QC1G1oT2","admin"),</v>
+        <v>("2","yves","Yves",NULL,"Pauchard","yves.pauchard@ucalgary.ca","$2a$10$GWg.rygxrh6caI2PaZTFvOreHBGaglUmkx1tyhutkxPN0QC1G1oT2","0"),</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -10561,22 +10555,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>592</v>
+      </c>
+      <c r="C4" t="s">
         <v>593</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>594</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>595</v>
       </c>
-      <c r="F4" t="s">
-        <v>596</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>604</v>
-      </c>
-      <c r="H4" t="s">
-        <v>597</v>
+        <v>602</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
       <c r="J4" t="str">
         <f>_xlfn.CONCAT("(",
@@ -10588,7 +10582,7 @@
 IF(F4="","NULL",_xlfn.CONCAT("""",F4,"""")),",",
 IF(G4="","NULL",_xlfn.CONCAT("""",G4,"""")),",",
 IF(H4="","NULL",_xlfn.CONCAT("""",H4,"""")),"),")</f>
-        <v>("3","zbhavyai","Bhavyai",NULL,"Gupta","zbhavyai@gmail.com","$2a$10$..4RvEGzO5/TiayeVSm1lOTHqo456ZPPCrf7G7.eyPvndgkICr/tq","faculty"),</v>
+        <v>("3","zbhavyai","Bhavyai",NULL,"Gupta","zbhavyai@gmail.com","$2a$10$..4RvEGzO5/TiayeVSm1lOTHqo456ZPPCrf7G7.eyPvndgkICr/tq","1"),</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -10596,25 +10590,25 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>596</v>
+      </c>
+      <c r="C5" t="s">
         <v>598</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>599</v>
+      </c>
+      <c r="E5" t="s">
         <v>600</v>
       </c>
-      <c r="D5" t="s">
-        <v>601</v>
-      </c>
-      <c r="E5" t="s">
-        <v>602</v>
-      </c>
       <c r="F5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="H5" t="s">
-        <v>354</v>
+        <v>605</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
       </c>
       <c r="J5" t="str">
         <f>_xlfn.CONCAT("(",
@@ -10626,7 +10620,7 @@
 IF(F5="","NULL",_xlfn.CONCAT("""",F5,"""")),",",
 IF(G5="","NULL",_xlfn.CONCAT("""",G5,"""")),",",
 IF(H5="","NULL",_xlfn.CONCAT("""",H5,"""")),");")</f>
-        <v>("4","mmylee","Michael","Man Yin","Lee","mmylee@ucalgary.ca","$2a$10$vrf9vKF0tT3xBQlEFbVjje.4LZgyCtRfBaIjCf4KO0QDQuvOKEijC","admin");</v>
+        <v>("4","mmylee","Michael","Man Yin","Lee","mmylee@ucalgary.ca","$2a$10$vrf9vKF0tT3xBQlEFbVjje.4LZgyCtRfBaIjCf4KO0QDQuvOKEijC","1");</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -10695,13 +10689,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>356</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>348</v>
@@ -10713,10 +10707,10 @@
         <v>350</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="J1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO loaner (",
@@ -10733,7 +10727,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -10743,10 +10737,10 @@
         <v>Mr</v>
       </c>
       <c r="D2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G2" s="1"/>
       <c r="J2" t="str">
@@ -10764,7 +10758,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -10774,10 +10768,10 @@
         <v>Mr</v>
       </c>
       <c r="D3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" t="str">
@@ -10795,7 +10789,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -10805,16 +10799,16 @@
         <v/>
       </c>
       <c r="D4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" si="1"/>
@@ -10823,7 +10817,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -10833,16 +10827,16 @@
         <v/>
       </c>
       <c r="D5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" si="1"/>
@@ -10851,7 +10845,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -10861,16 +10855,16 @@
         <v/>
       </c>
       <c r="D6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="1"/>
@@ -10879,7 +10873,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -10889,16 +10883,16 @@
         <v/>
       </c>
       <c r="D7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="1"/>
@@ -10907,7 +10901,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -10917,16 +10911,16 @@
         <v/>
       </c>
       <c r="D8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="1"/>
@@ -10935,7 +10929,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -10945,16 +10939,16 @@
         <v/>
       </c>
       <c r="D9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F9" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="1"/>
@@ -10963,7 +10957,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -10973,16 +10967,16 @@
         <v/>
       </c>
       <c r="D10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="1"/>
@@ -10991,7 +10985,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -11001,16 +10995,16 @@
         <v/>
       </c>
       <c r="D11" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="1"/>
@@ -11019,7 +11013,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -11029,16 +11023,16 @@
         <v/>
       </c>
       <c r="D12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F12" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="1"/>
@@ -11047,7 +11041,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -11057,16 +11051,16 @@
         <v/>
       </c>
       <c r="D13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F13" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="1"/>
@@ -11075,7 +11069,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -11085,10 +11079,10 @@
         <v>Mr</v>
       </c>
       <c r="D14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G14" s="1"/>
       <c r="J14" t="str">
@@ -11098,7 +11092,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -11108,10 +11102,10 @@
         <v>Mr</v>
       </c>
       <c r="D15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G15" s="1"/>
       <c r="J15" t="str">
@@ -11121,7 +11115,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -11131,10 +11125,10 @@
         <v>Mr</v>
       </c>
       <c r="D16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G16" s="1"/>
       <c r="J16" t="str">
@@ -11144,7 +11138,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -11154,16 +11148,16 @@
         <v/>
       </c>
       <c r="D17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F17" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="H17" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="1"/>
@@ -11172,7 +11166,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -11182,16 +11176,16 @@
         <v/>
       </c>
       <c r="D18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F18" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H18" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="1"/>
@@ -11200,7 +11194,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -11210,16 +11204,16 @@
         <v/>
       </c>
       <c r="D19" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F19" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H19" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="1"/>
@@ -11228,7 +11222,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -11238,16 +11232,16 @@
         <v/>
       </c>
       <c r="D20" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F20" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="1"/>
@@ -11256,7 +11250,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -11266,16 +11260,16 @@
         <v/>
       </c>
       <c r="D21" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H21" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J21" t="str">
         <f>_xlfn.CONCAT("(",
@@ -11312,16 +11306,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>585</v>
       </c>
       <c r="G1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO loan (",
@@ -11796,7 +11790,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A007853-9D1A-4913-959D-CC14E6BFBA3B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11806,16 +11802,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>407</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>346</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO transaction (",
@@ -12403,13 +12399,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E1" t="str">
         <f>_xlfn.CONCAT("INSERT INTO trn_quantities (",

</xml_diff>

<commit_message>
build: stats for upcoming due dates and overdue loans
</commit_message>
<xml_diff>
--- a/sql/02_dummy_data_generator.xlsx
+++ b/sql/02_dummy_data_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\budlib\budlib-api\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BAF87A-9004-4880-A5F7-D2053ED00DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05B3D0E-7E3E-4953-8E85-19DADB2E4805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11338,10 +11338,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>44223</v>
+        <v>44580</v>
       </c>
       <c r="E2" s="1">
-        <v>44254</v>
+        <v>44611</v>
       </c>
       <c r="G2" t="str">
         <f>_xlfn.CONCAT("(",
@@ -11350,7 +11350,7 @@
 IF(C2="","NULL",_xlfn.CONCAT("""",C2,"""")),",",
 IF(D2="","NULL",_xlfn.CONCAT("""",TEXT(D2,"YYYY-MM-DD"),"""")),",",
 IF(E2="","NULL",_xlfn.CONCAT("""",TEXT(E2,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("1","1","1","2021-01-27","2021-02-27"),</v>
+        <v>("1","1","1","2022-01-19","2022-02-19"),</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -11364,10 +11364,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="1">
-        <v>44212</v>
+        <v>44587</v>
       </c>
       <c r="E3" s="1">
-        <v>44243</v>
+        <v>44646</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G10" si="0">_xlfn.CONCAT("(",
@@ -11376,7 +11376,7 @@
 IF(C3="","NULL",_xlfn.CONCAT("""",C3,"""")),",",
 IF(D3="","NULL",_xlfn.CONCAT("""",TEXT(D3,"YYYY-MM-DD"),"""")),",",
 IF(E3="","NULL",_xlfn.CONCAT("""",TEXT(E3,"YYYY-MM-DD"),"""")),"),")</f>
-        <v>("2","2","2","2021-01-16","2021-02-16"),</v>
+        <v>("2","2","2","2022-01-26","2022-03-26"),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -11390,14 +11390,14 @@
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>44234</v>
+        <v>44593</v>
       </c>
       <c r="E4" s="1">
-        <v>44262</v>
+        <v>44652</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
-        <v>("3","8","3","2021-02-07","2021-03-07"),</v>
+        <v>("3","8","3","2022-02-01","2022-04-01"),</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -11411,14 +11411,14 @@
         <v>4</v>
       </c>
       <c r="D5" s="1">
-        <v>44247</v>
+        <v>44601</v>
       </c>
       <c r="E5" s="1">
-        <v>44275</v>
+        <v>44629</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
-        <v>("4","3","4","2021-02-20","2021-03-20"),</v>
+        <v>("4","3","4","2022-02-09","2022-03-09"),</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -11432,14 +11432,14 @@
         <v>5</v>
       </c>
       <c r="D6" s="1">
-        <v>44285</v>
+        <v>44609</v>
       </c>
       <c r="E6" s="1">
-        <v>44316</v>
+        <v>44637</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
-        <v>("5","1","5","2021-03-30","2021-04-30"),</v>
+        <v>("5","1","5","2022-02-17","2022-03-17"),</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -11453,14 +11453,14 @@
         <v>6</v>
       </c>
       <c r="D7" s="1">
-        <v>44268</v>
+        <v>44617</v>
       </c>
       <c r="E7" s="1">
-        <v>44300</v>
+        <v>44645</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
-        <v>("6","3","6","2021-03-13","2021-04-14"),</v>
+        <v>("6","3","6","2022-02-25","2022-03-25"),</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -11474,14 +11474,14 @@
         <v>7</v>
       </c>
       <c r="D8" s="1">
-        <v>44290</v>
+        <v>44623</v>
       </c>
       <c r="E8" s="1">
-        <v>44320</v>
+        <v>44654</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
-        <v>("7","6","7","2021-04-04","2021-05-04"),</v>
+        <v>("7","6","7","2022-03-03","2022-04-03"),</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -11495,14 +11495,14 @@
         <v>8</v>
       </c>
       <c r="D9" s="1">
-        <v>44287</v>
+        <v>44629</v>
       </c>
       <c r="E9" s="1">
-        <v>44317</v>
+        <v>44660</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
-        <v>("8","4","8","2021-04-01","2021-05-01"),</v>
+        <v>("8","4","8","2022-03-09","2022-04-09"),</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -11516,14 +11516,14 @@
         <v>9</v>
       </c>
       <c r="D10" s="1">
-        <v>44335</v>
+        <v>44635</v>
       </c>
       <c r="E10" s="1">
-        <v>44366</v>
+        <v>44666</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
-        <v>("9","5","9","2021-05-19","2021-06-19"),</v>
+        <v>("9","5","9","2022-03-15","2022-04-15"),</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -11537,10 +11537,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="1">
-        <v>44334</v>
+        <v>44641</v>
       </c>
       <c r="E11" s="1">
-        <v>44365</v>
+        <v>44672</v>
       </c>
       <c r="G11" t="str">
         <f>_xlfn.CONCAT("(",
@@ -11549,7 +11549,7 @@
 IF(C11="","NULL",_xlfn.CONCAT("""",C11,"""")),",",
 IF(D11="","NULL",_xlfn.CONCAT("""",TEXT(D11,"YYYY-MM-DD"),"""")),",",
 IF(E11="","NULL",_xlfn.CONCAT("""",TEXT(E11,"YYYY-MM-DD"),"""")),");")</f>
-        <v>("10","1","10","2021-05-18","2021-06-18");</v>
+        <v>("10","1","10","2022-03-21","2022-04-21");</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -11790,9 +11790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A007853-9D1A-4913-959D-CC14E6BFBA3B}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
build: changing librarySection to enum
</commit_message>
<xml_diff>
--- a/sql/02_dummy_data_generator.xlsx
+++ b/sql/02_dummy_data_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\budlib\budlib-api\sql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05B3D0E-7E3E-4953-8E85-19DADB2E4805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813B85EB-6946-4B3D-952B-B1B1A244BC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="704" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="605">
   <si>
     <t>book_id</t>
   </si>
@@ -1843,9 +1843,6 @@
   </si>
   <si>
     <t>Lee</t>
-  </si>
-  <si>
-    <t>PARENT</t>
   </si>
   <si>
     <t>$2a$10$..4RvEGzO5/TiayeVSm1lOTHqo456ZPPCrf7G7.eyPvndgkICr/tq</t>
@@ -2816,8 +2813,8 @@
         <v>1986</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="J2" t="s">
-        <v>601</v>
+      <c r="J2">
+        <v>0</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -2843,7 +2840,7 @@
 IF(N2="","NULL",_xlfn.CONCAT("""",N2,"""")),",",
 IF(O2="","NULL",_xlfn.CONCAT("""",O2,"""")),",",
 IF(P2="","NULL",_xlfn.CONCAT("""",P2,"""")),"),")</f>
-        <v>("Education Towards Freedom",NULL,"Rudel, Joan and Siegfried","Lanthorn Press, Peredur, East Grinstead, England","4","1986",NULL,NULL,NULL,"PARENT","1","0",NULL,NULL,NULL,NULL),</v>
+        <v>("Education Towards Freedom",NULL,"Rudel, Joan and Siegfried","Lanthorn Press, Peredur, East Grinstead, England","4","1986",NULL,NULL,NULL,"0","1","0",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -2863,8 +2860,8 @@
       <c r="H3" t="s">
         <v>412</v>
       </c>
-      <c r="J3" t="s">
-        <v>601</v>
+      <c r="J3">
+        <v>0</v>
       </c>
       <c r="K3">
         <v>4</v>
@@ -2890,7 +2887,7 @@
 IF(N3="","NULL",_xlfn.CONCAT("""",N3,"""")),",",
 IF(O3="","NULL",_xlfn.CONCAT("""",O3,"""")),",",
 IF(P3="","NULL",_xlfn.CONCAT("""",P3,"""")),"),")</f>
-        <v>("Bullying - Changing the Course of Your Child's Life",NULL,"Voors, William","Hazelden",NULL,"2000",NULL,"156838517X",NULL,"PARENT","4","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Bullying - Changing the Course of Your Child's Life",NULL,"Voors, William","Hazelden",NULL,"2000",NULL,"156838517X",NULL,"0","4","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -2910,8 +2907,8 @@
       <c r="H4" t="s">
         <v>413</v>
       </c>
-      <c r="J4" t="s">
-        <v>601</v>
+      <c r="J4">
+        <v>0</v>
       </c>
       <c r="K4">
         <v>9</v>
@@ -2921,7 +2918,7 @@
       </c>
       <c r="R4" t="str">
         <f t="shared" si="0"/>
-        <v>("Awakening Your Child's Natural Genius",NULL,"Armstrong, Thomas","Jeremy P. Tarcher, Inc., Los Angeles",NULL,"1991",NULL,"0874776082",NULL,"PARENT","9","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Awakening Your Child's Natural Genius",NULL,"Armstrong, Thomas","Jeremy P. Tarcher, Inc., Los Angeles",NULL,"1991",NULL,"0874776082",NULL,"0","9","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -2941,8 +2938,8 @@
       <c r="H5" t="s">
         <v>414</v>
       </c>
-      <c r="J5" t="s">
-        <v>601</v>
+      <c r="J5">
+        <v>0</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -2952,7 +2949,7 @@
       </c>
       <c r="R5" t="str">
         <f t="shared" si="0"/>
-        <v>("From Your Child's Teacher",NULL,"Bright, Robin","FP Hendricks Publishing Ltd.",NULL,"1998",NULL,"096829703X",NULL,"PARENT","3","0",NULL,NULL,NULL,NULL),</v>
+        <v>("From Your Child's Teacher",NULL,"Bright, Robin","FP Hendricks Publishing Ltd.",NULL,"1998",NULL,"096829703X",NULL,"0","3","0",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -2972,8 +2969,8 @@
       <c r="H6" t="s">
         <v>415</v>
       </c>
-      <c r="J6" t="s">
-        <v>601</v>
+      <c r="J6">
+        <v>0</v>
       </c>
       <c r="K6">
         <v>2</v>
@@ -2983,7 +2980,7 @@
       </c>
       <c r="R6" t="str">
         <f t="shared" si="0"/>
-        <v>("Parents Do Make a Difference",NULL,"Borba, Michele","Jossey-Bass",NULL,"1999",NULL,"0787946052",NULL,"PARENT","2","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Parents Do Make a Difference",NULL,"Borba, Michele","Jossey-Bass",NULL,"1999",NULL,"0787946052",NULL,"0","2","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -3003,8 +3000,8 @@
       <c r="H7" t="s">
         <v>416</v>
       </c>
-      <c r="J7" t="s">
-        <v>601</v>
+      <c r="J7">
+        <v>0</v>
       </c>
       <c r="K7">
         <v>4</v>
@@ -3014,7 +3011,7 @@
       </c>
       <c r="R7" t="str">
         <f t="shared" si="0"/>
-        <v>("Rythms of Learning",NULL,"Trostli, Roberto","Anthroposophic Press",NULL,"1998",NULL,"0880104511",NULL,"PARENT","4","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Rythms of Learning",NULL,"Trostli, Roberto","Anthroposophic Press",NULL,"1998",NULL,"0880104511",NULL,"0","4","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -3034,8 +3031,8 @@
       <c r="H8" t="s">
         <v>417</v>
       </c>
-      <c r="J8" t="s">
-        <v>601</v>
+      <c r="J8">
+        <v>0</v>
       </c>
       <c r="K8">
         <v>9</v>
@@ -3045,7 +3042,7 @@
       </c>
       <c r="R8" t="str">
         <f t="shared" si="0"/>
-        <v>("Parents as People",NULL,"Kane, Franklin G.","Aurora Publishers",NULL,"1987",NULL,"0889258201",NULL,"PARENT","9","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Parents as People",NULL,"Kane, Franklin G.","Aurora Publishers",NULL,"1987",NULL,"0889258201",NULL,"0","9","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -3065,8 +3062,8 @@
       <c r="H9" t="s">
         <v>418</v>
       </c>
-      <c r="J9" t="s">
-        <v>601</v>
+      <c r="J9">
+        <v>0</v>
       </c>
       <c r="K9">
         <v>10</v>
@@ -3076,7 +3073,7 @@
       </c>
       <c r="R9" t="str">
         <f t="shared" si="0"/>
-        <v>("Spelling for Parents",NULL,"Phenix, Jo / Scott-Dunne, Doreen","Pembrook Publishers Limited",NULL,"1994",NULL,"1551380196",NULL,"PARENT","10","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Spelling for Parents",NULL,"Phenix, Jo / Scott-Dunne, Doreen","Pembrook Publishers Limited",NULL,"1994",NULL,"1551380196",NULL,"0","10","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -3099,8 +3096,8 @@
       <c r="H10" t="s">
         <v>419</v>
       </c>
-      <c r="J10" t="s">
-        <v>601</v>
+      <c r="J10">
+        <v>0</v>
       </c>
       <c r="K10">
         <v>9</v>
@@ -3110,7 +3107,7 @@
       </c>
       <c r="R10" t="str">
         <f t="shared" si="0"/>
-        <v>("Lifeways - Working with Family Questions",NULL,"Davy, Gudrun / Voors, Bons","Hawthorn Press","3","1985",NULL,"0950706248",NULL,"PARENT","9","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Lifeways - Working with Family Questions",NULL,"Davy, Gudrun / Voors, Bons","Hawthorn Press","3","1985",NULL,"0950706248",NULL,"0","9","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -3130,8 +3127,8 @@
       <c r="H11" t="s">
         <v>420</v>
       </c>
-      <c r="J11" t="s">
-        <v>601</v>
+      <c r="J11">
+        <v>0</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -3141,7 +3138,7 @@
       </c>
       <c r="R11" t="str">
         <f t="shared" si="0"/>
-        <v>("Why Motor Skills Matter",NULL,"Losquadro Liddle, Tara","The McGraw-Hill Companies",NULL,"2004",NULL,"0071408185",NULL,"PARENT","1","0",NULL,NULL,NULL,NULL),</v>
+        <v>("Why Motor Skills Matter",NULL,"Losquadro Liddle, Tara","The McGraw-Hill Companies",NULL,"2004",NULL,"0071408185",NULL,"0","1","0",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -3161,8 +3158,8 @@
       <c r="H12" t="s">
         <v>421</v>
       </c>
-      <c r="J12" t="s">
-        <v>601</v>
+      <c r="J12">
+        <v>0</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -3172,7 +3169,7 @@
       </c>
       <c r="R12" t="str">
         <f t="shared" si="0"/>
-        <v>("A Guide to Child Health",NULL,"Gloeckler, Michaela / Goebel, Wolfgang","Floris Books",NULL,"1984",NULL,"0863151043",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("A Guide to Child Health",NULL,"Gloeckler, Michaela / Goebel, Wolfgang","Floris Books",NULL,"1984",NULL,"0863151043",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -3192,8 +3189,8 @@
       <c r="H13" t="s">
         <v>422</v>
       </c>
-      <c r="J13" t="s">
-        <v>601</v>
+      <c r="J13">
+        <v>0</v>
       </c>
       <c r="K13">
         <v>6</v>
@@ -3203,7 +3200,7 @@
       </c>
       <c r="R13" t="str">
         <f t="shared" si="0"/>
-        <v>("Navigating the Terrain of Childhood",NULL,"Petrash, Jack","Nova Institute Press",NULL,"2004",NULL,"0975855204",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Navigating the Terrain of Childhood",NULL,"Petrash, Jack","Nova Institute Press",NULL,"2004",NULL,"0975855204",NULL,"0","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -3224,8 +3221,8 @@
       <c r="I14" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="J14" t="s">
-        <v>601</v>
+      <c r="J14">
+        <v>0</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -3235,7 +3232,7 @@
       </c>
       <c r="R14" t="str">
         <f t="shared" si="0"/>
-        <v>("Healign Stories for Challenging Behaviour",NULL,"Perrow, Susan","Hawthorn Press",NULL,"2012",NULL,NULL,"9781903458785","PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Healign Stories for Challenging Behaviour",NULL,"Perrow, Susan","Hawthorn Press",NULL,"2012",NULL,NULL,"9781903458785","0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -3255,8 +3252,8 @@
       <c r="H15" t="s">
         <v>423</v>
       </c>
-      <c r="J15" t="s">
-        <v>601</v>
+      <c r="J15">
+        <v>0</v>
       </c>
       <c r="K15">
         <v>7</v>
@@ -3266,7 +3263,7 @@
       </c>
       <c r="R15" t="str">
         <f t="shared" si="0"/>
-        <v>("Hold on to Your Kids",NULL,"Neufeld, Gordon / Mate, Gabor","Vintage Canada",NULL,"2005",NULL,"0676974724",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Hold on to Your Kids",NULL,"Neufeld, Gordon / Mate, Gabor","Vintage Canada",NULL,"2005",NULL,"0676974724",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -3283,8 +3280,8 @@
         <v>1982</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="J16" t="s">
-        <v>601</v>
+      <c r="J16">
+        <v>0</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -3294,7 +3291,7 @@
       </c>
       <c r="R16" t="str">
         <f t="shared" si="0"/>
-        <v>("Echoes of a Dream",NULL,"Smith, Susan","Beacon Herald Fine Printing Division, Stratford, Ontario, Canada",NULL,"1982",NULL,NULL,NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Echoes of a Dream",NULL,"Smith, Susan","Beacon Herald Fine Printing Division, Stratford, Ontario, Canada",NULL,"1982",NULL,NULL,NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
@@ -3314,8 +3311,8 @@
       <c r="H17" t="s">
         <v>425</v>
       </c>
-      <c r="J17" t="s">
-        <v>601</v>
+      <c r="J17">
+        <v>0</v>
       </c>
       <c r="K17">
         <v>6</v>
@@ -3325,7 +3322,7 @@
       </c>
       <c r="R17" t="str">
         <f t="shared" si="0"/>
-        <v>("If Learning is so Natural, Why am I going to School?",NULL,"Nikiforuk, Andrew","Penguin Books",NULL,"1994",NULL,"0140242643",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("If Learning is so Natural, Why am I going to School?",NULL,"Nikiforuk, Andrew","Penguin Books",NULL,"1994",NULL,"0140242643",NULL,"0","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
@@ -3348,8 +3345,8 @@
       <c r="H18" t="s">
         <v>426</v>
       </c>
-      <c r="J18" t="s">
-        <v>601</v>
+      <c r="J18">
+        <v>0</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -3359,7 +3356,7 @@
       </c>
       <c r="R18" t="str">
         <f t="shared" si="0"/>
-        <v>("The Gift of Dyslexia",NULL,"Davis, Ronald D.","The Berkely Publishing Group","2","1997",NULL,"039952293X",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("The Gift of Dyslexia",NULL,"Davis, Ronald D.","The Berkely Publishing Group","2","1997",NULL,"039952293X",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
@@ -3379,8 +3376,8 @@
       <c r="H19" t="s">
         <v>427</v>
       </c>
-      <c r="J19" t="s">
-        <v>601</v>
+      <c r="J19">
+        <v>0</v>
       </c>
       <c r="K19">
         <v>7</v>
@@ -3390,7 +3387,7 @@
       </c>
       <c r="R19" t="str">
         <f t="shared" si="0"/>
-        <v>("the Out-of-Sync Child",NULL,"Stock Kranowitz, Carol","The Berkely Publishing Group",NULL,"2005",NULL,"0399531653",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("the Out-of-Sync Child",NULL,"Stock Kranowitz, Carol","The Berkely Publishing Group",NULL,"2005",NULL,"0399531653",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
@@ -3409,8 +3406,8 @@
       <c r="H20" t="s">
         <v>428</v>
       </c>
-      <c r="J20" t="s">
-        <v>601</v>
+      <c r="J20">
+        <v>0</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -3420,7 +3417,7 @@
       </c>
       <c r="R20" t="str">
         <f t="shared" si="0"/>
-        <v>("The Optimistic Child",NULL,"Seligman, Martin E.","Harper Perennial",NULL,"1995",NULL,"0060977094",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("The Optimistic Child",NULL,"Seligman, Martin E.","Harper Perennial",NULL,"1995",NULL,"0060977094",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -3439,8 +3436,8 @@
       <c r="H21" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="J21" t="s">
-        <v>601</v>
+      <c r="J21">
+        <v>0</v>
       </c>
       <c r="K21">
         <v>4</v>
@@ -3450,7 +3447,7 @@
       </c>
       <c r="R21" t="str">
         <f t="shared" si="0"/>
-        <v>("365 Outdoor Activities",NULL,"Bennett, Steve and Ruth","Bob Adams, Inc., Publishers",NULL,"1993",NULL,"1558502602",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("365 Outdoor Activities",NULL,"Bennett, Steve and Ruth","Bob Adams, Inc., Publishers",NULL,"1993",NULL,"1558502602",NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
@@ -3469,8 +3466,8 @@
       <c r="H22" t="s">
         <v>429</v>
       </c>
-      <c r="J22" t="s">
-        <v>601</v>
+      <c r="J22">
+        <v>0</v>
       </c>
       <c r="K22">
         <v>10</v>
@@ -3480,7 +3477,7 @@
       </c>
       <c r="R22" t="str">
         <f t="shared" si="0"/>
-        <v>("Kids are Worth it!",NULL,"Coloroso, Barbara","Somerville House Publishing",NULL,"1994",NULL,"0921051743",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Kids are Worth it!",NULL,"Coloroso, Barbara","Somerville House Publishing",NULL,"1994",NULL,"0921051743",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -3499,8 +3496,8 @@
       <c r="H23" t="s">
         <v>430</v>
       </c>
-      <c r="J23" t="s">
-        <v>601</v>
+      <c r="J23">
+        <v>0</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -3510,7 +3507,7 @@
       </c>
       <c r="R23" t="str">
         <f t="shared" si="0"/>
-        <v>("How to Keep Your Teenager Out of Troubl and What to Do if You Can't",NULL,"Bernstein, Neil I.","Workman Publishing",NULL,"2001",NULL,"0761115706",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("How to Keep Your Teenager Out of Troubl and What to Do if You Can't",NULL,"Bernstein, Neil I.","Workman Publishing",NULL,"2001",NULL,"0761115706",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -3529,8 +3526,8 @@
       <c r="H24" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="J24" t="s">
-        <v>601</v>
+      <c r="J24">
+        <v>0</v>
       </c>
       <c r="K24">
         <v>8</v>
@@ -3540,7 +3537,7 @@
       </c>
       <c r="R24" t="str">
         <f t="shared" si="0"/>
-        <v>("Commonsense Schooling",NULL,"Wilkinson, Roy","The Robinswook Press",NULL,"1990",NULL,"186981081",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Commonsense Schooling",NULL,"Wilkinson, Roy","The Robinswook Press",NULL,"1990",NULL,"186981081",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
@@ -3559,8 +3556,8 @@
       <c r="H25" t="s">
         <v>432</v>
       </c>
-      <c r="J25" t="s">
-        <v>601</v>
+      <c r="J25">
+        <v>0</v>
       </c>
       <c r="K25">
         <v>4</v>
@@ -3570,7 +3567,7 @@
       </c>
       <c r="R25" t="str">
         <f t="shared" si="0"/>
-        <v>("Grading the Teacher",NULL,"Jacobs, Nellie","Penguin Books",NULL,"1996",NULL,"0140256121",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Grading the Teacher",NULL,"Jacobs, Nellie","Penguin Books",NULL,"1996",NULL,"0140256121",NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
@@ -3589,8 +3586,8 @@
       <c r="H26" t="s">
         <v>433</v>
       </c>
-      <c r="J26" t="s">
-        <v>601</v>
+      <c r="J26">
+        <v>0</v>
       </c>
       <c r="K26">
         <v>6</v>
@@ -3600,7 +3597,7 @@
       </c>
       <c r="R26" t="str">
         <f t="shared" si="0"/>
-        <v>("On the Threshold of Adolsescence",NULL,"Koepke, Hermann","Anthroposophic Press",NULL,"1992",NULL,"0880103574",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("On the Threshold of Adolsescence",NULL,"Koepke, Hermann","Anthroposophic Press",NULL,"1992",NULL,"0880103574",NULL,"0","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
@@ -3622,8 +3619,8 @@
       <c r="H27" t="s">
         <v>434</v>
       </c>
-      <c r="J27" t="s">
-        <v>601</v>
+      <c r="J27">
+        <v>0</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -3633,7 +3630,7 @@
       </c>
       <c r="R27" t="str">
         <f t="shared" si="0"/>
-        <v>("Thirteen to Nineteen - Discovering the Light ",NULL,"Sleigh, Julian","Floris Books","2","1989",NULL,"0863150780",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Thirteen to Nineteen - Discovering the Light ",NULL,"Sleigh, Julian","Floris Books","2","1989",NULL,"0863150780",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
@@ -3652,8 +3649,8 @@
       <c r="H28" t="s">
         <v>435</v>
       </c>
-      <c r="J28" t="s">
-        <v>601</v>
+      <c r="J28">
+        <v>0</v>
       </c>
       <c r="K28">
         <v>9</v>
@@ -3663,7 +3660,7 @@
       </c>
       <c r="R28" t="str">
         <f t="shared" si="0"/>
-        <v>("Closing the Gap - A Strategy for Bringing Parents and Teens Together",NULL,"McGraw, Jay","Fireside",NULL,"2001",NULL,"0743224698",NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("Closing the Gap - A Strategy for Bringing Parents and Teens Together",NULL,"McGraw, Jay","Fireside",NULL,"2001",NULL,"0743224698",NULL,"0","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -3685,8 +3682,8 @@
       <c r="H29" t="s">
         <v>436</v>
       </c>
-      <c r="J29" t="s">
-        <v>601</v>
+      <c r="J29">
+        <v>0</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -3696,7 +3693,7 @@
       </c>
       <c r="R29" t="str">
         <f t="shared" si="0"/>
-        <v>("Voyage Through Childhood Into the Adult World",NULL,"Frommer, Eva A.","Hawthorn Press","2","1994",NULL,"1869890590",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Voyage Through Childhood Into the Adult World",NULL,"Frommer, Eva A.","Hawthorn Press","2","1994",NULL,"1869890590",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -3715,8 +3712,8 @@
       <c r="H30" t="s">
         <v>437</v>
       </c>
-      <c r="J30" t="s">
-        <v>601</v>
+      <c r="J30">
+        <v>0</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -3726,7 +3723,7 @@
       </c>
       <c r="R30" t="str">
         <f t="shared" si="0"/>
-        <v>("More Lifeways - Finding Support and Inspiration I Family Life",NULL,"Smith, Patti / Eklund Schaefer, Signe","Hawthorn Press",NULL,"1997",NULL,"1869890868",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("More Lifeways - Finding Support and Inspiration I Family Life",NULL,"Smith, Patti / Eklund Schaefer, Signe","Hawthorn Press",NULL,"1997",NULL,"1869890868",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -3745,8 +3742,8 @@
       <c r="H31" t="s">
         <v>438</v>
       </c>
-      <c r="J31" t="s">
-        <v>601</v>
+      <c r="J31">
+        <v>0</v>
       </c>
       <c r="K31">
         <v>8</v>
@@ -3756,7 +3753,7 @@
       </c>
       <c r="R31" t="str">
         <f t="shared" si="0"/>
-        <v>("The Motherly and Fatherly Roles in Education ",NULL,"Gabert, Erich","Anthroposophic Press",NULL,"1988",NULL,"0880101997",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("The Motherly and Fatherly Roles in Education ",NULL,"Gabert, Erich","Anthroposophic Press",NULL,"1988",NULL,"0880101997",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
@@ -3775,8 +3772,8 @@
       <c r="H32" t="s">
         <v>439</v>
       </c>
-      <c r="J32" t="s">
-        <v>601</v>
+      <c r="J32">
+        <v>0</v>
       </c>
       <c r="K32">
         <v>8</v>
@@ -3786,7 +3783,7 @@
       </c>
       <c r="R32" t="str">
         <f t="shared" si="0"/>
-        <v>("Raising a Daughter",NULL,"Elium, Jeanne and Don","Celestial Arts",NULL,"1994",NULL,"0890877084",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Raising a Daughter",NULL,"Elium, Jeanne and Don","Celestial Arts",NULL,"1994",NULL,"0890877084",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
@@ -3805,8 +3802,8 @@
       <c r="I33" t="s">
         <v>440</v>
       </c>
-      <c r="J33" t="s">
-        <v>601</v>
+      <c r="J33">
+        <v>0</v>
       </c>
       <c r="K33">
         <v>2</v>
@@ -3816,7 +3813,7 @@
       </c>
       <c r="R33" t="str">
         <f t="shared" si="0"/>
-        <v>("Adventures in Parenting",NULL,"Ross, Rachel C.","The Association of Waldorf Schools of North America (AWSNA)",NULL,"2008",NULL,NULL,"9781888364764","PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Adventures in Parenting",NULL,"Ross, Rachel C.","The Association of Waldorf Schools of North America (AWSNA)",NULL,"2008",NULL,NULL,"9781888364764","0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
@@ -3835,8 +3832,8 @@
       <c r="H34" t="s">
         <v>441</v>
       </c>
-      <c r="J34" t="s">
-        <v>601</v>
+      <c r="J34">
+        <v>0</v>
       </c>
       <c r="K34">
         <v>10</v>
@@ -3846,7 +3843,7 @@
       </c>
       <c r="R34" t="str">
         <f t="shared" si="0"/>
-        <v>("Spiritual Parenting - A Loving Guide for the New Age Parent",NULL,"Carroll, David","Paragon House, New York",NULL,"1990",NULL,"1557781125",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Spiritual Parenting - A Loving Guide for the New Age Parent",NULL,"Carroll, David","Paragon House, New York",NULL,"1990",NULL,"1557781125",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
@@ -3865,8 +3862,8 @@
       <c r="H35" s="5" t="s">
         <v>442</v>
       </c>
-      <c r="J35" t="s">
-        <v>601</v>
+      <c r="J35">
+        <v>0</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -3876,7 +3873,7 @@
       </c>
       <c r="R35" t="str">
         <f t="shared" si="0"/>
-        <v>("Reading Magic",NULL,"Fox, Mem","Harcourt, Inc.",NULL,"2001",NULL,"015601763",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Reading Magic",NULL,"Fox, Mem","Harcourt, Inc.",NULL,"2001",NULL,"015601763",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
@@ -3895,8 +3892,8 @@
       <c r="H36" t="s">
         <v>443</v>
       </c>
-      <c r="J36" t="s">
-        <v>601</v>
+      <c r="J36">
+        <v>0</v>
       </c>
       <c r="K36">
         <v>10</v>
@@ -3906,7 +3903,7 @@
       </c>
       <c r="R36" t="str">
         <f t="shared" si="0"/>
-        <v>("Raising a Creative Child",NULL,"MacGregor, Cynthia","Carol Publishing Group",NULL,"1996",NULL,"0806517417",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Raising a Creative Child",NULL,"MacGregor, Cynthia","Carol Publishing Group",NULL,"1996",NULL,"0806517417",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
@@ -3925,8 +3922,8 @@
       <c r="H37" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="J37" t="s">
-        <v>601</v>
+      <c r="J37">
+        <v>0</v>
       </c>
       <c r="K37">
         <v>7</v>
@@ -3936,7 +3933,7 @@
       </c>
       <c r="R37" t="str">
         <f t="shared" si="0"/>
-        <v>("Parenting for a Healthy Future",NULL,"Coplen, Dotty","Hawthorn Press",NULL,"1995",NULL,"186989531",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Parenting for a Healthy Future",NULL,"Coplen, Dotty","Hawthorn Press",NULL,"1995",NULL,"186989531",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.3">
@@ -3955,8 +3952,8 @@
       <c r="H38" t="s">
         <v>445</v>
       </c>
-      <c r="J38" t="s">
-        <v>601</v>
+      <c r="J38">
+        <v>0</v>
       </c>
       <c r="K38">
         <v>8</v>
@@ -3966,7 +3963,7 @@
       </c>
       <c r="R38" t="str">
         <f t="shared" si="0"/>
-        <v>("How to Talk to Kids will Listen and Listen so Kids Will Talk",NULL,"Faber, Adele / Mazlish, Elaine","Avon Books",NULL,"1980",NULL,"0380570009",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("How to Talk to Kids will Listen and Listen so Kids Will Talk",NULL,"Faber, Adele / Mazlish, Elaine","Avon Books",NULL,"1980",NULL,"0380570009",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.3">
@@ -3985,8 +3982,8 @@
       <c r="H39" t="s">
         <v>446</v>
       </c>
-      <c r="J39" t="s">
-        <v>601</v>
+      <c r="J39">
+        <v>0</v>
       </c>
       <c r="K39">
         <v>8</v>
@@ -3996,7 +3993,7 @@
       </c>
       <c r="R39" t="str">
         <f t="shared" si="0"/>
-        <v>("School's Out",NULL,"Nikiforuk, Andrew","Macfarlane Walter and Ross, Toronto",NULL,"1993",NULL,"0921912838",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("School's Out",NULL,"Nikiforuk, Andrew","Macfarlane Walter and Ross, Toronto",NULL,"1993",NULL,"0921912838",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.3">
@@ -4015,8 +4012,8 @@
       <c r="H40" t="s">
         <v>447</v>
       </c>
-      <c r="J40" t="s">
-        <v>601</v>
+      <c r="J40">
+        <v>0</v>
       </c>
       <c r="K40">
         <v>2</v>
@@ -4026,7 +4023,7 @@
       </c>
       <c r="R40" t="str">
         <f t="shared" si="0"/>
-        <v>("Children's Symptoms",NULL,"Valman, Bernard / Youger-Lewis Catherine","Reader's Digest Association (Canada) Ltd. Montreal",NULL,"1998",NULL,"0888506120",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Children's Symptoms",NULL,"Valman, Bernard / Youger-Lewis Catherine","Reader's Digest Association (Canada) Ltd. Montreal",NULL,"1998",NULL,"0888506120",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
@@ -4045,8 +4042,8 @@
       <c r="H41" t="s">
         <v>448</v>
       </c>
-      <c r="J41" t="s">
-        <v>601</v>
+      <c r="J41">
+        <v>0</v>
       </c>
       <c r="K41">
         <v>10</v>
@@ -4056,7 +4053,7 @@
       </c>
       <c r="R41" t="str">
         <f t="shared" si="0"/>
-        <v>("Families Apart - Ten Keys to Successful Co-Parenting",NULL,"Blau, Melinda","The Berkely Publishing Group",NULL,"1995",NULL,"039952150X",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Families Apart - Ten Keys to Successful Co-Parenting",NULL,"Blau, Melinda","The Berkely Publishing Group",NULL,"1995",NULL,"039952150X",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
@@ -4075,8 +4072,8 @@
       <c r="H42" t="s">
         <v>449</v>
       </c>
-      <c r="J42" t="s">
-        <v>601</v>
+      <c r="J42">
+        <v>0</v>
       </c>
       <c r="K42">
         <v>10</v>
@@ -4086,7 +4083,7 @@
       </c>
       <c r="R42" t="str">
         <f t="shared" si="0"/>
-        <v>("The Complete Kid's Allergy and Asthma Guide",NULL,"Gold, Milton","Robert Rose Inc.",NULL,"2003",NULL,"0778800784",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("The Complete Kid's Allergy and Asthma Guide",NULL,"Gold, Milton","Robert Rose Inc.",NULL,"2003",NULL,"0778800784",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
@@ -4105,8 +4102,8 @@
       <c r="H43" t="s">
         <v>450</v>
       </c>
-      <c r="J43" t="s">
-        <v>601</v>
+      <c r="J43">
+        <v>0</v>
       </c>
       <c r="K43">
         <v>5</v>
@@ -4116,7 +4113,7 @@
       </c>
       <c r="R43" t="str">
         <f t="shared" si="0"/>
-        <v>("Sharing Nature with Children",NULL,"Cornell, Joseph","Dawn Publications",NULL,"1979",NULL,"0916124142",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Sharing Nature with Children",NULL,"Cornell, Joseph","Dawn Publications",NULL,"1979",NULL,"0916124142",NULL,"0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
@@ -4135,8 +4132,8 @@
       <c r="H44" t="s">
         <v>451</v>
       </c>
-      <c r="J44" t="s">
-        <v>601</v>
+      <c r="J44">
+        <v>0</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -4146,7 +4143,7 @@
       </c>
       <c r="R44" t="str">
         <f t="shared" si="0"/>
-        <v>("How Childern Play",NULL,"Haller, Ingeborg","Floris Books",NULL,"1991",NULL,"0863151272",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("How Childern Play",NULL,"Haller, Ingeborg","Floris Books",NULL,"1991",NULL,"0863151272",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
@@ -4165,8 +4162,8 @@
       <c r="H45" t="s">
         <v>452</v>
       </c>
-      <c r="J45" t="s">
-        <v>601</v>
+      <c r="J45">
+        <v>0</v>
       </c>
       <c r="K45">
         <v>2</v>
@@ -4176,7 +4173,7 @@
       </c>
       <c r="R45" t="str">
         <f t="shared" si="0"/>
-        <v>("Remember the Light",NULL,"Fisher, Mary Pat","Fenton Valley Press",NULL,"1986",NULL,"0961514973",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Remember the Light",NULL,"Fisher, Mary Pat","Fenton Valley Press",NULL,"1986",NULL,"0961514973",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
@@ -4195,8 +4192,8 @@
       <c r="H46" t="s">
         <v>453</v>
       </c>
-      <c r="J46" t="s">
-        <v>601</v>
+      <c r="J46">
+        <v>0</v>
       </c>
       <c r="K46">
         <v>5</v>
@@ -4206,7 +4203,7 @@
       </c>
       <c r="R46" t="str">
         <f t="shared" si="0"/>
-        <v>("Making Soft Toys",NULL,"Jaffke, Freya","Celestial Arts",NULL,"1981",NULL,"0897420446",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Making Soft Toys",NULL,"Jaffke, Freya","Celestial Arts",NULL,"1981",NULL,"0897420446",NULL,"0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
@@ -4228,8 +4225,8 @@
       <c r="H47" s="5" t="s">
         <v>454</v>
       </c>
-      <c r="J47" t="s">
-        <v>601</v>
+      <c r="J47">
+        <v>0</v>
       </c>
       <c r="K47">
         <v>4</v>
@@ -4239,7 +4236,7 @@
       </c>
       <c r="R47" t="str">
         <f t="shared" si="0"/>
-        <v>("Summer",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"094626023",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Summer",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"094626023",NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
@@ -4258,8 +4255,8 @@
       <c r="H48" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="J48" t="s">
-        <v>601</v>
+      <c r="J48">
+        <v>0</v>
       </c>
       <c r="K48">
         <v>4</v>
@@ -4269,7 +4266,7 @@
       </c>
       <c r="R48" t="str">
         <f t="shared" si="0"/>
-        <v>("Conception Birth and Early Childhood",NULL,"Glas, Norbert","Anthroposophic Press",NULL,"1983",NULL,"091142548",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Conception Birth and Early Childhood",NULL,"Glas, Norbert","Anthroposophic Press",NULL,"1983",NULL,"091142548",NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
@@ -4288,8 +4285,8 @@
       <c r="H49" t="s">
         <v>456</v>
       </c>
-      <c r="J49" t="s">
-        <v>601</v>
+      <c r="J49">
+        <v>0</v>
       </c>
       <c r="K49">
         <v>5</v>
@@ -4299,7 +4296,7 @@
       </c>
       <c r="R49" t="str">
         <f t="shared" si="0"/>
-        <v>("Children at Play",NULL,"Britz-Crecelius, Heidi","Parkstreet Press, Rochester, Vermont",NULL,"1996",NULL,"0892816295",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Children at Play",NULL,"Britz-Crecelius, Heidi","Parkstreet Press, Rochester, Vermont",NULL,"1996",NULL,"0892816295",NULL,"0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.3">
@@ -4318,8 +4315,8 @@
       <c r="H50" t="s">
         <v>457</v>
       </c>
-      <c r="J50" t="s">
-        <v>601</v>
+      <c r="J50">
+        <v>0</v>
       </c>
       <c r="K50">
         <v>4</v>
@@ -4329,7 +4326,7 @@
       </c>
       <c r="R50" t="str">
         <f t="shared" si="0"/>
-        <v>("50 Simple Things Kids Can Do to Save The Earth",NULL,"Javna, John","Andrews and McMeel",NULL,"1990",NULL,"0836223012",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("50 Simple Things Kids Can Do to Save The Earth",NULL,"Javna, John","Andrews and McMeel",NULL,"1990",NULL,"0836223012",NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
@@ -4348,8 +4345,8 @@
       <c r="H51" t="s">
         <v>458</v>
       </c>
-      <c r="J51" t="s">
-        <v>601</v>
+      <c r="J51">
+        <v>0</v>
       </c>
       <c r="K51">
         <v>7</v>
@@ -4359,7 +4356,7 @@
       </c>
       <c r="R51" t="str">
         <f t="shared" si="0"/>
-        <v>("Sewing for Baby",NULL,"Martensson, Kerstin","?",NULL,"1987",NULL,"0913212105",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Sewing for Baby",NULL,"Martensson, Kerstin","?",NULL,"1987",NULL,"0913212105",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.3">
@@ -4378,8 +4375,8 @@
       <c r="H52" t="s">
         <v>459</v>
       </c>
-      <c r="J52" t="s">
-        <v>601</v>
+      <c r="J52">
+        <v>0</v>
       </c>
       <c r="K52">
         <v>9</v>
@@ -4389,7 +4386,7 @@
       </c>
       <c r="R52" t="str">
         <f t="shared" si="0"/>
-        <v>("Advent for Children",NULL,"Jaffke, Freya","Floris Books",NULL,"1979",NULL,"0863150098",NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("Advent for Children",NULL,"Jaffke, Freya","Floris Books",NULL,"1979",NULL,"0863150098",NULL,"0","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
@@ -4408,8 +4405,8 @@
       <c r="H53" t="s">
         <v>460</v>
       </c>
-      <c r="J53" t="s">
-        <v>601</v>
+      <c r="J53">
+        <v>0</v>
       </c>
       <c r="K53">
         <v>6</v>
@@ -4419,7 +4416,7 @@
       </c>
       <c r="R53" t="str">
         <f t="shared" si="0"/>
-        <v>("Making Dolls",NULL,"Reinckens, Sunnhild","Floris Books",NULL,"1989",NULL,"0863150934",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Making Dolls",NULL,"Reinckens, Sunnhild","Floris Books",NULL,"1989",NULL,"0863150934",NULL,"0","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
@@ -4438,8 +4435,8 @@
       <c r="H54" t="s">
         <v>461</v>
       </c>
-      <c r="J54" t="s">
-        <v>601</v>
+      <c r="J54">
+        <v>0</v>
       </c>
       <c r="K54">
         <v>2</v>
@@ -4449,7 +4446,7 @@
       </c>
       <c r="R54" t="str">
         <f t="shared" si="0"/>
-        <v>("The Nature Corner",NULL,"v Leeuwen, M / Moeskops, J","Floris Books",NULL,"1990",NULL,"0863151116",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("The Nature Corner",NULL,"v Leeuwen, M / Moeskops, J","Floris Books",NULL,"1990",NULL,"0863151116",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
@@ -4468,8 +4465,8 @@
       <c r="H55" t="s">
         <v>462</v>
       </c>
-      <c r="J55" t="s">
-        <v>601</v>
+      <c r="J55">
+        <v>0</v>
       </c>
       <c r="K55">
         <v>3</v>
@@ -4479,7 +4476,7 @@
       </c>
       <c r="R55" t="str">
         <f t="shared" si="0"/>
-        <v>("The Christmas Craft Book",NULL,"Berger, Thomas","Floris Books",NULL,"2001",NULL,"0863151108",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("The Christmas Craft Book",NULL,"Berger, Thomas","Floris Books",NULL,"2001",NULL,"0863151108",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.3">
@@ -4498,8 +4495,8 @@
       <c r="H56" t="s">
         <v>463</v>
       </c>
-      <c r="J56" t="s">
-        <v>601</v>
+      <c r="J56">
+        <v>0</v>
       </c>
       <c r="K56">
         <v>9</v>
@@ -4509,7 +4506,7 @@
       </c>
       <c r="R56" t="str">
         <f t="shared" si="0"/>
-        <v>("The Harvest Craft Book",NULL,"Berger, Thomas","Floris Books",NULL,"1993",NULL,"0863151477",NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("The Harvest Craft Book",NULL,"Berger, Thomas","Floris Books",NULL,"1993",NULL,"0863151477",NULL,"0","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.3">
@@ -4528,8 +4525,8 @@
       <c r="H57" t="s">
         <v>464</v>
       </c>
-      <c r="J57" t="s">
-        <v>601</v>
+      <c r="J57">
+        <v>0</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -4539,7 +4536,7 @@
       </c>
       <c r="R57" t="str">
         <f t="shared" si="0"/>
-        <v>("The Easter Craft Book",NULL,"Berger, Thomas and Petra","Floris Books",NULL,"1994",NULL,"0863151612",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("The Easter Craft Book",NULL,"Berger, Thomas and Petra","Floris Books",NULL,"1994",NULL,"0863151612",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
@@ -4558,8 +4555,8 @@
       <c r="H58" t="s">
         <v>465</v>
       </c>
-      <c r="J58" t="s">
-        <v>601</v>
+      <c r="J58">
+        <v>0</v>
       </c>
       <c r="K58">
         <v>6</v>
@@ -4569,7 +4566,7 @@
       </c>
       <c r="R58" t="str">
         <f t="shared" si="0"/>
-        <v>("The Gnome Graft Book",NULL,"Berger, Thomas and Petra","Floris Books",NULL,"2001",NULL,"0863153003",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("The Gnome Graft Book",NULL,"Berger, Thomas and Petra","Floris Books",NULL,"2001",NULL,"0863153003",NULL,"0","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
@@ -4591,8 +4588,8 @@
       <c r="H59" t="s">
         <v>466</v>
       </c>
-      <c r="J59" t="s">
-        <v>601</v>
+      <c r="J59">
+        <v>0</v>
       </c>
       <c r="K59">
         <v>1</v>
@@ -4602,7 +4599,7 @@
       </c>
       <c r="R59" t="str">
         <f t="shared" si="0"/>
-        <v>("Festivals with Children",NULL,"Barz, Brigitte","Floris Books","2","1991",NULL,"0863150551",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Festivals with Children",NULL,"Barz, Brigitte","Floris Books","2","1991",NULL,"0863150551",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
@@ -4624,8 +4621,8 @@
       <c r="H60" t="s">
         <v>467</v>
       </c>
-      <c r="J60" t="s">
-        <v>601</v>
+      <c r="J60">
+        <v>0</v>
       </c>
       <c r="K60">
         <v>5</v>
@@ -4635,7 +4632,7 @@
       </c>
       <c r="R60" t="str">
         <f t="shared" si="0"/>
-        <v>("Autumn",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"0946206031",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Autumn",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"0946206031",NULL,"0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
@@ -4657,8 +4654,8 @@
       <c r="H61" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="J61" t="s">
-        <v>601</v>
+      <c r="J61">
+        <v>0</v>
       </c>
       <c r="K61">
         <v>8</v>
@@ -4668,7 +4665,7 @@
       </c>
       <c r="R61" t="str">
         <f t="shared" si="0"/>
-        <v>("Gateways",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"094626058",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Gateways",NULL,"Steiner Schools","Wynstones Press, Brookthorpe, Glaucester, UK","2","1983",NULL,"094626058",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
@@ -4687,8 +4684,8 @@
       <c r="H62" t="s">
         <v>424</v>
       </c>
-      <c r="J62" t="s">
-        <v>601</v>
+      <c r="J62">
+        <v>0</v>
       </c>
       <c r="K62">
         <v>9</v>
@@ -4698,7 +4695,7 @@
       </c>
       <c r="R62" t="str">
         <f t="shared" si="0"/>
-        <v>("Stories They'll Remember",NULL,"Lord, Frank M.","Treehouse Communication Inc.",NULL,"1987",NULL,NULL,NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("Stories They'll Remember",NULL,"Lord, Frank M.","Treehouse Communication Inc.",NULL,"1987",NULL,NULL,NULL,"0","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.3">
@@ -4717,8 +4714,8 @@
       <c r="H63" t="s">
         <v>469</v>
       </c>
-      <c r="J63" t="s">
-        <v>601</v>
+      <c r="J63">
+        <v>0</v>
       </c>
       <c r="K63">
         <v>5</v>
@@ -4728,7 +4725,7 @@
       </c>
       <c r="R63" t="str">
         <f t="shared" si="0"/>
-        <v>("Natural Childhood",NULL,"Thomson, John","Fireside, Simon &amp; Schuster Inc.",NULL,"1994",NULL,"0020207395",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Natural Childhood",NULL,"Thomson, John","Fireside, Simon &amp; Schuster Inc.",NULL,"1994",NULL,"0020207395",NULL,"0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
@@ -4747,8 +4744,8 @@
       <c r="H64" t="s">
         <v>470</v>
       </c>
-      <c r="J64" t="s">
-        <v>601</v>
+      <c r="J64">
+        <v>0</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -4758,7 +4755,7 @@
       </c>
       <c r="R64" t="str">
         <f t="shared" si="0"/>
-        <v>("Festivals Family and Food",NULL,"Carey, Diana / Large, Judy","Hawthorn Press",NULL,"1983",NULL,"095070623X",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Festivals Family and Food",NULL,"Carey, Diana / Large, Judy","Hawthorn Press",NULL,"1983",NULL,"095070623X",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.3">
@@ -4774,8 +4771,8 @@
       <c r="H65" t="s">
         <v>471</v>
       </c>
-      <c r="J65" t="s">
-        <v>601</v>
+      <c r="J65">
+        <v>0</v>
       </c>
       <c r="K65">
         <v>1</v>
@@ -4785,7 +4782,7 @@
       </c>
       <c r="R65" t="str">
         <f t="shared" si="0"/>
-        <v>("All Year Round",NULL,"Druitt, Ann / Fynes-Clinton, Christine / Rowling, Maije","Hawthorn Press",NULL,NULL,NULL,"1869890477",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("All Year Round",NULL,"Druitt, Ann / Fynes-Clinton, Christine / Rowling, Maije","Hawthorn Press",NULL,NULL,NULL,"1869890477",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.3">
@@ -4804,8 +4801,8 @@
       <c r="H66" t="s">
         <v>472</v>
       </c>
-      <c r="J66" t="s">
-        <v>601</v>
+      <c r="J66">
+        <v>0</v>
       </c>
       <c r="K66">
         <v>3</v>
@@ -4815,7 +4812,7 @@
       </c>
       <c r="R66" t="str">
         <f t="shared" si="0"/>
-        <v>("Days, Weeks and Months",NULL,"Joy, Margaret","Faber and Faber, London Boston",NULL,"1984",NULL,"0571131719",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Days, Weeks and Months",NULL,"Joy, Margaret","Faber and Faber, London Boston",NULL,"1984",NULL,"0571131719",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.3">
@@ -4834,8 +4831,8 @@
       <c r="H67" t="s">
         <v>473</v>
       </c>
-      <c r="J67" t="s">
-        <v>601</v>
+      <c r="J67">
+        <v>0</v>
       </c>
       <c r="K67">
         <v>7</v>
@@ -4861,7 +4858,7 @@
 IF(N67="","NULL",_xlfn.CONCAT("""",N67,"""")),",",
 IF(O67="","NULL",_xlfn.CONCAT("""",O67,"""")),",",
 IF(P67="","NULL",_xlfn.CONCAT("""",P67,"""")),"),")</f>
-        <v>("The Children's Year",NULL,"Cooper, Stephanie / Fynes-Clinton, Christine / Rowling, Marye","Hawthorn Press",NULL,"1986",NULL,"1869890000",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("The Children's Year",NULL,"Cooper, Stephanie / Fynes-Clinton, Christine / Rowling, Marye","Hawthorn Press",NULL,"1986",NULL,"1869890000",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.3">
@@ -4880,8 +4877,8 @@
       <c r="H68" t="s">
         <v>474</v>
       </c>
-      <c r="J68" t="s">
-        <v>601</v>
+      <c r="J68">
+        <v>0</v>
       </c>
       <c r="K68">
         <v>6</v>
@@ -4891,7 +4888,7 @@
       </c>
       <c r="R68" t="str">
         <f t="shared" si="1"/>
-        <v>("Understanding Waldorf Education ",NULL,"Petrash, Jack","Gryphon House Inc.",NULL,"2002",NULL,"0876592469",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Understanding Waldorf Education ",NULL,"Petrash, Jack","Gryphon House Inc.",NULL,"2002",NULL,"0876592469",NULL,"0","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.3">
@@ -4910,8 +4907,8 @@
       <c r="H69" t="s">
         <v>475</v>
       </c>
-      <c r="J69" t="s">
-        <v>601</v>
+      <c r="J69">
+        <v>0</v>
       </c>
       <c r="K69">
         <v>8</v>
@@ -4921,7 +4918,7 @@
       </c>
       <c r="R69" t="str">
         <f t="shared" si="1"/>
-        <v>("Parent's Guide to the Best Books for Children",NULL,"Lipson, Eden Ross","Times Books",NULL,"1988",NULL,"0812917758",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Parent's Guide to the Best Books for Children",NULL,"Lipson, Eden Ross","Times Books",NULL,"1988",NULL,"0812917758",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.3">
@@ -4940,8 +4937,8 @@
       <c r="H70" t="s">
         <v>476</v>
       </c>
-      <c r="J70" t="s">
-        <v>601</v>
+      <c r="J70">
+        <v>0</v>
       </c>
       <c r="K70">
         <v>10</v>
@@ -4951,7 +4948,7 @@
       </c>
       <c r="R70" t="str">
         <f t="shared" si="1"/>
-        <v>("Waldorf Education - A Family Guide",NULL,"Johnson Fenner, Pamela / Rivers, Karen L.","Michealmas Press",NULL,"1992",NULL,"0964783215",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Waldorf Education - A Family Guide",NULL,"Johnson Fenner, Pamela / Rivers, Karen L.","Michealmas Press",NULL,"1992",NULL,"0964783215",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.3">
@@ -4970,8 +4967,8 @@
       <c r="H71" t="s">
         <v>424</v>
       </c>
-      <c r="J71" t="s">
-        <v>601</v>
+      <c r="J71">
+        <v>0</v>
       </c>
       <c r="K71">
         <v>2</v>
@@ -4981,7 +4978,7 @@
       </c>
       <c r="R71" t="str">
         <f t="shared" si="1"/>
-        <v>("Pentatonic Songs",NULL,"Lebret, Elisabeth","Waldorf Schools of Ontario",NULL,"1985",NULL,NULL,NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Pentatonic Songs",NULL,"Lebret, Elisabeth","Waldorf Schools of Ontario",NULL,"1985",NULL,NULL,NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.3">
@@ -5000,8 +4997,8 @@
       <c r="H72" t="s">
         <v>477</v>
       </c>
-      <c r="J72" t="s">
-        <v>601</v>
+      <c r="J72">
+        <v>0</v>
       </c>
       <c r="K72">
         <v>8</v>
@@ -5011,7 +5008,7 @@
       </c>
       <c r="R72" t="str">
         <f t="shared" si="1"/>
-        <v>("Painting with Children",NULL,"Muller, Brunhild","Floris Books",NULL,"1987",NULL,"0863150489",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Painting with Children",NULL,"Muller, Brunhild","Floris Books",NULL,"1987",NULL,"0863150489",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.3">
@@ -5030,8 +5027,8 @@
       <c r="H73" t="s">
         <v>424</v>
       </c>
-      <c r="J73" t="s">
-        <v>601</v>
+      <c r="J73">
+        <v>0</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -5041,7 +5038,7 @@
       </c>
       <c r="R73" t="str">
         <f t="shared" si="1"/>
-        <v>("Child and Man (Journal)",NULL,"Masters, Brian (Editor)","Imprint",NULL,"1995",NULL,NULL,NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Child and Man (Journal)",NULL,"Masters, Brian (Editor)","Imprint",NULL,"1995",NULL,NULL,NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.3">
@@ -5060,8 +5057,8 @@
       <c r="H74" t="s">
         <v>424</v>
       </c>
-      <c r="J74" t="s">
-        <v>601</v>
+      <c r="J74">
+        <v>0</v>
       </c>
       <c r="K74">
         <v>4</v>
@@ -5071,7 +5068,7 @@
       </c>
       <c r="R74" t="str">
         <f t="shared" si="1"/>
-        <v>("Rudolf Steiner Waldorf Education",NULL,"Steiner Schools","The Robinswook Press",NULL,"1989",NULL,NULL,NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Rudolf Steiner Waldorf Education",NULL,"Steiner Schools","The Robinswook Press",NULL,"1989",NULL,NULL,NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.3">
@@ -5090,8 +5087,8 @@
       <c r="H75" t="s">
         <v>478</v>
       </c>
-      <c r="J75" t="s">
-        <v>601</v>
+      <c r="J75">
+        <v>0</v>
       </c>
       <c r="K75">
         <v>10</v>
@@ -5101,7 +5098,7 @@
       </c>
       <c r="R75" t="str">
         <f t="shared" si="1"/>
-        <v>("Earth Child (Paperback)",NULL,"Sheehan, Kathryn / Waidner, Mary","Council Oak Books",NULL,"991",NULL,"0933031394",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Earth Child (Paperback)",NULL,"Sheehan, Kathryn / Waidner, Mary","Council Oak Books",NULL,"991",NULL,"0933031394",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.3">
@@ -5120,8 +5117,8 @@
       <c r="I76" t="s">
         <v>479</v>
       </c>
-      <c r="J76" t="s">
-        <v>601</v>
+      <c r="J76">
+        <v>0</v>
       </c>
       <c r="K76">
         <v>5</v>
@@ -5131,7 +5128,7 @@
       </c>
       <c r="R76" t="str">
         <f t="shared" si="1"/>
-        <v>("Earthways ",NULL,"Petrash, Carol","The Gryphon House Book",NULL,"1992",NULL,NULL,"9780876591567","PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Earthways ",NULL,"Petrash, Carol","The Gryphon House Book",NULL,"1992",NULL,NULL,"9780876591567","0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.3">
@@ -5150,8 +5147,8 @@
       <c r="H77" s="5" t="s">
         <v>480</v>
       </c>
-      <c r="J77" t="s">
-        <v>601</v>
+      <c r="J77">
+        <v>0</v>
       </c>
       <c r="K77">
         <v>2</v>
@@ -5161,7 +5158,7 @@
       </c>
       <c r="R77" t="str">
         <f t="shared" si="1"/>
-        <v>("Work and Play in Early Childhood",NULL,"Jaffke, Freya","Anthroposophic Press",NULL,"1991",NULL,"088014422",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Work and Play in Early Childhood",NULL,"Jaffke, Freya","Anthroposophic Press",NULL,"1991",NULL,"088014422",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.3">
@@ -5180,8 +5177,8 @@
       <c r="H78" t="s">
         <v>424</v>
       </c>
-      <c r="J78" t="s">
-        <v>601</v>
+      <c r="J78">
+        <v>0</v>
       </c>
       <c r="K78">
         <v>3</v>
@@ -5191,7 +5188,7 @@
       </c>
       <c r="R78" t="str">
         <f t="shared" si="1"/>
-        <v>("Adventuring with Children",NULL,"Jeffrey, Nan","Avalon House Printing",NULL,"1992",NULL,NULL,NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Adventuring with Children",NULL,"Jeffrey, Nan","Avalon House Printing",NULL,"1992",NULL,NULL,NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.3">
@@ -5210,8 +5207,8 @@
       <c r="H79" t="s">
         <v>481</v>
       </c>
-      <c r="J79" t="s">
-        <v>601</v>
+      <c r="J79">
+        <v>0</v>
       </c>
       <c r="K79">
         <v>9</v>
@@ -5221,7 +5218,7 @@
       </c>
       <c r="R79" t="str">
         <f t="shared" si="1"/>
-        <v>("Becoming the Parent You Want to Be",NULL,"Davis, Laura / Keyser, Janis","Broadway Books, NY",NULL,"1997",NULL,"0553067508",NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("Becoming the Parent You Want to Be",NULL,"Davis, Laura / Keyser, Janis","Broadway Books, NY",NULL,"1997",NULL,"0553067508",NULL,"0","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.3">
@@ -5240,8 +5237,8 @@
       <c r="H80" t="s">
         <v>482</v>
       </c>
-      <c r="J80" t="s">
-        <v>601</v>
+      <c r="J80">
+        <v>0</v>
       </c>
       <c r="K80">
         <v>7</v>
@@ -5251,7 +5248,7 @@
       </c>
       <c r="R80" t="str">
         <f t="shared" si="1"/>
-        <v>("Vegetarian Baby and Child",NULL,"Jackson, Petra","Crescent Books, NY",NULL,"1995",NULL,"0517121522",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Vegetarian Baby and Child",NULL,"Jackson, Petra","Crescent Books, NY",NULL,"1995",NULL,"0517121522",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.3">
@@ -5270,8 +5267,8 @@
       <c r="H81" t="s">
         <v>483</v>
       </c>
-      <c r="J81" t="s">
-        <v>601</v>
+      <c r="J81">
+        <v>0</v>
       </c>
       <c r="K81">
         <v>4</v>
@@ -5281,7 +5278,7 @@
       </c>
       <c r="R81" t="str">
         <f t="shared" si="1"/>
-        <v>("Your Self-Confident Baby",NULL,"Gerber, Magda","John Wiley &amp; Sons, Inc.",NULL,"1998",NULL,"0471178837",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Your Self-Confident Baby",NULL,"Gerber, Magda","John Wiley &amp; Sons, Inc.",NULL,"1998",NULL,"0471178837",NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.3">
@@ -5300,8 +5297,8 @@
       <c r="H82" t="s">
         <v>484</v>
       </c>
-      <c r="J82" t="s">
-        <v>601</v>
+      <c r="J82">
+        <v>0</v>
       </c>
       <c r="K82">
         <v>7</v>
@@ -5311,7 +5308,7 @@
       </c>
       <c r="R82" t="str">
         <f t="shared" si="1"/>
-        <v>("Mitten Strings of God",NULL,"Kenison, Katrina","Warner Books",NULL,"2000",NULL,"044+525316",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Mitten Strings of God",NULL,"Kenison, Katrina","Warner Books",NULL,"2000",NULL,"044+525316",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.3">
@@ -5330,8 +5327,8 @@
       <c r="H83" t="s">
         <v>485</v>
       </c>
-      <c r="J83" t="s">
-        <v>601</v>
+      <c r="J83">
+        <v>0</v>
       </c>
       <c r="K83">
         <v>7</v>
@@ -5341,7 +5338,7 @@
       </c>
       <c r="R83" t="str">
         <f t="shared" si="1"/>
-        <v>("Loving Hands - The Traditional Art of Baby Massage",NULL,"Leboyer, Frederick","Newmarket Press",NULL,"1997",NULL,"1557043140",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Loving Hands - The Traditional Art of Baby Massage",NULL,"Leboyer, Frederick","Newmarket Press",NULL,"1997",NULL,"1557043140",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.3">
@@ -5360,8 +5357,8 @@
       <c r="H84" t="s">
         <v>486</v>
       </c>
-      <c r="J84" t="s">
-        <v>601</v>
+      <c r="J84">
+        <v>0</v>
       </c>
       <c r="K84">
         <v>10</v>
@@ -5371,7 +5368,7 @@
       </c>
       <c r="R84" t="str">
         <f t="shared" si="1"/>
-        <v>("Keeping Childhood",NULL,"Aldrich, Nancy","Childhood Press",NULL,"1989",NULL,"0962358304",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Keeping Childhood",NULL,"Aldrich, Nancy","Childhood Press",NULL,"1989",NULL,"0962358304",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.3">
@@ -5390,8 +5387,8 @@
       <c r="H85" t="s">
         <v>487</v>
       </c>
-      <c r="J85" t="s">
-        <v>601</v>
+      <c r="J85">
+        <v>0</v>
       </c>
       <c r="K85">
         <v>3</v>
@@ -5401,7 +5398,7 @@
       </c>
       <c r="R85" t="str">
         <f t="shared" si="1"/>
-        <v>("You Are Your Child's First Teacher",NULL,"Baldwin Dancy, Rahima","Celestial Arts",NULL,"1989",NULL,"0890875197",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("You Are Your Child's First Teacher",NULL,"Baldwin Dancy, Rahima","Celestial Arts",NULL,"1989",NULL,"0890875197",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.3">
@@ -5420,8 +5417,8 @@
       <c r="H86" t="s">
         <v>488</v>
       </c>
-      <c r="J86" t="s">
-        <v>601</v>
+      <c r="J86">
+        <v>0</v>
       </c>
       <c r="K86">
         <v>8</v>
@@ -5431,7 +5428,7 @@
       </c>
       <c r="R86" t="str">
         <f t="shared" si="1"/>
-        <v>("Learning All the Time",NULL,"Holt, John","Addison-Wesley Publishing Company, Inc.",NULL,"1989",NULL,"020112095X",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Learning All the Time",NULL,"Holt, John","Addison-Wesley Publishing Company, Inc.",NULL,"1989",NULL,"020112095X",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.3">
@@ -5450,8 +5447,8 @@
       <c r="H87" t="s">
         <v>489</v>
       </c>
-      <c r="J87" t="s">
-        <v>601</v>
+      <c r="J87">
+        <v>0</v>
       </c>
       <c r="K87">
         <v>2</v>
@@ -5461,7 +5458,7 @@
       </c>
       <c r="R87" t="str">
         <f t="shared" si="1"/>
-        <v>("Our Last Best Shot",NULL,"Sessions Stepp, Laura","Riverhead Books, NY",NULL,"2000",NULL,"1573228753",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Our Last Best Shot",NULL,"Sessions Stepp, Laura","Riverhead Books, NY",NULL,"2000",NULL,"1573228753",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.3">
@@ -5480,8 +5477,8 @@
       <c r="H88" t="s">
         <v>490</v>
       </c>
-      <c r="J88" t="s">
-        <v>601</v>
+      <c r="J88">
+        <v>0</v>
       </c>
       <c r="K88">
         <v>7</v>
@@ -5491,7 +5488,7 @@
       </c>
       <c r="R88" t="str">
         <f t="shared" si="1"/>
-        <v>("The Hurried Child ",NULL,"Elkind, David","Addison-Wesley Publishing Company, Inc.",NULL,"1981",NULL,"0201039672",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("The Hurried Child ",NULL,"Elkind, David","Addison-Wesley Publishing Company, Inc.",NULL,"1981",NULL,"0201039672",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.3">
@@ -5510,8 +5507,8 @@
       <c r="H89" t="s">
         <v>491</v>
       </c>
-      <c r="J89" t="s">
-        <v>601</v>
+      <c r="J89">
+        <v>0</v>
       </c>
       <c r="K89">
         <v>2</v>
@@ -5521,7 +5518,7 @@
       </c>
       <c r="R89" t="str">
         <f t="shared" si="1"/>
-        <v>("Reading Is More than Phonics",NULL,"Goodman, Vera","Reading Wings",NULL,"1999",NULL,"096999382X",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Reading Is More than Phonics",NULL,"Goodman, Vera","Reading Wings",NULL,"1999",NULL,"096999382X",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.3">
@@ -5540,8 +5537,8 @@
       <c r="H90" t="s">
         <v>492</v>
       </c>
-      <c r="J90" t="s">
-        <v>601</v>
+      <c r="J90">
+        <v>0</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -5551,7 +5548,7 @@
       </c>
       <c r="R90" t="str">
         <f t="shared" si="1"/>
-        <v>("Raising a Family - Living on Planet Parenthood",NULL,"Elium, Jeanne and Don","Celestial Arts",NULL,"1997",NULL,"0890878188",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Raising a Family - Living on Planet Parenthood",NULL,"Elium, Jeanne and Don","Celestial Arts",NULL,"1997",NULL,"0890878188",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.3">
@@ -5570,8 +5567,8 @@
       <c r="H91" s="5" t="s">
         <v>493</v>
       </c>
-      <c r="J91" t="s">
-        <v>601</v>
+      <c r="J91">
+        <v>0</v>
       </c>
       <c r="K91">
         <v>4</v>
@@ -5581,7 +5578,7 @@
       </c>
       <c r="R91" t="str">
         <f t="shared" si="1"/>
-        <v>("Wakdorf Education for Adolescence",NULL,"Steiner, Rudolf","Kolisko Archive Publications",NULL,"1980",NULL,"096492378",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Wakdorf Education for Adolescence",NULL,"Steiner, Rudolf","Kolisko Archive Publications",NULL,"1980",NULL,"096492378",NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.3">
@@ -5600,8 +5597,8 @@
       <c r="H92" t="s">
         <v>494</v>
       </c>
-      <c r="J92" t="s">
-        <v>601</v>
+      <c r="J92">
+        <v>0</v>
       </c>
       <c r="K92">
         <v>10</v>
@@ -5611,7 +5608,7 @@
       </c>
       <c r="R92" t="str">
         <f t="shared" si="1"/>
-        <v>("Life Strategies for Teens",NULL,"McGraw, Jay","Fireside",NULL,"2000",NULL,"074321546X",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Life Strategies for Teens",NULL,"McGraw, Jay","Fireside",NULL,"2000",NULL,"074321546X",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.3">
@@ -5630,8 +5627,8 @@
       <c r="H93" t="s">
         <v>495</v>
       </c>
-      <c r="J93" t="s">
-        <v>601</v>
+      <c r="J93">
+        <v>0</v>
       </c>
       <c r="K93">
         <v>5</v>
@@ -5641,7 +5638,7 @@
       </c>
       <c r="R93" t="str">
         <f t="shared" si="1"/>
-        <v>("Summer Children - Ready or Not For School",NULL,"Uphoff, James K","J&amp;J Publishing Co.",NULL,"1986",NULL,"0961856106",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Summer Children - Ready or Not For School",NULL,"Uphoff, James K","J&amp;J Publishing Co.",NULL,"1986",NULL,"0961856106",NULL,"0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.3">
@@ -5660,8 +5657,8 @@
       <c r="H94" t="s">
         <v>496</v>
       </c>
-      <c r="J94" t="s">
-        <v>601</v>
+      <c r="J94">
+        <v>0</v>
       </c>
       <c r="K94">
         <v>4</v>
@@ -5671,7 +5668,7 @@
       </c>
       <c r="R94" t="str">
         <f t="shared" si="1"/>
-        <v>("An Education for the 21st Century - Essays on Waldorf Education ",NULL,"Maher, Stanford","Novalis Press",NULL,"1995",NULL,"0958388512",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("An Education for the 21st Century - Essays on Waldorf Education ",NULL,"Maher, Stanford","Novalis Press",NULL,"1995",NULL,"0958388512",NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.3">
@@ -5690,8 +5687,8 @@
       <c r="H95" t="s">
         <v>497</v>
       </c>
-      <c r="J95" t="s">
-        <v>601</v>
+      <c r="J95">
+        <v>0</v>
       </c>
       <c r="K95">
         <v>3</v>
@@ -5701,7 +5698,7 @@
       </c>
       <c r="R95" t="str">
         <f t="shared" si="1"/>
-        <v>("Exrtaordinary Minds",NULL,"Gardner, Howard","Basic Books",NULL,"1997",NULL,"0465021255",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Exrtaordinary Minds",NULL,"Gardner, Howard","Basic Books",NULL,"1997",NULL,"0465021255",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.3">
@@ -5720,8 +5717,8 @@
       <c r="H96" t="s">
         <v>498</v>
       </c>
-      <c r="J96" t="s">
-        <v>601</v>
+      <c r="J96">
+        <v>0</v>
       </c>
       <c r="K96">
         <v>4</v>
@@ -5731,7 +5728,7 @@
       </c>
       <c r="R96" t="str">
         <f t="shared" si="1"/>
-        <v>("Multiple Intelligences",NULL,"Gardner, Howard","Basic Books",NULL,"1993",NULL,"046501822X",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Multiple Intelligences",NULL,"Gardner, Howard","Basic Books",NULL,"1993",NULL,"046501822X",NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.3">
@@ -5750,8 +5747,8 @@
       <c r="H97" t="s">
         <v>499</v>
       </c>
-      <c r="J97" t="s">
-        <v>601</v>
+      <c r="J97">
+        <v>0</v>
       </c>
       <c r="K97">
         <v>3</v>
@@ -5761,7 +5758,7 @@
       </c>
       <c r="R97" t="str">
         <f t="shared" si="1"/>
-        <v>("Frames of Mind",NULL,"Gardner, Howard","Basic Books",NULL,"1983",NULL,"0465025099",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Frames of Mind",NULL,"Gardner, Howard","Basic Books",NULL,"1983",NULL,"0465025099",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.3">
@@ -5780,8 +5777,8 @@
       <c r="H98" t="s">
         <v>500</v>
       </c>
-      <c r="J98" t="s">
-        <v>601</v>
+      <c r="J98">
+        <v>0</v>
       </c>
       <c r="K98">
         <v>2</v>
@@ -5791,7 +5788,7 @@
       </c>
       <c r="R98" t="str">
         <f t="shared" si="1"/>
-        <v>("Turning",NULL,"Anthroposiphic Press","Anthroposophic Press",NULL,"1994",NULL,"0880103841",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Turning",NULL,"Anthroposiphic Press","Anthroposophic Press",NULL,"1994",NULL,"0880103841",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.3">
@@ -5810,8 +5807,8 @@
       <c r="H99" t="s">
         <v>501</v>
       </c>
-      <c r="J99" t="s">
-        <v>601</v>
+      <c r="J99">
+        <v>0</v>
       </c>
       <c r="K99">
         <v>6</v>
@@ -5821,7 +5818,7 @@
       </c>
       <c r="R99" t="str">
         <f t="shared" si="1"/>
-        <v>("Teaching as a Lively Art",NULL,"Spock, Marjorie","Anthroposophic Press",NULL,"1985",NULL,"088010127X",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Teaching as a Lively Art",NULL,"Spock, Marjorie","Anthroposophic Press",NULL,"1985",NULL,"088010127X",NULL,"0","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.3">
@@ -5840,8 +5837,8 @@
       <c r="H100" t="s">
         <v>502</v>
       </c>
-      <c r="J100" t="s">
-        <v>601</v>
+      <c r="J100">
+        <v>0</v>
       </c>
       <c r="K100">
         <v>2</v>
@@ -5851,7 +5848,7 @@
       </c>
       <c r="R100" t="str">
         <f t="shared" si="1"/>
-        <v>("Celebrating the Festivals with Children",NULL,"Lenz, Friedel","Anthroposophic Press",NULL,"1989",NULL,"0880101512",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Celebrating the Festivals with Children",NULL,"Lenz, Friedel","Anthroposophic Press",NULL,"1989",NULL,"0880101512",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.3">
@@ -5870,8 +5867,8 @@
       <c r="H101" t="s">
         <v>503</v>
       </c>
-      <c r="J101" t="s">
-        <v>601</v>
+      <c r="J101">
+        <v>0</v>
       </c>
       <c r="K101">
         <v>3</v>
@@ -5881,7 +5878,7 @@
       </c>
       <c r="R101" t="str">
         <f t="shared" si="1"/>
-        <v>("The Education of the Child",NULL,"Steiner, Rudolf","Rudolf Steiner Press",NULL,"1979",NULL,"0854400303",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("The Education of the Child",NULL,"Steiner, Rudolf","Rudolf Steiner Press",NULL,"1979",NULL,"0854400303",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.3">
@@ -5900,8 +5897,8 @@
       <c r="H102" t="s">
         <v>504</v>
       </c>
-      <c r="J102" t="s">
-        <v>601</v>
+      <c r="J102">
+        <v>0</v>
       </c>
       <c r="K102">
         <v>3</v>
@@ -5911,7 +5908,7 @@
       </c>
       <c r="R102" t="str">
         <f t="shared" si="1"/>
-        <v>("The Child and the Machine",NULL,"Armstrong, Alison / Casement, Charles","Key Porter Books",NULL,"1998",NULL,"1552630048",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("The Child and the Machine",NULL,"Armstrong, Alison / Casement, Charles","Key Porter Books",NULL,"1998",NULL,"1552630048",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
@@ -5930,8 +5927,8 @@
       <c r="H103" t="s">
         <v>505</v>
       </c>
-      <c r="J103" t="s">
-        <v>601</v>
+      <c r="J103">
+        <v>0</v>
       </c>
       <c r="K103">
         <v>3</v>
@@ -5941,7 +5938,7 @@
       </c>
       <c r="R103" t="str">
         <f t="shared" si="1"/>
-        <v>("Between From and Freedom",NULL,"Staley, Betty","Hawthorn Press",NULL,"1996",NULL,"1869890086",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Between From and Freedom",NULL,"Staley, Betty","Hawthorn Press",NULL,"1996",NULL,"1869890086",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.3">
@@ -5960,8 +5957,8 @@
       <c r="I104" t="s">
         <v>506</v>
       </c>
-      <c r="J104" t="s">
-        <v>601</v>
+      <c r="J104">
+        <v>0</v>
       </c>
       <c r="K104">
         <v>9</v>
@@ -5971,7 +5968,7 @@
       </c>
       <c r="R104" t="str">
         <f t="shared" si="1"/>
-        <v>("The Curse of the Good Girl",NULL,"Simmons, Rachel","Penguin Books",NULL,"2010",NULL,NULL,"9780143117988","PARENT","9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("The Curse of the Good Girl",NULL,"Simmons, Rachel","Penguin Books",NULL,"2010",NULL,NULL,"9780143117988","0","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.3">
@@ -5990,8 +5987,8 @@
       <c r="H105" t="s">
         <v>507</v>
       </c>
-      <c r="J105" t="s">
-        <v>601</v>
+      <c r="J105">
+        <v>0</v>
       </c>
       <c r="K105">
         <v>6</v>
@@ -6001,7 +5998,7 @@
       </c>
       <c r="R105" t="str">
         <f t="shared" si="1"/>
-        <v>("Too Old Too Soon",NULL,"Fields, Doug","Harvest House Publishers",NULL,"1991",NULL,"0890818487",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Too Old Too Soon",NULL,"Fields, Doug","Harvest House Publishers",NULL,"1991",NULL,"0890818487",NULL,"0","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.3">
@@ -6020,8 +6017,8 @@
       <c r="H106" s="5" t="s">
         <v>508</v>
       </c>
-      <c r="J106" t="s">
-        <v>601</v>
+      <c r="J106">
+        <v>0</v>
       </c>
       <c r="K106">
         <v>5</v>
@@ -6031,7 +6028,7 @@
       </c>
       <c r="R106" t="str">
         <f t="shared" si="1"/>
-        <v>("A Child Is Born",NULL,"zur Linden, Wilhelm","Rudolf Steiner Press",NULL,"1980",NULL,"085443574",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("A Child Is Born",NULL,"zur Linden, Wilhelm","Rudolf Steiner Press",NULL,"1980",NULL,"085443574",NULL,"0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.3">
@@ -6050,8 +6047,8 @@
       <c r="H107" t="s">
         <v>509</v>
       </c>
-      <c r="J107" t="s">
-        <v>601</v>
+      <c r="J107">
+        <v>0</v>
       </c>
       <c r="K107">
         <v>4</v>
@@ -6061,7 +6058,7 @@
       </c>
       <c r="R107" t="str">
         <f t="shared" si="1"/>
-        <v>("Steiner Education in Theory and Practice",NULL,"Childs, Gilbert","Floris Books",NULL,"1991",NULL,"0863151310",NULL,"PARENT","4","4",NULL,NULL,NULL,NULL),</v>
+        <v>("Steiner Education in Theory and Practice",NULL,"Childs, Gilbert","Floris Books",NULL,"1991",NULL,"0863151310",NULL,"0","4","4",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.3">
@@ -6080,8 +6077,8 @@
       <c r="H108" t="s">
         <v>510</v>
       </c>
-      <c r="J108" t="s">
-        <v>601</v>
+      <c r="J108">
+        <v>0</v>
       </c>
       <c r="K108">
         <v>7</v>
@@ -6091,7 +6088,7 @@
       </c>
       <c r="R108" t="str">
         <f t="shared" si="1"/>
-        <v>("When a Child Is Born",NULL,"zur Linden, Wilhelm","Thorsons Publishers Inc., NY",NULL,"1984",NULL,"0722509561",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("When a Child Is Born",NULL,"zur Linden, Wilhelm","Thorsons Publishers Inc., NY",NULL,"1984",NULL,"0722509561",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.3">
@@ -6110,8 +6107,8 @@
       <c r="H109" t="s">
         <v>511</v>
       </c>
-      <c r="J109" t="s">
-        <v>601</v>
+      <c r="J109">
+        <v>0</v>
       </c>
       <c r="K109">
         <v>10</v>
@@ -6121,7 +6118,7 @@
       </c>
       <c r="R109" t="str">
         <f t="shared" si="1"/>
-        <v>("The Curriculum of the First Waldorf School",NULL,"von Heydebrand, Caroline","Steiner Schools Fellowhsip Publications",NULL,"1989",NULL,"0951033131",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("The Curriculum of the First Waldorf School",NULL,"von Heydebrand, Caroline","Steiner Schools Fellowhsip Publications",NULL,"1989",NULL,"0951033131",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.3">
@@ -6140,8 +6137,8 @@
       <c r="H110" t="s">
         <v>512</v>
       </c>
-      <c r="J110" t="s">
-        <v>601</v>
+      <c r="J110">
+        <v>0</v>
       </c>
       <c r="K110">
         <v>1</v>
@@ -6151,7 +6148,7 @@
       </c>
       <c r="R110" t="str">
         <f t="shared" si="1"/>
-        <v>("Reincarnation and Karma - Their Significance in Modern Culture",NULL,"Steiner, Rudolf","Steiner Book Centre, Inc., Vancouver",NULL,"1977",NULL,"0919924069",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Reincarnation and Karma - Their Significance in Modern Culture",NULL,"Steiner, Rudolf","Steiner Book Centre, Inc., Vancouver",NULL,"1977",NULL,"0919924069",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.3">
@@ -6173,8 +6170,8 @@
       <c r="H111" t="s">
         <v>513</v>
       </c>
-      <c r="J111" t="s">
-        <v>601</v>
+      <c r="J111">
+        <v>0</v>
       </c>
       <c r="K111">
         <v>3</v>
@@ -6184,7 +6181,7 @@
       </c>
       <c r="R111" t="str">
         <f t="shared" si="1"/>
-        <v>("Theosophy",NULL,"Steiner, Rudolf","Rudolf Steiner Press","4","1973",NULL,"0854402705",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Theosophy",NULL,"Steiner, Rudolf","Rudolf Steiner Press","4","1973",NULL,"0854402705",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.3">
@@ -6203,8 +6200,8 @@
       <c r="H112" t="s">
         <v>424</v>
       </c>
-      <c r="J112" t="s">
-        <v>601</v>
+      <c r="J112">
+        <v>0</v>
       </c>
       <c r="K112">
         <v>7</v>
@@ -6214,7 +6211,7 @@
       </c>
       <c r="R112" t="str">
         <f t="shared" si="1"/>
-        <v>("The Younger Generation",NULL,"Steiner, Rudolf","Anthroposophic Press",NULL,"1967",NULL,NULL,NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("The Younger Generation",NULL,"Steiner, Rudolf","Anthroposophic Press",NULL,"1967",NULL,NULL,NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.3">
@@ -6233,8 +6230,8 @@
       <c r="H113" t="s">
         <v>514</v>
       </c>
-      <c r="J113" t="s">
-        <v>601</v>
+      <c r="J113">
+        <v>0</v>
       </c>
       <c r="K113">
         <v>1</v>
@@ -6244,7 +6241,7 @@
       </c>
       <c r="R113" t="str">
         <f t="shared" si="1"/>
-        <v>("The Kingdom of Childhood",NULL,"Steiner, Rudolf","Rudolf Steiner Press",NULL,"1982",NULL,"0854402845",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("The Kingdom of Childhood",NULL,"Steiner, Rudolf","Rudolf Steiner Press",NULL,"1982",NULL,"0854402845",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.3">
@@ -6263,8 +6260,8 @@
       <c r="H114" t="s">
         <v>515</v>
       </c>
-      <c r="J114" t="s">
-        <v>601</v>
+      <c r="J114">
+        <v>0</v>
       </c>
       <c r="K114">
         <v>3</v>
@@ -6274,7 +6271,7 @@
       </c>
       <c r="R114" t="str">
         <f t="shared" si="1"/>
-        <v>("Encountering the Self",NULL,"Koepke, Hermann","Anthroposophic Press",NULL,"1989",NULL,"0880102799",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Encountering the Self",NULL,"Koepke, Hermann","Anthroposophic Press",NULL,"1989",NULL,"0880102799",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.3">
@@ -6293,8 +6290,8 @@
       <c r="H115" t="s">
         <v>516</v>
       </c>
-      <c r="J115" t="s">
-        <v>601</v>
+      <c r="J115">
+        <v>0</v>
       </c>
       <c r="K115">
         <v>3</v>
@@ -6304,7 +6301,7 @@
       </c>
       <c r="R115" t="str">
         <f t="shared" si="1"/>
-        <v>("The Recovery of Man in Childhood",NULL,"Harwood, A.C.","Anthroposophic Press",NULL,"1982",NULL,"088010001X",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("The Recovery of Man in Childhood",NULL,"Harwood, A.C.","Anthroposophic Press",NULL,"1982",NULL,"088010001X",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.3">
@@ -6323,8 +6320,8 @@
       <c r="H116" t="s">
         <v>517</v>
       </c>
-      <c r="J116" t="s">
-        <v>601</v>
+      <c r="J116">
+        <v>0</v>
       </c>
       <c r="K116">
         <v>10</v>
@@ -6334,7 +6331,7 @@
       </c>
       <c r="R116" t="str">
         <f t="shared" si="1"/>
-        <v>("Rudold Steiner - Life, Work, Inner Path and Social Initiatives",NULL,"Lissau, Rudi","Hawthorn Press",NULL,"1987",NULL,"1869890068",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Rudold Steiner - Life, Work, Inner Path and Social Initiatives",NULL,"Lissau, Rudi","Hawthorn Press",NULL,"1987",NULL,"1869890068",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.3">
@@ -6353,8 +6350,8 @@
       <c r="H117" t="s">
         <v>518</v>
       </c>
-      <c r="J117" t="s">
-        <v>601</v>
+      <c r="J117">
+        <v>0</v>
       </c>
       <c r="K117">
         <v>5</v>
@@ -6364,7 +6361,7 @@
       </c>
       <c r="R117" t="str">
         <f t="shared" si="1"/>
-        <v>("The First Three Years of The Child",NULL,"Konig, Karl","Anthroposophic Press",NULL,"1984",NULL,"0880100435",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("The First Three Years of The Child",NULL,"Konig, Karl","Anthroposophic Press",NULL,"1984",NULL,"0880100435",NULL,"0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.3">
@@ -6383,8 +6380,8 @@
       <c r="H118" t="s">
         <v>519</v>
       </c>
-      <c r="J118" t="s">
-        <v>601</v>
+      <c r="J118">
+        <v>0</v>
       </c>
       <c r="K118">
         <v>2</v>
@@ -6394,7 +6391,7 @@
       </c>
       <c r="R118" t="str">
         <f t="shared" si="1"/>
-        <v>("Confessions of a Waldorf Parent",NULL,"Gorman, Margaret","Rudolf Steiner College Publications",NULL,"1990",NULL,"0945803060",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Confessions of a Waldorf Parent",NULL,"Gorman, Margaret","Rudolf Steiner College Publications",NULL,"1990",NULL,"0945803060",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.3">
@@ -6413,8 +6410,8 @@
       <c r="H119" s="5" t="s">
         <v>520</v>
       </c>
-      <c r="J119" t="s">
-        <v>601</v>
+      <c r="J119">
+        <v>0</v>
       </c>
       <c r="K119">
         <v>6</v>
@@ -6424,7 +6421,7 @@
       </c>
       <c r="R119" t="str">
         <f t="shared" si="1"/>
-        <v>("Creativity in Education - The Waldorf Approach",NULL,"Querido, Rene M.","H. S. Dakin Company",NULL,"1987",NULL,"09304205",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Creativity in Education - The Waldorf Approach",NULL,"Querido, Rene M.","H. S. Dakin Company",NULL,"1987",NULL,"09304205",NULL,"0","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.3">
@@ -6443,8 +6440,8 @@
       <c r="H120" t="s">
         <v>424</v>
       </c>
-      <c r="J120" t="s">
-        <v>601</v>
+      <c r="J120">
+        <v>0</v>
       </c>
       <c r="K120">
         <v>9</v>
@@ -6454,7 +6451,7 @@
       </c>
       <c r="R120" t="str">
         <f t="shared" si="1"/>
-        <v>("The Child, The Teachers and The Community",NULL,"Smit, Jorgen","Mercury Press",NULL,"1992",NULL,NULL,NULL,"PARENT","9","9",NULL,NULL,NULL,NULL),</v>
+        <v>("The Child, The Teachers and The Community",NULL,"Smit, Jorgen","Mercury Press",NULL,"1992",NULL,NULL,NULL,"0","9","9",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.3">
@@ -6473,8 +6470,8 @@
       <c r="H121" t="s">
         <v>424</v>
       </c>
-      <c r="J121" t="s">
-        <v>601</v>
+      <c r="J121">
+        <v>0</v>
       </c>
       <c r="K121">
         <v>7</v>
@@ -6484,7 +6481,7 @@
       </c>
       <c r="R121" t="str">
         <f t="shared" si="1"/>
-        <v>("The Philosophy of Freedom",NULL,"Steiner, Rudolf","Anthroposophic Press",NULL,"1964",NULL,NULL,NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("The Philosophy of Freedom",NULL,"Steiner, Rudolf","Anthroposophic Press",NULL,"1964",NULL,NULL,NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.3">
@@ -6503,8 +6500,8 @@
       <c r="H122" t="s">
         <v>521</v>
       </c>
-      <c r="J122" t="s">
-        <v>601</v>
+      <c r="J122">
+        <v>0</v>
       </c>
       <c r="K122">
         <v>7</v>
@@ -6514,7 +6511,7 @@
       </c>
       <c r="R122" t="str">
         <f t="shared" si="1"/>
-        <v>("Questions of Destiny",NULL,"Pietzner, Carlo","Anthroposophic Press",NULL,"1988",NULL,"0880102640",NULL,"PARENT","7","7",NULL,NULL,NULL,NULL),</v>
+        <v>("Questions of Destiny",NULL,"Pietzner, Carlo","Anthroposophic Press",NULL,"1988",NULL,"0880102640",NULL,"0","7","7",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.3">
@@ -6533,8 +6530,8 @@
       <c r="H123" t="s">
         <v>522</v>
       </c>
-      <c r="J123" t="s">
-        <v>601</v>
+      <c r="J123">
+        <v>0</v>
       </c>
       <c r="K123">
         <v>6</v>
@@ -6544,7 +6541,7 @@
       </c>
       <c r="R123" t="str">
         <f t="shared" si="1"/>
-        <v>("Anthroposophy - A Way of Life",NULL,"Edmunds, Francis","Carnant Books",NULL,"1982",NULL,"0903580659",NULL,"PARENT","6","6",NULL,NULL,NULL,NULL),</v>
+        <v>("Anthroposophy - A Way of Life",NULL,"Edmunds, Francis","Carnant Books",NULL,"1982",NULL,"0903580659",NULL,"0","6","6",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.3">
@@ -6563,8 +6560,8 @@
       <c r="H124" t="s">
         <v>424</v>
       </c>
-      <c r="J124" t="s">
-        <v>601</v>
+      <c r="J124">
+        <v>0</v>
       </c>
       <c r="K124">
         <v>2</v>
@@ -6574,7 +6571,7 @@
       </c>
       <c r="R124" t="str">
         <f t="shared" si="1"/>
-        <v>("Waldorf: Education for Tomorrow",NULL,"Toronto Waldorf Schools","Torornto Waldorf Schools",NULL,"1970",NULL,NULL,NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Waldorf: Education for Tomorrow",NULL,"Toronto Waldorf Schools","Torornto Waldorf Schools",NULL,"1970",NULL,NULL,NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.3">
@@ -6596,8 +6593,8 @@
       <c r="H125" t="s">
         <v>523</v>
       </c>
-      <c r="J125" t="s">
-        <v>601</v>
+      <c r="J125">
+        <v>0</v>
       </c>
       <c r="K125">
         <v>5</v>
@@ -6607,7 +6604,7 @@
       </c>
       <c r="R125" t="str">
         <f t="shared" si="1"/>
-        <v>("Waldorf Parenting Book",NULL,"Cusick, Lois","Rudolf Steiner College Publications","3","1992",NULL,"0916786757",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("Waldorf Parenting Book",NULL,"Cusick, Lois","Rudolf Steiner College Publications","3","1992",NULL,"0916786757",NULL,"0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.3">
@@ -6626,8 +6623,8 @@
       <c r="H126" t="s">
         <v>524</v>
       </c>
-      <c r="J126" t="s">
-        <v>601</v>
+      <c r="J126">
+        <v>0</v>
       </c>
       <c r="K126">
         <v>2</v>
@@ -6637,7 +6634,7 @@
       </c>
       <c r="R126" t="str">
         <f t="shared" si="1"/>
-        <v>("The Goetheanum - Rudolf Steiner's Architectual Impulse",NULL,"Biesantz, Hagen / Klingborg, Arne","Rudolf Steiner Press",NULL,"1979",NULL,"0854403558",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("The Goetheanum - Rudolf Steiner's Architectual Impulse",NULL,"Biesantz, Hagen / Klingborg, Arne","Rudolf Steiner Press",NULL,"1979",NULL,"0854403558",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.3">
@@ -6656,8 +6653,8 @@
       <c r="H127" t="s">
         <v>525</v>
       </c>
-      <c r="J127" t="s">
-        <v>601</v>
+      <c r="J127">
+        <v>0</v>
       </c>
       <c r="K127">
         <v>1</v>
@@ -6667,7 +6664,7 @@
       </c>
       <c r="R127" t="str">
         <f t="shared" si="1"/>
-        <v>("The Plug-In Drug - Television, Children and the Family",NULL,"Winn, Marie","Penguin Books",NULL,"1985",NULL,"0140076980",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("The Plug-In Drug - Television, Children and the Family",NULL,"Winn, Marie","Penguin Books",NULL,"1985",NULL,"0140076980",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.3">
@@ -6689,8 +6686,8 @@
       <c r="H128" t="s">
         <v>526</v>
       </c>
-      <c r="J128" t="s">
-        <v>601</v>
+      <c r="J128">
+        <v>0</v>
       </c>
       <c r="K128">
         <v>1</v>
@@ -6700,7 +6697,7 @@
       </c>
       <c r="R128" t="str">
         <f t="shared" si="1"/>
-        <v>("Who's Bringing Them Up?",NULL,"Large, Martin","Hawthorn Press","2","1990",NULL,"1869890248",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Who's Bringing Them Up?",NULL,"Large, Martin","Hawthorn Press","2","1990",NULL,"1869890248",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.3">
@@ -6719,8 +6716,8 @@
       <c r="H129" t="s">
         <v>527</v>
       </c>
-      <c r="J129" t="s">
-        <v>601</v>
+      <c r="J129">
+        <v>0</v>
       </c>
       <c r="K129">
         <v>5</v>
@@ -6730,7 +6727,7 @@
       </c>
       <c r="R129" t="str">
         <f t="shared" si="1"/>
-        <v>("The Young Child",NULL,"De Haes, Daniel Udo","Floris Books",NULL,"1986",NULL,"0863150373",NULL,"PARENT","5","5",NULL,NULL,NULL,NULL),</v>
+        <v>("The Young Child",NULL,"De Haes, Daniel Udo","Floris Books",NULL,"1986",NULL,"0863150373",NULL,"0","5","5",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.3">
@@ -6752,8 +6749,8 @@
       <c r="H130" t="s">
         <v>528</v>
       </c>
-      <c r="J130" t="s">
-        <v>601</v>
+      <c r="J130">
+        <v>0</v>
       </c>
       <c r="K130">
         <v>1</v>
@@ -6763,7 +6760,7 @@
       </c>
       <c r="R130" t="str">
         <f t="shared" si="1"/>
-        <v>("Vision in Action ",NULL,"Schaefer, Christopher / Voors, Tyno","Lindisfarne Press","2","1986",NULL,"0940262746",NULL,"PARENT","1","1",NULL,NULL,NULL,NULL),</v>
+        <v>("Vision in Action ",NULL,"Schaefer, Christopher / Voors, Tyno","Lindisfarne Press","2","1986",NULL,"0940262746",NULL,"0","1","1",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.3">
@@ -6782,8 +6779,8 @@
       <c r="H131" t="s">
         <v>529</v>
       </c>
-      <c r="J131" t="s">
-        <v>601</v>
+      <c r="J131">
+        <v>0</v>
       </c>
       <c r="K131">
         <v>3</v>
@@ -6809,7 +6806,7 @@
 IF(N131="","NULL",_xlfn.CONCAT("""",N131,"""")),",",
 IF(O131="","NULL",_xlfn.CONCAT("""",O131,"""")),",",
 IF(P131="","NULL",_xlfn.CONCAT("""",P131,"""")),"),")</f>
-        <v>("Endangered Minds ",NULL,"Healy, Jane M.","Touchstone Book",NULL,"1990",NULL,"067174920X",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL),</v>
+        <v>("Endangered Minds ",NULL,"Healy, Jane M.","Touchstone Book",NULL,"1990",NULL,"067174920X",NULL,"0","3","3",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.3">
@@ -6831,8 +6828,8 @@
       <c r="H132" t="s">
         <v>530</v>
       </c>
-      <c r="J132" t="s">
-        <v>601</v>
+      <c r="J132">
+        <v>0</v>
       </c>
       <c r="K132">
         <v>8</v>
@@ -6842,7 +6839,7 @@
       </c>
       <c r="R132" t="str">
         <f t="shared" si="2"/>
-        <v>("Waldorf Student Reading List",NULL,"Johnson Fenner, Pamela / Rivers, Karen L.","Michealmas Press","3","1995",NULL,"0964783207",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("Waldorf Student Reading List",NULL,"Johnson Fenner, Pamela / Rivers, Karen L.","Michealmas Press","3","1995",NULL,"0964783207",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.3">
@@ -6861,8 +6858,8 @@
       <c r="H133" t="s">
         <v>531</v>
       </c>
-      <c r="J133" t="s">
-        <v>601</v>
+      <c r="J133">
+        <v>0</v>
       </c>
       <c r="K133">
         <v>10</v>
@@ -6872,7 +6869,7 @@
       </c>
       <c r="R133" t="str">
         <f t="shared" si="2"/>
-        <v>("The Recovery of Man in Childhood",NULL,"Harwood, A.C.","The Myrin Book, NY",NULL,"1992",NULL,"0913098434",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("The Recovery of Man in Childhood",NULL,"Harwood, A.C.","The Myrin Book, NY",NULL,"1992",NULL,"0913098434",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.3">
@@ -6891,8 +6888,8 @@
       <c r="H134" t="s">
         <v>532</v>
       </c>
-      <c r="J134" t="s">
-        <v>601</v>
+      <c r="J134">
+        <v>0</v>
       </c>
       <c r="K134">
         <v>8</v>
@@ -6902,7 +6899,7 @@
       </c>
       <c r="R134" t="str">
         <f t="shared" si="2"/>
-        <v>("The First Seven Years -  Physiology of Childhood",NULL,"Schoorel, Edmond","Rudolf Steiner College Press",NULL,"2004",NULL,"0945803680",NULL,"PARENT","8","8",NULL,NULL,NULL,NULL),</v>
+        <v>("The First Seven Years -  Physiology of Childhood",NULL,"Schoorel, Edmond","Rudolf Steiner College Press",NULL,"2004",NULL,"0945803680",NULL,"0","8","8",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.3">
@@ -6921,8 +6918,8 @@
       <c r="H135" t="s">
         <v>533</v>
       </c>
-      <c r="J135" t="s">
-        <v>601</v>
+      <c r="J135">
+        <v>0</v>
       </c>
       <c r="K135">
         <v>2</v>
@@ -6932,7 +6929,7 @@
       </c>
       <c r="R135" t="str">
         <f t="shared" si="2"/>
-        <v>("Rudolf Steiner Education and The Developing Child",NULL,"Aeppli, Willi","Anthroposophic Press",NULL,"1986",NULL,"0880101644",NULL,"PARENT","2","2",NULL,NULL,NULL,NULL),</v>
+        <v>("Rudolf Steiner Education and The Developing Child",NULL,"Aeppli, Willi","Anthroposophic Press",NULL,"1986",NULL,"0880101644",NULL,"0","2","2",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.3">
@@ -6951,8 +6948,8 @@
       <c r="H136" t="s">
         <v>534</v>
       </c>
-      <c r="J136" t="s">
-        <v>601</v>
+      <c r="J136">
+        <v>0</v>
       </c>
       <c r="K136">
         <v>10</v>
@@ -6962,7 +6959,7 @@
       </c>
       <c r="R136" t="str">
         <f t="shared" si="2"/>
-        <v>("Waldorf Schools  -Upper Grades and High School",NULL,"Pusch, Ruth","Mercury Press",NULL,"1993",NULL,"0929979303",NULL,"PARENT","10","10",NULL,NULL,NULL,NULL),</v>
+        <v>("Waldorf Schools  -Upper Grades and High School",NULL,"Pusch, Ruth","Mercury Press",NULL,"1993",NULL,"0929979303",NULL,"0","10","10",NULL,NULL,NULL,NULL),</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.3">
@@ -6981,8 +6978,8 @@
       <c r="H137" t="s">
         <v>535</v>
       </c>
-      <c r="J137" t="s">
-        <v>601</v>
+      <c r="J137">
+        <v>0</v>
       </c>
       <c r="K137">
         <v>3</v>
@@ -7008,7 +7005,7 @@
 IF(N137="","NULL",_xlfn.CONCAT("""",N137,"""")),",",
 IF(O137="","NULL",_xlfn.CONCAT("""",O137,"""")),",",
 IF(P137="","NULL",_xlfn.CONCAT("""",P137,"""")),");")</f>
-        <v>("Waldorf Schools  -Kindergarten and Early Grades",NULL,"Pusch, Ruth","Mercury Press",NULL,"1996",NULL,"092997929X",NULL,"PARENT","3","3",NULL,NULL,NULL,NULL);</v>
+        <v>("Waldorf Schools  -Kindergarten and Early Grades",NULL,"Pusch, Ruth","Mercury Press",NULL,"1996",NULL,"092997929X",NULL,"0","3","3",NULL,NULL,NULL,NULL);</v>
       </c>
     </row>
   </sheetData>
@@ -10497,7 +10494,7 @@
         <v>590</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -10532,7 +10529,7 @@
         <v>591</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -10567,7 +10564,7 @@
         <v>595</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -10605,7 +10602,7 @@
         <v>597</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="H5">
         <v>1</v>

</xml_diff>